<commit_message>
Issue #267: Namespace Updates - ID Requested: HYB2 - Hayabusa2
Update namespace registry with HYB2 - Hayabusa2.

This dictionary contains classes and attributes specific to the Hayabusa2 mission and instruments. It has been created to support the Hayabusa 2 data archive.

Resolves #267
</commit_message>
<xml_diff>
--- a/model-ontology/src/ontology/Data/pds-namespace-registry.xlsx
+++ b/model-ontology/src/ontology/Data/pds-namespace-registry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20367"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\AAAPDS4\AADataModel\0000_Design\Namespaces_1002\NameSpaceRegistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{87C73744-6FB4-4083-AE18-606C56810CB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D43093-C62B-4F56-BE56-154ED8752095}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1155" yWindow="1065" windowWidth="26655" windowHeight="12855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1157" yWindow="1063" windowWidth="26657" windowHeight="12857" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Namespaces" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Namespaces!$A$11:$Q$29</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1325" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1343" uniqueCount="519">
   <si>
     <t>Registration Date</t>
   </si>
@@ -1559,6 +1559,36 @@
   </si>
   <si>
     <t>https://voparis-ns.obspm.fr/pds4/epn/v1</t>
+  </si>
+  <si>
+    <t>hyb2</t>
+  </si>
+  <si>
+    <t>mission/hyb2</t>
+  </si>
+  <si>
+    <t>Carol Neese</t>
+  </si>
+  <si>
+    <t>nees at psi.edu</t>
+  </si>
+  <si>
+    <t>This is the Hayabusa2 Mission Specific Data Dictionary.</t>
+  </si>
+  <si>
+    <t>C. Neese</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hayabusa2 </t>
+  </si>
+  <si>
+    <t>PDS4_HYB2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://pds.nasa.gov/pds4/mission/hyb2/v1 </t>
+  </si>
+  <si>
+    <t>sbnpsi</t>
   </si>
 </sst>
 </file>
@@ -1725,7 +1755,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1811,14 +1841,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1832,6 +1856,16 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2145,39 +2179,39 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U88"/>
+  <dimension ref="A1:U89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="15.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="22" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="22" customWidth="1"/>
-    <col min="3" max="3" width="46.140625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="22" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="22" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" style="22" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="22" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" style="22" customWidth="1"/>
-    <col min="9" max="9" width="25.28515625" style="22" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" style="22" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" style="22" customWidth="1"/>
+    <col min="1" max="1" width="14.3828125" style="22" customWidth="1"/>
+    <col min="2" max="2" width="16.69140625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="46.15234375" style="12" customWidth="1"/>
+    <col min="4" max="4" width="13.3828125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="14.3828125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="22.84375" style="22" customWidth="1"/>
+    <col min="7" max="7" width="12.3828125" style="22" customWidth="1"/>
+    <col min="8" max="8" width="21.3828125" style="22" customWidth="1"/>
+    <col min="9" max="9" width="25.3046875" style="22" customWidth="1"/>
+    <col min="10" max="10" width="13.15234375" style="22" customWidth="1"/>
+    <col min="11" max="11" width="18.765625" style="22" customWidth="1"/>
     <col min="12" max="12" width="23" style="22" customWidth="1"/>
-    <col min="13" max="13" width="38.7109375" style="22" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" style="22" customWidth="1"/>
-    <col min="15" max="15" width="53.85546875" style="22" customWidth="1"/>
-    <col min="16" max="16" width="16.140625" style="27" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" style="22" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" style="22" customWidth="1"/>
-    <col min="19" max="19" width="11.140625" style="22" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" style="22" customWidth="1"/>
-    <col min="21" max="16384" width="8.85546875" style="22"/>
+    <col min="13" max="13" width="38.69140625" style="22" customWidth="1"/>
+    <col min="14" max="14" width="10.15234375" style="22" customWidth="1"/>
+    <col min="15" max="15" width="53.84375" style="22" customWidth="1"/>
+    <col min="16" max="16" width="16.15234375" style="27" customWidth="1"/>
+    <col min="17" max="17" width="14.15234375" style="22" customWidth="1"/>
+    <col min="18" max="18" width="11.3828125" style="22" customWidth="1"/>
+    <col min="19" max="19" width="11.15234375" style="22" customWidth="1"/>
+    <col min="20" max="20" width="13.69140625" style="22" customWidth="1"/>
+    <col min="21" max="16384" width="8.84375" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="47.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>179</v>
       </c>
@@ -2239,12 +2273,12 @@
         <v>302</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="33" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+    <row r="2" spans="1:20" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="30" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="16" t="s">
         <v>2</v>
       </c>
@@ -2304,12 +2338,12 @@
       </c>
       <c r="T3" s="17"/>
     </row>
-    <row r="4" spans="1:20" s="33" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+    <row r="4" spans="1:20" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="30" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A5" s="16" t="s">
         <v>102</v>
       </c>
@@ -2369,7 +2403,7 @@
       </c>
       <c r="T5" s="17"/>
     </row>
-    <row r="6" spans="1:20" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A6" s="16" t="s">
         <v>189</v>
       </c>
@@ -2429,7 +2463,7 @@
       </c>
       <c r="T6" s="17"/>
     </row>
-    <row r="7" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="16" t="s">
         <v>26</v>
       </c>
@@ -2491,7 +2525,7 @@
         <v>42277</v>
       </c>
     </row>
-    <row r="8" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="16" t="s">
         <v>101</v>
       </c>
@@ -2551,14 +2585,14 @@
       </c>
       <c r="T8" s="17"/>
     </row>
-    <row r="9" spans="1:20" s="28" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" s="28" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A9" s="19" t="s">
         <v>499</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>499</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="36" t="s">
         <v>508</v>
       </c>
       <c r="D9" s="19" t="s">
@@ -2611,12 +2645,12 @@
       </c>
       <c r="T9" s="20"/>
     </row>
-    <row r="10" spans="1:20" s="33" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+    <row r="10" spans="1:20" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="30" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:20" s="28" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" s="28" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A11" s="19" t="s">
         <v>36</v>
       </c>
@@ -2676,7 +2710,7 @@
       </c>
       <c r="T11" s="17"/>
     </row>
-    <row r="12" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A12" s="16" t="s">
         <v>3</v>
       </c>
@@ -2736,7 +2770,7 @@
       </c>
       <c r="T12" s="17"/>
     </row>
-    <row r="13" spans="1:20" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A13" s="16" t="s">
         <v>63</v>
       </c>
@@ -2796,7 +2830,7 @@
       </c>
       <c r="T13" s="17"/>
     </row>
-    <row r="14" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="16" t="s">
         <v>14</v>
       </c>
@@ -2856,7 +2890,7 @@
       </c>
       <c r="T14" s="17"/>
     </row>
-    <row r="15" spans="1:20" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A15" s="16" t="s">
         <v>41</v>
       </c>
@@ -2916,7 +2950,7 @@
       </c>
       <c r="T15" s="17"/>
     </row>
-    <row r="16" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A16" s="16" t="s">
         <v>5</v>
       </c>
@@ -2976,7 +3010,7 @@
       </c>
       <c r="T16" s="17"/>
     </row>
-    <row r="17" spans="1:20" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A17" s="16" t="s">
         <v>276</v>
       </c>
@@ -3036,7 +3070,7 @@
       </c>
       <c r="T17" s="17"/>
     </row>
-    <row r="18" spans="1:20" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A18" s="16" t="s">
         <v>277</v>
       </c>
@@ -3096,14 +3130,14 @@
       </c>
       <c r="T18" s="17"/>
     </row>
-    <row r="19" spans="1:20" s="28" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" s="28" customFormat="1" ht="47.6" x14ac:dyDescent="0.4">
       <c r="A19" s="19" t="s">
         <v>488</v>
       </c>
       <c r="B19" s="19" t="s">
         <v>488</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="34" t="s">
         <v>489</v>
       </c>
       <c r="D19" s="19" t="s">
@@ -3156,7 +3190,7 @@
       </c>
       <c r="T19" s="20"/>
     </row>
-    <row r="20" spans="1:20" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A20" s="16" t="s">
         <v>18</v>
       </c>
@@ -3216,7 +3250,7 @@
       </c>
       <c r="T20" s="17"/>
     </row>
-    <row r="21" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A21" s="16" t="s">
         <v>2</v>
       </c>
@@ -3276,7 +3310,7 @@
       </c>
       <c r="T21" s="17"/>
     </row>
-    <row r="22" spans="1:20" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A22" s="16" t="s">
         <v>8</v>
       </c>
@@ -3336,7 +3370,7 @@
       </c>
       <c r="T22" s="17"/>
     </row>
-    <row r="23" spans="1:20" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A23" s="16" t="s">
         <v>285</v>
       </c>
@@ -3396,7 +3430,7 @@
       </c>
       <c r="T23" s="17"/>
     </row>
-    <row r="24" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A24" s="16" t="s">
         <v>9</v>
       </c>
@@ -3456,7 +3490,7 @@
       </c>
       <c r="T24" s="17"/>
     </row>
-    <row r="25" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A25" s="16" t="s">
         <v>11</v>
       </c>
@@ -3514,7 +3548,7 @@
       </c>
       <c r="T25" s="17"/>
     </row>
-    <row r="26" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A26" s="16" t="s">
         <v>39</v>
       </c>
@@ -3574,7 +3608,7 @@
       </c>
       <c r="T26" s="17"/>
     </row>
-    <row r="27" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="16" t="s">
         <v>226</v>
       </c>
@@ -3634,14 +3668,14 @@
       </c>
       <c r="T27" s="17"/>
     </row>
-    <row r="28" spans="1:20" s="28" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" s="28" customFormat="1" ht="47.6" x14ac:dyDescent="0.4">
       <c r="A28" s="19" t="s">
         <v>480</v>
       </c>
       <c r="B28" s="19" t="s">
         <v>480</v>
       </c>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="34" t="s">
         <v>481</v>
       </c>
       <c r="D28" s="19" t="s">
@@ -3694,7 +3728,7 @@
       </c>
       <c r="T28" s="20"/>
     </row>
-    <row r="29" spans="1:20" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A29" s="16" t="s">
         <v>19</v>
       </c>
@@ -3754,12 +3788,12 @@
       </c>
       <c r="T29" s="17"/>
     </row>
-    <row r="30" spans="1:20" s="33" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="32" t="s">
+    <row r="30" spans="1:20" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="30" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A31" s="16" t="s">
         <v>67</v>
       </c>
@@ -3819,84 +3853,84 @@
       </c>
       <c r="T31" s="17"/>
     </row>
-    <row r="32" spans="1:20" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="16" t="s">
+    <row r="32" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="19" t="s">
+        <v>509</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>510</v>
+      </c>
+      <c r="C32" s="37" t="s">
+        <v>517</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>509</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>516</v>
+      </c>
+      <c r="G32" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H32" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I32" s="19" t="s">
+        <v>515</v>
+      </c>
+      <c r="J32" s="19" t="s">
+        <v>518</v>
+      </c>
+      <c r="K32" s="19" t="s">
+        <v>484</v>
+      </c>
+      <c r="L32" s="19" t="s">
+        <v>511</v>
+      </c>
+      <c r="M32" s="19" t="s">
+        <v>512</v>
+      </c>
+      <c r="N32" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="O32" s="19" t="s">
+        <v>513</v>
+      </c>
+      <c r="P32" s="25">
+        <v>44193</v>
+      </c>
+      <c r="Q32" s="19" t="s">
+        <v>514</v>
+      </c>
+      <c r="R32" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="S32" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="T32" s="20"/>
+    </row>
+    <row r="33" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B33" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C33" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D33" s="16" t="s">
         <v>68</v>
-      </c>
-      <c r="E32" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F32" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="G32" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="H32" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="I32" s="16" t="s">
-        <v>209</v>
-      </c>
-      <c r="J32" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K32" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="L32" s="16" t="s">
-        <v>248</v>
-      </c>
-      <c r="M32" s="16" t="s">
-        <v>262</v>
-      </c>
-      <c r="N32" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="O32" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="P32" s="24">
-        <v>42119</v>
-      </c>
-      <c r="Q32" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="R32" s="16" t="s">
-        <v>304</v>
-      </c>
-      <c r="S32" s="16" t="s">
-        <v>304</v>
-      </c>
-      <c r="T32" s="17"/>
-    </row>
-    <row r="33" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>55</v>
       </c>
       <c r="E33" s="16" t="s">
         <v>25</v>
       </c>
       <c r="F33" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G33" s="16" t="s">
         <v>20</v>
@@ -3905,31 +3939,31 @@
         <v>12</v>
       </c>
       <c r="I33" s="16" t="s">
-        <v>119</v>
+        <v>209</v>
       </c>
       <c r="J33" s="16" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K33" s="16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="L33" s="16" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="M33" s="16" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="N33" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O33" s="16" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="P33" s="24">
-        <v>41837</v>
+        <v>42119</v>
       </c>
       <c r="Q33" s="16" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="R33" s="16" t="s">
         <v>304</v>
@@ -3939,15 +3973,15 @@
       </c>
       <c r="T33" s="17"/>
     </row>
-    <row r="34" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A34" s="16" t="s">
         <v>55</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="D34" s="16" t="s">
         <v>55</v>
@@ -3983,7 +4017,7 @@
         <v>110</v>
       </c>
       <c r="O34" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P34" s="24">
         <v>41837</v>
@@ -3999,24 +4033,24 @@
       </c>
       <c r="T34" s="17"/>
     </row>
-    <row r="35" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A35" s="16" t="s">
-        <v>474</v>
+        <v>55</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>475</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>476</v>
+        <v>55</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>78</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>474</v>
+        <v>55</v>
       </c>
       <c r="E35" s="16" t="s">
         <v>25</v>
       </c>
       <c r="F35" s="16" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="G35" s="16" t="s">
         <v>20</v>
@@ -4025,31 +4059,31 @@
         <v>12</v>
       </c>
       <c r="I35" s="16" t="s">
-        <v>477</v>
+        <v>119</v>
       </c>
       <c r="J35" s="16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K35" s="16" t="s">
-        <v>478</v>
+        <v>126</v>
       </c>
       <c r="L35" s="16" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="M35" s="16" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="N35" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O35" s="16" t="s">
-        <v>479</v>
+        <v>153</v>
       </c>
       <c r="P35" s="24">
-        <v>43935</v>
+        <v>41837</v>
       </c>
       <c r="Q35" s="16" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="R35" s="16" t="s">
         <v>304</v>
@@ -4059,18 +4093,18 @@
       </c>
       <c r="T35" s="17"/>
     </row>
-    <row r="36" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A36" s="16" t="s">
-        <v>34</v>
+        <v>474</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>91</v>
+        <v>475</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>476</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>34</v>
+        <v>474</v>
       </c>
       <c r="E36" s="16" t="s">
         <v>25</v>
@@ -4085,31 +4119,31 @@
         <v>12</v>
       </c>
       <c r="I36" s="16" t="s">
-        <v>210</v>
+        <v>477</v>
       </c>
       <c r="J36" s="16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K36" s="16" t="s">
-        <v>128</v>
+        <v>478</v>
       </c>
       <c r="L36" s="16" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="M36" s="16" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="N36" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O36" s="16" t="s">
-        <v>155</v>
+        <v>479</v>
       </c>
       <c r="P36" s="24">
-        <v>41600</v>
+        <v>43935</v>
       </c>
       <c r="Q36" s="16" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="R36" s="16" t="s">
         <v>304</v>
@@ -4119,18 +4153,18 @@
       </c>
       <c r="T36" s="17"/>
     </row>
-    <row r="37" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A37" s="16" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="E37" s="16" t="s">
         <v>25</v>
@@ -4145,7 +4179,7 @@
         <v>12</v>
       </c>
       <c r="I37" s="16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J37" s="16" t="s">
         <v>5</v>
@@ -4163,13 +4197,13 @@
         <v>110</v>
       </c>
       <c r="O37" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P37" s="24">
-        <v>42220</v>
+        <v>41600</v>
       </c>
       <c r="Q37" s="16" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="R37" s="16" t="s">
         <v>304</v>
@@ -4179,24 +4213,24 @@
       </c>
       <c r="T37" s="17"/>
     </row>
-    <row r="38" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A38" s="16" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E38" s="16" t="s">
         <v>25</v>
       </c>
       <c r="F38" s="16" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="G38" s="16" t="s">
         <v>20</v>
@@ -4205,31 +4239,31 @@
         <v>12</v>
       </c>
       <c r="I38" s="16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J38" s="16" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K38" s="16" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="L38" s="16" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="M38" s="16" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="N38" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O38" s="16" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="P38" s="24">
-        <v>42158</v>
+        <v>42220</v>
       </c>
       <c r="Q38" s="16" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="R38" s="16" t="s">
         <v>304</v>
@@ -4239,15 +4273,15 @@
       </c>
       <c r="T38" s="17"/>
     </row>
-    <row r="39" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A39" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="D39" s="16" t="s">
         <v>43</v>
@@ -4283,7 +4317,7 @@
         <v>110</v>
       </c>
       <c r="O39" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="P39" s="24">
         <v>42158</v>
@@ -4299,24 +4333,24 @@
       </c>
       <c r="T39" s="17"/>
     </row>
-    <row r="40" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A40" s="16" t="s">
-        <v>234</v>
+        <v>43</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>235</v>
+        <v>43</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>236</v>
+        <v>79</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>234</v>
+        <v>43</v>
       </c>
       <c r="E40" s="16" t="s">
         <v>25</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>237</v>
+        <v>120</v>
       </c>
       <c r="G40" s="16" t="s">
         <v>20</v>
@@ -4325,31 +4359,31 @@
         <v>12</v>
       </c>
       <c r="I40" s="16" t="s">
-        <v>238</v>
+        <v>213</v>
       </c>
       <c r="J40" s="16" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K40" s="16" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="L40" s="16" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="M40" s="16" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="N40" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O40" s="16" t="s">
-        <v>239</v>
+        <v>159</v>
       </c>
       <c r="P40" s="24">
-        <v>42650</v>
+        <v>42158</v>
       </c>
       <c r="Q40" s="16" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="R40" s="16" t="s">
         <v>304</v>
@@ -4359,24 +4393,24 @@
       </c>
       <c r="T40" s="17"/>
     </row>
-    <row r="41" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A41" s="16" t="s">
-        <v>35</v>
+        <v>234</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>50</v>
+        <v>235</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>94</v>
+        <v>236</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>35</v>
+        <v>234</v>
       </c>
       <c r="E41" s="16" t="s">
         <v>25</v>
       </c>
       <c r="F41" s="16" t="s">
-        <v>110</v>
+        <v>237</v>
       </c>
       <c r="G41" s="16" t="s">
         <v>20</v>
@@ -4385,31 +4419,31 @@
         <v>12</v>
       </c>
       <c r="I41" s="16" t="s">
-        <v>212</v>
+        <v>238</v>
       </c>
       <c r="J41" s="16" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="K41" s="16" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="L41" s="16" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="M41" s="16" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="N41" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O41" s="16" t="s">
-        <v>157</v>
+        <v>239</v>
       </c>
       <c r="P41" s="24">
-        <v>41771</v>
+        <v>42650</v>
       </c>
       <c r="Q41" s="16" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="R41" s="16" t="s">
         <v>304</v>
@@ -4419,83 +4453,84 @@
       </c>
       <c r="T41" s="17"/>
     </row>
-    <row r="42" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A42" s="16" t="s">
-        <v>305</v>
+        <v>35</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>305</v>
-      </c>
-      <c r="C42" s="29" t="s">
-        <v>306</v>
+        <v>50</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>94</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>305</v>
+        <v>35</v>
       </c>
       <c r="E42" s="16" t="s">
-        <v>303</v>
+        <v>25</v>
       </c>
       <c r="F42" s="16" t="s">
-        <v>307</v>
+        <v>110</v>
       </c>
       <c r="G42" s="16" t="s">
         <v>20</v>
       </c>
       <c r="H42" s="16" t="s">
-        <v>175</v>
+        <v>12</v>
       </c>
       <c r="I42" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="J42" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="K42" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="L42" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="M42" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="N42" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="O42" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="P42" s="24">
+        <v>41771</v>
+      </c>
+      <c r="Q42" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="R42" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="S42" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="T42" s="17"/>
+    </row>
+    <row r="43" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+      <c r="A43" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="J42" s="16" t="s">
+      <c r="B43" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="K42" s="16" t="s">
+      <c r="C43" s="35" t="s">
+        <v>306</v>
+      </c>
+      <c r="D43" s="16" t="s">
         <v>305</v>
-      </c>
-      <c r="L42" s="16" t="s">
-        <v>308</v>
-      </c>
-      <c r="M42" s="16" t="s">
-        <v>472</v>
-      </c>
-      <c r="N42" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="O42" s="16" t="s">
-        <v>309</v>
-      </c>
-      <c r="P42" s="24">
-        <v>43788</v>
-      </c>
-      <c r="Q42" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="R42" s="16" t="s">
-        <v>304</v>
-      </c>
-      <c r="S42" s="16" t="s">
-        <v>310</v>
-      </c>
-      <c r="T42" s="17"/>
-      <c r="U42" s="30"/>
-    </row>
-    <row r="43" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="B43" s="16"/>
-      <c r="C43" s="29" t="s">
-        <v>312</v>
-      </c>
-      <c r="D43" s="16" t="s">
-        <v>313</v>
       </c>
       <c r="E43" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F43" s="16" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="G43" s="16" t="s">
         <v>20</v>
@@ -4516,45 +4551,45 @@
         <v>308</v>
       </c>
       <c r="M43" s="16" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="N43" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O43" s="16" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="P43" s="24">
         <v>43788</v>
       </c>
       <c r="Q43" s="16" t="s">
-        <v>316</v>
+        <v>27</v>
       </c>
       <c r="R43" s="16" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="S43" s="16" t="s">
         <v>310</v>
       </c>
       <c r="T43" s="17"/>
-      <c r="U43" s="30"/>
-    </row>
-    <row r="44" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U43" s="29"/>
+    </row>
+    <row r="44" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A44" s="16" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="B44" s="16"/>
-      <c r="C44" s="29" t="s">
-        <v>318</v>
+      <c r="C44" s="35" t="s">
+        <v>312</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="E44" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F44" s="16" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="G44" s="16" t="s">
         <v>20</v>
@@ -4562,9 +4597,15 @@
       <c r="H44" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="I44" s="16"/>
-      <c r="J44" s="16"/>
-      <c r="K44" s="16"/>
+      <c r="I44" s="16" t="s">
+        <v>305</v>
+      </c>
+      <c r="J44" s="16" t="s">
+        <v>305</v>
+      </c>
+      <c r="K44" s="16" t="s">
+        <v>305</v>
+      </c>
       <c r="L44" s="16" t="s">
         <v>308</v>
       </c>
@@ -4575,7 +4616,7 @@
         <v>110</v>
       </c>
       <c r="O44" s="16" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="P44" s="24">
         <v>43788</v>
@@ -4584,30 +4625,30 @@
         <v>316</v>
       </c>
       <c r="R44" s="16" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="S44" s="16" t="s">
         <v>310</v>
       </c>
       <c r="T44" s="17"/>
-      <c r="U44" s="30"/>
-    </row>
-    <row r="45" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U44" s="29"/>
+    </row>
+    <row r="45" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A45" s="16" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B45" s="16"/>
-      <c r="C45" s="29" t="s">
-        <v>323</v>
+      <c r="C45" s="35" t="s">
+        <v>318</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="E45" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F45" s="16" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="G45" s="16" t="s">
         <v>20</v>
@@ -4628,7 +4669,7 @@
         <v>110</v>
       </c>
       <c r="O45" s="16" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="P45" s="24">
         <v>43788</v>
@@ -4637,30 +4678,30 @@
         <v>316</v>
       </c>
       <c r="R45" s="16" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="S45" s="16" t="s">
         <v>310</v>
       </c>
       <c r="T45" s="17"/>
-      <c r="U45" s="30"/>
-    </row>
-    <row r="46" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U45" s="29"/>
+    </row>
+    <row r="46" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A46" s="16" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="B46" s="16"/>
-      <c r="C46" s="29" t="s">
-        <v>328</v>
+      <c r="C46" s="35" t="s">
+        <v>323</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="E46" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F46" s="16" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="G46" s="16" t="s">
         <v>20</v>
@@ -4681,7 +4722,7 @@
         <v>110</v>
       </c>
       <c r="O46" s="16" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="P46" s="24">
         <v>43788</v>
@@ -4696,24 +4737,24 @@
         <v>310</v>
       </c>
       <c r="T46" s="17"/>
-      <c r="U46" s="30"/>
-    </row>
-    <row r="47" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U46" s="29"/>
+    </row>
+    <row r="47" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A47" s="16" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="B47" s="16"/>
-      <c r="C47" s="29" t="s">
-        <v>333</v>
+      <c r="C47" s="35" t="s">
+        <v>328</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="E47" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F47" s="16" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="G47" s="16" t="s">
         <v>20</v>
@@ -4734,7 +4775,7 @@
         <v>110</v>
       </c>
       <c r="O47" s="16" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="P47" s="24">
         <v>43788</v>
@@ -4749,24 +4790,24 @@
         <v>310</v>
       </c>
       <c r="T47" s="17"/>
-      <c r="U47" s="30"/>
-    </row>
-    <row r="48" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U47" s="29"/>
+    </row>
+    <row r="48" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A48" s="16" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="B48" s="16"/>
-      <c r="C48" s="29" t="s">
-        <v>338</v>
+      <c r="C48" s="35" t="s">
+        <v>333</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="E48" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F48" s="16" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="G48" s="16" t="s">
         <v>20</v>
@@ -4787,7 +4828,7 @@
         <v>110</v>
       </c>
       <c r="O48" s="16" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="P48" s="24">
         <v>43788</v>
@@ -4802,24 +4843,24 @@
         <v>310</v>
       </c>
       <c r="T48" s="17"/>
-      <c r="U48" s="30"/>
-    </row>
-    <row r="49" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U48" s="29"/>
+    </row>
+    <row r="49" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A49" s="16" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="B49" s="16"/>
-      <c r="C49" s="29" t="s">
-        <v>343</v>
+      <c r="C49" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="E49" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F49" s="16" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G49" s="16" t="s">
         <v>20</v>
@@ -4840,7 +4881,7 @@
         <v>110</v>
       </c>
       <c r="O49" s="16" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="P49" s="24">
         <v>43788</v>
@@ -4855,24 +4896,24 @@
         <v>310</v>
       </c>
       <c r="T49" s="17"/>
-      <c r="U49" s="30"/>
-    </row>
-    <row r="50" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U49" s="29"/>
+    </row>
+    <row r="50" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A50" s="16" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="B50" s="16"/>
-      <c r="C50" s="29" t="s">
-        <v>348</v>
+      <c r="C50" s="35" t="s">
+        <v>343</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="E50" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F50" s="16" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="G50" s="16" t="s">
         <v>20</v>
@@ -4893,7 +4934,7 @@
         <v>110</v>
       </c>
       <c r="O50" s="16" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="P50" s="24">
         <v>43788</v>
@@ -4908,24 +4949,24 @@
         <v>310</v>
       </c>
       <c r="T50" s="17"/>
-      <c r="U50" s="30"/>
-    </row>
-    <row r="51" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U50" s="29"/>
+    </row>
+    <row r="51" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A51" s="16" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="B51" s="16"/>
-      <c r="C51" s="29" t="s">
-        <v>353</v>
+      <c r="C51" s="35" t="s">
+        <v>348</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="E51" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F51" s="16" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="G51" s="16" t="s">
         <v>20</v>
@@ -4946,7 +4987,7 @@
         <v>110</v>
       </c>
       <c r="O51" s="16" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="P51" s="24">
         <v>43788</v>
@@ -4961,24 +5002,24 @@
         <v>310</v>
       </c>
       <c r="T51" s="17"/>
-      <c r="U51" s="30"/>
-    </row>
-    <row r="52" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U51" s="29"/>
+    </row>
+    <row r="52" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A52" s="16" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="B52" s="16"/>
-      <c r="C52" s="29" t="s">
-        <v>358</v>
+      <c r="C52" s="35" t="s">
+        <v>353</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="E52" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F52" s="16" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="G52" s="16" t="s">
         <v>20</v>
@@ -4999,7 +5040,7 @@
         <v>110</v>
       </c>
       <c r="O52" s="16" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="P52" s="24">
         <v>43788</v>
@@ -5014,24 +5055,24 @@
         <v>310</v>
       </c>
       <c r="T52" s="17"/>
-      <c r="U52" s="30"/>
-    </row>
-    <row r="53" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U52" s="29"/>
+    </row>
+    <row r="53" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A53" s="16" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="B53" s="16"/>
-      <c r="C53" s="29" t="s">
-        <v>363</v>
+      <c r="C53" s="35" t="s">
+        <v>358</v>
       </c>
       <c r="D53" s="16" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="E53" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F53" s="16" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="G53" s="16" t="s">
         <v>20</v>
@@ -5052,7 +5093,7 @@
         <v>110</v>
       </c>
       <c r="O53" s="16" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="P53" s="24">
         <v>43788</v>
@@ -5067,24 +5108,24 @@
         <v>310</v>
       </c>
       <c r="T53" s="17"/>
-      <c r="U53" s="30"/>
-    </row>
-    <row r="54" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U53" s="29"/>
+    </row>
+    <row r="54" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A54" s="16" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="B54" s="16"/>
-      <c r="C54" s="29" t="s">
-        <v>368</v>
+      <c r="C54" s="35" t="s">
+        <v>363</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="E54" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F54" s="16" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="G54" s="16" t="s">
         <v>20</v>
@@ -5105,7 +5146,7 @@
         <v>110</v>
       </c>
       <c r="O54" s="16" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="P54" s="24">
         <v>43788</v>
@@ -5120,24 +5161,24 @@
         <v>310</v>
       </c>
       <c r="T54" s="17"/>
-      <c r="U54" s="30"/>
-    </row>
-    <row r="55" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U54" s="29"/>
+    </row>
+    <row r="55" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A55" s="16" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="B55" s="16"/>
-      <c r="C55" s="29" t="s">
-        <v>373</v>
+      <c r="C55" s="35" t="s">
+        <v>368</v>
       </c>
       <c r="D55" s="16" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="E55" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F55" s="16" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="G55" s="16" t="s">
         <v>20</v>
@@ -5158,7 +5199,7 @@
         <v>110</v>
       </c>
       <c r="O55" s="16" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="P55" s="24">
         <v>43788</v>
@@ -5173,174 +5214,168 @@
         <v>310</v>
       </c>
       <c r="T55" s="17"/>
-      <c r="U55" s="30"/>
-    </row>
-    <row r="56" spans="1:21" s="28" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A56" s="19" t="s">
+      <c r="U55" s="29"/>
+    </row>
+    <row r="56" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+      <c r="A56" s="16" t="s">
+        <v>372</v>
+      </c>
+      <c r="B56" s="16"/>
+      <c r="C56" s="35" t="s">
+        <v>373</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>374</v>
+      </c>
+      <c r="E56" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="F56" s="16" t="s">
+        <v>375</v>
+      </c>
+      <c r="G56" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H56" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="I56" s="16"/>
+      <c r="J56" s="16"/>
+      <c r="K56" s="16"/>
+      <c r="L56" s="16" t="s">
+        <v>308</v>
+      </c>
+      <c r="M56" s="16" t="s">
+        <v>471</v>
+      </c>
+      <c r="N56" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="O56" s="16" t="s">
+        <v>376</v>
+      </c>
+      <c r="P56" s="24">
+        <v>43788</v>
+      </c>
+      <c r="Q56" s="16" t="s">
+        <v>316</v>
+      </c>
+      <c r="R56" s="16" t="s">
+        <v>310</v>
+      </c>
+      <c r="S56" s="16" t="s">
+        <v>310</v>
+      </c>
+      <c r="T56" s="17"/>
+      <c r="U56" s="29"/>
+    </row>
+    <row r="57" spans="1:21" s="28" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+      <c r="A57" s="19" t="s">
         <v>492</v>
       </c>
-      <c r="B56" s="19" t="s">
+      <c r="B57" s="19" t="s">
         <v>493</v>
       </c>
-      <c r="C56" s="28" t="s">
+      <c r="C57" s="34" t="s">
         <v>494</v>
       </c>
-      <c r="D56" s="19" t="s">
+      <c r="D57" s="19" t="s">
         <v>492</v>
       </c>
-      <c r="E56" s="19" t="s">
+      <c r="E57" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F56" s="19" t="s">
+      <c r="F57" s="19" t="s">
         <v>498</v>
       </c>
-      <c r="G56" s="19" t="s">
+      <c r="G57" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H56" s="19" t="s">
+      <c r="H57" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="I56" s="19" t="s">
+      <c r="I57" s="19" t="s">
         <v>492</v>
       </c>
-      <c r="J56" s="19" t="s">
+      <c r="J57" s="19" t="s">
         <v>492</v>
       </c>
-      <c r="K56" s="19" t="s">
+      <c r="K57" s="19" t="s">
         <v>495</v>
       </c>
-      <c r="L56" s="19" t="s">
+      <c r="L57" s="19" t="s">
         <v>496</v>
       </c>
-      <c r="M56" s="19" t="s">
+      <c r="M57" s="19" t="s">
         <v>262</v>
       </c>
-      <c r="N56" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="O56" s="19" t="s">
+      <c r="N57" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="O57" s="19" t="s">
         <v>497</v>
       </c>
-      <c r="P56" s="25">
+      <c r="P57" s="25">
         <v>44111</v>
       </c>
-      <c r="Q56" s="19" t="s">
+      <c r="Q57" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="R56" s="19" t="s">
-        <v>304</v>
-      </c>
-      <c r="S56" s="19" t="s">
-        <v>304</v>
-      </c>
-      <c r="T56" s="20"/>
-    </row>
-    <row r="57" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="16"/>
-      <c r="B57" s="16"/>
-      <c r="C57" s="16"/>
-      <c r="D57" s="16"/>
-      <c r="E57" s="16"/>
-      <c r="F57" s="16"/>
-      <c r="G57" s="16"/>
-      <c r="H57" s="16"/>
-      <c r="I57" s="16"/>
-      <c r="J57" s="16"/>
-      <c r="K57" s="16"/>
-      <c r="L57" s="16"/>
-      <c r="M57" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="N57" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="O57" s="16"/>
-      <c r="P57" s="24">
-        <v>43788</v>
-      </c>
-      <c r="Q57" s="16"/>
-      <c r="R57" s="16"/>
-      <c r="S57" s="16"/>
-      <c r="T57" s="17"/>
-      <c r="U57" s="30"/>
-    </row>
-    <row r="58" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="B58" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="C58" s="29" t="s">
-        <v>378</v>
-      </c>
-      <c r="D58" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="E58" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="F58" s="16" t="s">
-        <v>379</v>
-      </c>
-      <c r="G58" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="H58" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="I58" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="J58" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="K58" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="L58" s="16" t="s">
-        <v>380</v>
-      </c>
+      <c r="R57" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="S57" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="T57" s="20"/>
+    </row>
+    <row r="58" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="16"/>
+      <c r="B58" s="16"/>
+      <c r="C58" s="16"/>
+      <c r="D58" s="16"/>
+      <c r="E58" s="16"/>
+      <c r="F58" s="16"/>
+      <c r="G58" s="16"/>
+      <c r="H58" s="16"/>
+      <c r="I58" s="16"/>
+      <c r="J58" s="16"/>
+      <c r="K58" s="16"/>
+      <c r="L58" s="16"/>
       <c r="M58" s="16" t="s">
-        <v>257</v>
+        <v>110</v>
       </c>
       <c r="N58" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="O58" s="16" t="s">
-        <v>381</v>
-      </c>
+      <c r="O58" s="16"/>
       <c r="P58" s="24">
         <v>43788</v>
       </c>
-      <c r="Q58" s="16" t="s">
-        <v>382</v>
-      </c>
-      <c r="R58" s="16" t="s">
-        <v>304</v>
-      </c>
-      <c r="S58" s="16" t="s">
-        <v>310</v>
-      </c>
+      <c r="Q58" s="16"/>
+      <c r="R58" s="16"/>
+      <c r="S58" s="16"/>
       <c r="T58" s="17"/>
-      <c r="U58" s="30"/>
-    </row>
-    <row r="59" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U58" s="29"/>
+    </row>
+    <row r="59" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A59" s="16" t="s">
-        <v>383</v>
-      </c>
-      <c r="B59" s="16"/>
-      <c r="C59" s="29" t="s">
-        <v>384</v>
+        <v>377</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="C59" s="35" t="s">
+        <v>378</v>
       </c>
       <c r="D59" s="16" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="E59" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F59" s="16" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="G59" s="16" t="s">
         <v>20</v>
@@ -5361,19 +5396,19 @@
         <v>380</v>
       </c>
       <c r="M59" s="16" t="s">
-        <v>470</v>
+        <v>257</v>
       </c>
       <c r="N59" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O59" s="16" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="P59" s="24">
         <v>43788</v>
       </c>
       <c r="Q59" s="16" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="R59" s="16" t="s">
         <v>304</v>
@@ -5382,24 +5417,24 @@
         <v>310</v>
       </c>
       <c r="T59" s="17"/>
-      <c r="U59" s="30"/>
-    </row>
-    <row r="60" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U59" s="29"/>
+    </row>
+    <row r="60" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A60" s="16" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="B60" s="16"/>
-      <c r="C60" s="29" t="s">
-        <v>390</v>
+      <c r="C60" s="35" t="s">
+        <v>384</v>
       </c>
       <c r="D60" s="16" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="E60" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F60" s="16" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="G60" s="16" t="s">
         <v>20</v>
@@ -5420,19 +5455,19 @@
         <v>380</v>
       </c>
       <c r="M60" s="16" t="s">
-        <v>257</v>
+        <v>470</v>
       </c>
       <c r="N60" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O60" s="16" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="P60" s="24">
         <v>43788</v>
       </c>
       <c r="Q60" s="16" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="R60" s="16" t="s">
         <v>304</v>
@@ -5441,24 +5476,24 @@
         <v>310</v>
       </c>
       <c r="T60" s="17"/>
-      <c r="U60" s="30"/>
-    </row>
-    <row r="61" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U60" s="29"/>
+    </row>
+    <row r="61" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A61" s="16" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="B61" s="16"/>
-      <c r="C61" s="29" t="s">
-        <v>395</v>
+      <c r="C61" s="35" t="s">
+        <v>390</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="E61" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F61" s="16" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="G61" s="16" t="s">
         <v>20</v>
@@ -5485,7 +5520,7 @@
         <v>110</v>
       </c>
       <c r="O61" s="16" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="P61" s="24">
         <v>43788</v>
@@ -5500,24 +5535,24 @@
         <v>310</v>
       </c>
       <c r="T61" s="17"/>
-      <c r="U61" s="30"/>
-    </row>
-    <row r="62" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U61" s="29"/>
+    </row>
+    <row r="62" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A62" s="16" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="B62" s="16"/>
-      <c r="C62" s="29" t="s">
-        <v>400</v>
+      <c r="C62" s="35" t="s">
+        <v>395</v>
       </c>
       <c r="D62" s="16" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="E62" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F62" s="16" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="G62" s="16" t="s">
         <v>20</v>
@@ -5538,19 +5573,19 @@
         <v>380</v>
       </c>
       <c r="M62" s="16" t="s">
-        <v>470</v>
+        <v>257</v>
       </c>
       <c r="N62" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O62" s="16" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="P62" s="24">
         <v>43788</v>
       </c>
       <c r="Q62" s="16" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="R62" s="16" t="s">
         <v>304</v>
@@ -5559,114 +5594,114 @@
         <v>310</v>
       </c>
       <c r="T62" s="17"/>
-      <c r="U62" s="30"/>
-    </row>
-    <row r="63" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="16"/>
+      <c r="U62" s="29"/>
+    </row>
+    <row r="63" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+      <c r="A63" s="16" t="s">
+        <v>399</v>
+      </c>
       <c r="B63" s="16"/>
-      <c r="C63" s="16"/>
-      <c r="D63" s="16"/>
-      <c r="E63" s="16"/>
-      <c r="F63" s="16"/>
-      <c r="G63" s="16"/>
-      <c r="H63" s="16"/>
-      <c r="I63" s="16"/>
-      <c r="J63" s="16"/>
-      <c r="K63" s="16"/>
-      <c r="L63" s="16"/>
+      <c r="C63" s="35" t="s">
+        <v>400</v>
+      </c>
+      <c r="D63" s="16" t="s">
+        <v>401</v>
+      </c>
+      <c r="E63" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="F63" s="16" t="s">
+        <v>402</v>
+      </c>
+      <c r="G63" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H63" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="I63" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="J63" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="K63" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="L63" s="16" t="s">
+        <v>380</v>
+      </c>
       <c r="M63" s="16" t="s">
-        <v>257</v>
+        <v>470</v>
       </c>
       <c r="N63" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="O63" s="16"/>
+      <c r="O63" s="16" t="s">
+        <v>403</v>
+      </c>
       <c r="P63" s="24">
         <v>43788</v>
       </c>
-      <c r="Q63" s="16"/>
-      <c r="R63" s="16"/>
-      <c r="S63" s="16"/>
+      <c r="Q63" s="16" t="s">
+        <v>388</v>
+      </c>
+      <c r="R63" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="S63" s="16" t="s">
+        <v>310</v>
+      </c>
       <c r="T63" s="17"/>
-      <c r="U63" s="30"/>
-    </row>
-    <row r="64" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="16" t="s">
-        <v>404</v>
-      </c>
-      <c r="B64" s="16" t="s">
-        <v>404</v>
-      </c>
-      <c r="C64" s="29" t="s">
-        <v>405</v>
-      </c>
-      <c r="D64" s="16" t="s">
-        <v>404</v>
-      </c>
-      <c r="E64" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="F64" s="16" t="s">
-        <v>406</v>
-      </c>
-      <c r="G64" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="H64" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="I64" s="16" t="s">
-        <v>404</v>
-      </c>
-      <c r="J64" s="16" t="s">
-        <v>404</v>
-      </c>
-      <c r="K64" s="16" t="s">
-        <v>404</v>
-      </c>
-      <c r="L64" s="16" t="s">
-        <v>407</v>
-      </c>
+      <c r="U63" s="29"/>
+    </row>
+    <row r="64" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A64" s="16"/>
+      <c r="B64" s="16"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="16"/>
+      <c r="H64" s="16"/>
+      <c r="I64" s="16"/>
+      <c r="J64" s="16"/>
+      <c r="K64" s="16"/>
+      <c r="L64" s="16"/>
       <c r="M64" s="16" t="s">
         <v>257</v>
       </c>
       <c r="N64" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="O64" s="16" t="s">
-        <v>408</v>
-      </c>
+      <c r="O64" s="16"/>
       <c r="P64" s="24">
         <v>43788</v>
       </c>
-      <c r="Q64" s="16" t="s">
-        <v>382</v>
-      </c>
-      <c r="R64" s="16" t="s">
-        <v>310</v>
-      </c>
-      <c r="S64" s="16" t="s">
-        <v>310</v>
-      </c>
+      <c r="Q64" s="16"/>
+      <c r="R64" s="16"/>
+      <c r="S64" s="16"/>
       <c r="T64" s="17"/>
-      <c r="U64" s="30"/>
-    </row>
-    <row r="65" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U64" s="29"/>
+    </row>
+    <row r="65" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A65" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="B65" s="16"/>
-      <c r="C65" s="29" t="s">
-        <v>410</v>
+        <v>404</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="C65" s="35" t="s">
+        <v>405</v>
       </c>
       <c r="D65" s="16" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="E65" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F65" s="16" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="G65" s="16" t="s">
         <v>20</v>
@@ -5693,7 +5728,7 @@
         <v>110</v>
       </c>
       <c r="O65" s="16" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="P65" s="24">
         <v>43788</v>
@@ -5702,30 +5737,30 @@
         <v>382</v>
       </c>
       <c r="R65" s="16" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="S65" s="16" t="s">
         <v>310</v>
       </c>
       <c r="T65" s="17"/>
-      <c r="U65" s="30"/>
-    </row>
-    <row r="66" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U65" s="29"/>
+    </row>
+    <row r="66" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A66" s="16" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="B66" s="16"/>
-      <c r="C66" s="29" t="s">
-        <v>415</v>
+      <c r="C66" s="35" t="s">
+        <v>410</v>
       </c>
       <c r="D66" s="16" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="E66" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F66" s="16" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="G66" s="16" t="s">
         <v>20</v>
@@ -5752,7 +5787,7 @@
         <v>110</v>
       </c>
       <c r="O66" s="16" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="P66" s="24">
         <v>43788</v>
@@ -5761,30 +5796,30 @@
         <v>382</v>
       </c>
       <c r="R66" s="16" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="S66" s="16" t="s">
         <v>310</v>
       </c>
       <c r="T66" s="17"/>
-      <c r="U66" s="30"/>
-    </row>
-    <row r="67" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U66" s="29"/>
+    </row>
+    <row r="67" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A67" s="16" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B67" s="16"/>
-      <c r="C67" s="29" t="s">
-        <v>420</v>
+      <c r="C67" s="35" t="s">
+        <v>415</v>
       </c>
       <c r="D67" s="16" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="E67" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F67" s="16" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="G67" s="16" t="s">
         <v>20</v>
@@ -5811,7 +5846,7 @@
         <v>110</v>
       </c>
       <c r="O67" s="16" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="P67" s="24">
         <v>43788</v>
@@ -5826,24 +5861,24 @@
         <v>310</v>
       </c>
       <c r="T67" s="17"/>
-      <c r="U67" s="30"/>
-    </row>
-    <row r="68" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U67" s="29"/>
+    </row>
+    <row r="68" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A68" s="16" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B68" s="16"/>
-      <c r="C68" s="29" t="s">
-        <v>425</v>
+      <c r="C68" s="35" t="s">
+        <v>420</v>
       </c>
       <c r="D68" s="16" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="E68" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F68" s="16" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="G68" s="16" t="s">
         <v>20</v>
@@ -5870,7 +5905,7 @@
         <v>110</v>
       </c>
       <c r="O68" s="16" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="P68" s="24">
         <v>43788</v>
@@ -5885,24 +5920,24 @@
         <v>310</v>
       </c>
       <c r="T68" s="17"/>
-      <c r="U68" s="30"/>
-    </row>
-    <row r="69" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U68" s="29"/>
+    </row>
+    <row r="69" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A69" s="16" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="B69" s="16"/>
-      <c r="C69" s="29" t="s">
-        <v>430</v>
+      <c r="C69" s="35" t="s">
+        <v>425</v>
       </c>
       <c r="D69" s="16" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="E69" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F69" s="16" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="G69" s="16" t="s">
         <v>20</v>
@@ -5929,7 +5964,7 @@
         <v>110</v>
       </c>
       <c r="O69" s="16" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="P69" s="24">
         <v>43788</v>
@@ -5944,24 +5979,24 @@
         <v>310</v>
       </c>
       <c r="T69" s="17"/>
-      <c r="U69" s="30"/>
-    </row>
-    <row r="70" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U69" s="29"/>
+    </row>
+    <row r="70" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A70" s="16" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="B70" s="16"/>
-      <c r="C70" s="29" t="s">
-        <v>435</v>
+      <c r="C70" s="35" t="s">
+        <v>430</v>
       </c>
       <c r="D70" s="16" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="E70" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F70" s="16" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="G70" s="16" t="s">
         <v>20</v>
@@ -5988,7 +6023,7 @@
         <v>110</v>
       </c>
       <c r="O70" s="16" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="P70" s="24">
         <v>43788</v>
@@ -6003,24 +6038,24 @@
         <v>310</v>
       </c>
       <c r="T70" s="17"/>
-      <c r="U70" s="30"/>
-    </row>
-    <row r="71" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U70" s="29"/>
+    </row>
+    <row r="71" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A71" s="16" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B71" s="16"/>
-      <c r="C71" s="29" t="s">
-        <v>440</v>
+      <c r="C71" s="35" t="s">
+        <v>435</v>
       </c>
       <c r="D71" s="16" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="E71" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F71" s="16" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="G71" s="16" t="s">
         <v>20</v>
@@ -6047,7 +6082,7 @@
         <v>110</v>
       </c>
       <c r="O71" s="16" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="P71" s="24">
         <v>43788</v>
@@ -6062,24 +6097,24 @@
         <v>310</v>
       </c>
       <c r="T71" s="17"/>
-      <c r="U71" s="30"/>
-    </row>
-    <row r="72" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U71" s="29"/>
+    </row>
+    <row r="72" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A72" s="16" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="B72" s="16"/>
-      <c r="C72" s="29" t="s">
-        <v>445</v>
+      <c r="C72" s="35" t="s">
+        <v>440</v>
       </c>
       <c r="D72" s="16" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="E72" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F72" s="16" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="G72" s="16" t="s">
         <v>20</v>
@@ -6106,7 +6141,7 @@
         <v>110</v>
       </c>
       <c r="O72" s="16" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="P72" s="24">
         <v>43788</v>
@@ -6121,24 +6156,24 @@
         <v>310</v>
       </c>
       <c r="T72" s="17"/>
-      <c r="U72" s="30"/>
-    </row>
-    <row r="73" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U72" s="29"/>
+    </row>
+    <row r="73" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A73" s="16" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="B73" s="16"/>
-      <c r="C73" s="29" t="s">
-        <v>450</v>
+      <c r="C73" s="35" t="s">
+        <v>445</v>
       </c>
       <c r="D73" s="16" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="E73" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F73" s="16" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="G73" s="16" t="s">
         <v>20</v>
@@ -6165,7 +6200,7 @@
         <v>110</v>
       </c>
       <c r="O73" s="16" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="P73" s="24">
         <v>43788</v>
@@ -6180,24 +6215,24 @@
         <v>310</v>
       </c>
       <c r="T73" s="17"/>
-      <c r="U73" s="30"/>
-    </row>
-    <row r="74" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U73" s="29"/>
+    </row>
+    <row r="74" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A74" s="16" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="B74" s="16"/>
-      <c r="C74" s="29" t="s">
-        <v>455</v>
+      <c r="C74" s="35" t="s">
+        <v>450</v>
       </c>
       <c r="D74" s="16" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="E74" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F74" s="16" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="G74" s="16" t="s">
         <v>20</v>
@@ -6224,7 +6259,7 @@
         <v>110</v>
       </c>
       <c r="O74" s="16" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="P74" s="24">
         <v>43788</v>
@@ -6239,24 +6274,24 @@
         <v>310</v>
       </c>
       <c r="T74" s="17"/>
-      <c r="U74" s="30"/>
-    </row>
-    <row r="75" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U74" s="29"/>
+    </row>
+    <row r="75" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A75" s="16" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="B75" s="16"/>
-      <c r="C75" s="29" t="s">
-        <v>460</v>
+      <c r="C75" s="35" t="s">
+        <v>455</v>
       </c>
       <c r="D75" s="16" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="E75" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F75" s="16" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="G75" s="16" t="s">
         <v>20</v>
@@ -6283,7 +6318,7 @@
         <v>110</v>
       </c>
       <c r="O75" s="16" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="P75" s="24">
         <v>43788</v>
@@ -6298,24 +6333,24 @@
         <v>310</v>
       </c>
       <c r="T75" s="17"/>
-      <c r="U75" s="30"/>
-    </row>
-    <row r="76" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U75" s="29"/>
+    </row>
+    <row r="76" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A76" s="16" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="B76" s="16"/>
-      <c r="C76" s="29" t="s">
-        <v>465</v>
+      <c r="C76" s="35" t="s">
+        <v>460</v>
       </c>
       <c r="D76" s="16" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="E76" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F76" s="16" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="G76" s="16" t="s">
         <v>20</v>
@@ -6342,7 +6377,7 @@
         <v>110</v>
       </c>
       <c r="O76" s="16" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="P76" s="24">
         <v>43788</v>
@@ -6357,81 +6392,84 @@
         <v>310</v>
       </c>
       <c r="T76" s="17"/>
-      <c r="U76" s="30"/>
-    </row>
-    <row r="77" spans="1:21" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="32" t="s">
+      <c r="U76" s="29"/>
+    </row>
+    <row r="77" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+      <c r="A77" s="16" t="s">
+        <v>464</v>
+      </c>
+      <c r="B77" s="16"/>
+      <c r="C77" s="35" t="s">
+        <v>465</v>
+      </c>
+      <c r="D77" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="E77" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="F77" s="16" t="s">
+        <v>467</v>
+      </c>
+      <c r="G77" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H77" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="I77" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="J77" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="K77" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="L77" s="16" t="s">
+        <v>407</v>
+      </c>
+      <c r="M77" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="N77" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="O77" s="16" t="s">
+        <v>468</v>
+      </c>
+      <c r="P77" s="24">
+        <v>43788</v>
+      </c>
+      <c r="Q77" s="16" t="s">
+        <v>382</v>
+      </c>
+      <c r="R77" s="16" t="s">
+        <v>310</v>
+      </c>
+      <c r="S77" s="16" t="s">
+        <v>310</v>
+      </c>
+      <c r="T77" s="17"/>
+      <c r="U77" s="29"/>
+    </row>
+    <row r="78" spans="1:21" s="31" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A78" s="30" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="78" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="16" t="s">
+    <row r="79" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B78" s="16" t="s">
+      <c r="B79" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="C78" s="16" t="s">
+      <c r="C79" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="D78" s="16" t="s">
+      <c r="D79" s="16" t="s">
         <v>60</v>
-      </c>
-      <c r="E78" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F78" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="G78" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="H78" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="I78" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="J78" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="K78" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="L78" s="16" t="s">
-        <v>249</v>
-      </c>
-      <c r="M78" s="16" t="s">
-        <v>256</v>
-      </c>
-      <c r="N78" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="O78" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="P78" s="24">
-        <v>42507</v>
-      </c>
-      <c r="Q78" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="R78" s="16"/>
-      <c r="S78" s="16"/>
-      <c r="T78" s="17"/>
-    </row>
-    <row r="79" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B79" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C79" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="D79" s="16" t="s">
-        <v>4</v>
       </c>
       <c r="E79" s="16" t="s">
         <v>25</v>
@@ -6446,48 +6484,48 @@
         <v>12</v>
       </c>
       <c r="I79" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J79" s="16" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="K79" s="16" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L79" s="16" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="M79" s="16" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="N79" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O79" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P79" s="24">
-        <v>41002</v>
+        <v>42507</v>
       </c>
       <c r="Q79" s="16" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="R79" s="16"/>
       <c r="S79" s="16"/>
       <c r="T79" s="17"/>
     </row>
-    <row r="80" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A80" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B80" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C80" s="16" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D80" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E80" s="16" t="s">
         <v>25</v>
@@ -6502,25 +6540,25 @@
         <v>12</v>
       </c>
       <c r="I80" s="16" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="J80" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K80" s="16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L80" s="16" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="M80" s="16" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="N80" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O80" s="16" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P80" s="24">
         <v>41002</v>
@@ -6532,18 +6570,18 @@
       <c r="S80" s="16"/>
       <c r="T80" s="17"/>
     </row>
-    <row r="81" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A81" s="16" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B81" s="16" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C81" s="16" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D81" s="16" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E81" s="16" t="s">
         <v>25</v>
@@ -6558,25 +6596,25 @@
         <v>12</v>
       </c>
       <c r="I81" s="16" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="J81" s="16" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="K81" s="16" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="L81" s="16" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="M81" s="16" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="N81" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O81" s="16" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="P81" s="24">
         <v>41002</v>
@@ -6588,40 +6626,72 @@
       <c r="S81" s="16"/>
       <c r="T81" s="17"/>
     </row>
-    <row r="82" spans="1:20" s="34" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="32" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="83" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="12" t="s">
+    <row r="82" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A82" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B82" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C82" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D82" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E82" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F82" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="G82" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H82" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I82" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="J82" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="K82" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="L82" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="M82" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="N82" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="O82" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="P82" s="24">
+        <v>41002</v>
+      </c>
+      <c r="Q82" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="R82" s="16"/>
+      <c r="S82" s="16"/>
+      <c r="T82" s="17"/>
+    </row>
+    <row r="83" spans="1:20" s="32" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A83" s="30" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A84" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="B83" s="3"/>
-      <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
-      <c r="E83" s="3"/>
-      <c r="F83" s="3"/>
-      <c r="G83" s="3"/>
-      <c r="I83" s="12"/>
-      <c r="J83" s="3"/>
-      <c r="K83" s="3"/>
-      <c r="L83" s="3"/>
-      <c r="M83" s="3"/>
-      <c r="N83" s="3"/>
-      <c r="O83" s="3"/>
-      <c r="P83" s="26"/>
-      <c r="Q83" s="3"/>
-      <c r="R83" s="3"/>
-      <c r="S83" s="3"/>
-      <c r="T83" s="3"/>
-    </row>
-    <row r="84" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="12" t="s">
-        <v>185</v>
-      </c>
       <c r="B84" s="3"/>
-      <c r="C84" s="3"/>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
@@ -6639,17 +6709,16 @@
       <c r="S84" s="3"/>
       <c r="T84" s="3"/>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A85" s="13" t="s">
-        <v>186</v>
+    <row r="85" spans="1:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A85" s="12" t="s">
+        <v>185</v>
       </c>
       <c r="B85" s="3"/>
-      <c r="C85" s="3"/>
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
-      <c r="I85" s="13"/>
+      <c r="I85" s="12"/>
       <c r="J85" s="3"/>
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
@@ -6662,12 +6731,11 @@
       <c r="S85" s="3"/>
       <c r="T85" s="3"/>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A86" s="13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B86" s="3"/>
-      <c r="C86" s="3"/>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
@@ -6685,24 +6753,47 @@
       <c r="S86" s="3"/>
       <c r="T86" s="3"/>
     </row>
-    <row r="87" spans="1:20" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A87" s="21" t="s">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A87" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="B87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
+      <c r="G87" s="3"/>
+      <c r="I87" s="13"/>
+      <c r="J87" s="3"/>
+      <c r="K87" s="3"/>
+      <c r="L87" s="3"/>
+      <c r="M87" s="3"/>
+      <c r="N87" s="3"/>
+      <c r="O87" s="3"/>
+      <c r="P87" s="26"/>
+      <c r="Q87" s="3"/>
+      <c r="R87" s="3"/>
+      <c r="S87" s="3"/>
+      <c r="T87" s="3"/>
+    </row>
+    <row r="88" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A88" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="P87" s="27"/>
-    </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A88" s="22" t="s">
+      <c r="C88" s="12"/>
+      <c r="P88" s="27"/>
+    </row>
+    <row r="89" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A89" s="22" t="s">
         <v>225</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A34:O37">
-    <sortCondition ref="A34:A37"/>
+  <sortState ref="A35:O38">
+    <sortCondition ref="A35:A38"/>
   </sortState>
   <mergeCells count="6">
-    <mergeCell ref="A77:XFD77"/>
-    <mergeCell ref="A82:XFD82"/>
+    <mergeCell ref="A78:XFD78"/>
+    <mergeCell ref="A83:XFD83"/>
     <mergeCell ref="A2:XFD2"/>
     <mergeCell ref="A4:XFD4"/>
     <mergeCell ref="A10:XFD10"/>
@@ -6725,14 +6816,14 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="141.5703125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="11.84375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="12.3828125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="141.53515625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
@@ -6743,7 +6834,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="6">
         <v>42080</v>
       </c>
@@ -6754,7 +6845,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="6">
         <v>42119</v>
       </c>
@@ -6765,7 +6856,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="6">
         <v>42131</v>
       </c>
@@ -6776,7 +6867,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="6">
         <v>42158</v>
       </c>
@@ -6787,7 +6878,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="6">
         <v>42248</v>
       </c>
@@ -6798,7 +6889,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="6">
         <v>42249</v>
       </c>
@@ -6809,7 +6900,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" s="6">
         <v>42507</v>
       </c>
@@ -6820,7 +6911,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" s="6">
         <v>42582</v>
       </c>
@@ -6831,7 +6922,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" s="6">
         <v>42724</v>
       </c>
@@ -6842,74 +6933,74 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11" s="33">
         <v>42835</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="32" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
-      <c r="B12" s="34"/>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A12" s="33"/>
+      <c r="B12" s="32"/>
       <c r="C12" s="7" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
-      <c r="B13" s="34"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A13" s="33"/>
+      <c r="B13" s="32"/>
       <c r="C13" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="34"/>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A14" s="33"/>
+      <c r="B14" s="32"/>
       <c r="C14" s="7" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
-      <c r="B15" s="34"/>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A15" s="33"/>
+      <c r="B15" s="32"/>
       <c r="C15" s="7" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
-      <c r="B16" s="34"/>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A16" s="33"/>
+      <c r="B16" s="32"/>
       <c r="C16" s="7" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
-      <c r="B17" s="34"/>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A17" s="33"/>
+      <c r="B17" s="32"/>
       <c r="C17" s="7" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
-      <c r="B18" s="34"/>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A18" s="33"/>
+      <c r="B18" s="32"/>
       <c r="C18" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
-      <c r="B19" s="34"/>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A19" s="33"/>
+      <c r="B19" s="32"/>
       <c r="C19" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" s="8">
         <v>42839</v>
       </c>
@@ -6920,7 +7011,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" s="8">
         <v>42839</v>
       </c>
@@ -6931,7 +7022,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" s="10">
         <v>42858</v>
       </c>
@@ -6942,7 +7033,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23" s="10">
         <v>42858</v>
       </c>
@@ -6953,7 +7044,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24" s="6">
         <v>42928</v>
       </c>
@@ -6964,7 +7055,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25" s="6">
         <v>42969</v>
       </c>
@@ -6975,7 +7066,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26" s="14">
         <v>42969</v>
       </c>
@@ -6986,7 +7077,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27" s="6">
         <v>43718</v>
       </c>
@@ -6997,7 +7088,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A28" s="6">
         <v>43804</v>
       </c>

</xml_diff>

<commit_message>
Issue #267: Namespace Updates - ID Requested: HYB2 - Hayabusa2 (#279)
Update namespace registry with HYB2 - Hayabusa2.

This dictionary contains classes and attributes specific to the Hayabusa2 mission and instruments. It has been created to support the Hayabusa 2 data archive.

Resolves #267
</commit_message>
<xml_diff>
--- a/model-ontology/src/ontology/Data/pds-namespace-registry.xlsx
+++ b/model-ontology/src/ontology/Data/pds-namespace-registry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20367"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\AAAPDS4\AADataModel\0000_Design\Namespaces_1002\NameSpaceRegistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{87C73744-6FB4-4083-AE18-606C56810CB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D43093-C62B-4F56-BE56-154ED8752095}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1155" yWindow="1065" windowWidth="26655" windowHeight="12855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1157" yWindow="1063" windowWidth="26657" windowHeight="12857" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Namespaces" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Namespaces!$A$11:$Q$29</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1325" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1343" uniqueCount="519">
   <si>
     <t>Registration Date</t>
   </si>
@@ -1559,6 +1559,36 @@
   </si>
   <si>
     <t>https://voparis-ns.obspm.fr/pds4/epn/v1</t>
+  </si>
+  <si>
+    <t>hyb2</t>
+  </si>
+  <si>
+    <t>mission/hyb2</t>
+  </si>
+  <si>
+    <t>Carol Neese</t>
+  </si>
+  <si>
+    <t>nees at psi.edu</t>
+  </si>
+  <si>
+    <t>This is the Hayabusa2 Mission Specific Data Dictionary.</t>
+  </si>
+  <si>
+    <t>C. Neese</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hayabusa2 </t>
+  </si>
+  <si>
+    <t>PDS4_HYB2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://pds.nasa.gov/pds4/mission/hyb2/v1 </t>
+  </si>
+  <si>
+    <t>sbnpsi</t>
   </si>
 </sst>
 </file>
@@ -1725,7 +1755,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1811,14 +1841,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1832,6 +1856,16 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2145,39 +2179,39 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U88"/>
+  <dimension ref="A1:U89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="15.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="22" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="22" customWidth="1"/>
-    <col min="3" max="3" width="46.140625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="22" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="22" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" style="22" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="22" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" style="22" customWidth="1"/>
-    <col min="9" max="9" width="25.28515625" style="22" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" style="22" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" style="22" customWidth="1"/>
+    <col min="1" max="1" width="14.3828125" style="22" customWidth="1"/>
+    <col min="2" max="2" width="16.69140625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="46.15234375" style="12" customWidth="1"/>
+    <col min="4" max="4" width="13.3828125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="14.3828125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="22.84375" style="22" customWidth="1"/>
+    <col min="7" max="7" width="12.3828125" style="22" customWidth="1"/>
+    <col min="8" max="8" width="21.3828125" style="22" customWidth="1"/>
+    <col min="9" max="9" width="25.3046875" style="22" customWidth="1"/>
+    <col min="10" max="10" width="13.15234375" style="22" customWidth="1"/>
+    <col min="11" max="11" width="18.765625" style="22" customWidth="1"/>
     <col min="12" max="12" width="23" style="22" customWidth="1"/>
-    <col min="13" max="13" width="38.7109375" style="22" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" style="22" customWidth="1"/>
-    <col min="15" max="15" width="53.85546875" style="22" customWidth="1"/>
-    <col min="16" max="16" width="16.140625" style="27" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" style="22" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" style="22" customWidth="1"/>
-    <col min="19" max="19" width="11.140625" style="22" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" style="22" customWidth="1"/>
-    <col min="21" max="16384" width="8.85546875" style="22"/>
+    <col min="13" max="13" width="38.69140625" style="22" customWidth="1"/>
+    <col min="14" max="14" width="10.15234375" style="22" customWidth="1"/>
+    <col min="15" max="15" width="53.84375" style="22" customWidth="1"/>
+    <col min="16" max="16" width="16.15234375" style="27" customWidth="1"/>
+    <col min="17" max="17" width="14.15234375" style="22" customWidth="1"/>
+    <col min="18" max="18" width="11.3828125" style="22" customWidth="1"/>
+    <col min="19" max="19" width="11.15234375" style="22" customWidth="1"/>
+    <col min="20" max="20" width="13.69140625" style="22" customWidth="1"/>
+    <col min="21" max="16384" width="8.84375" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="47.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>179</v>
       </c>
@@ -2239,12 +2273,12 @@
         <v>302</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="33" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+    <row r="2" spans="1:20" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="30" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="16" t="s">
         <v>2</v>
       </c>
@@ -2304,12 +2338,12 @@
       </c>
       <c r="T3" s="17"/>
     </row>
-    <row r="4" spans="1:20" s="33" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+    <row r="4" spans="1:20" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="30" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A5" s="16" t="s">
         <v>102</v>
       </c>
@@ -2369,7 +2403,7 @@
       </c>
       <c r="T5" s="17"/>
     </row>
-    <row r="6" spans="1:20" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A6" s="16" t="s">
         <v>189</v>
       </c>
@@ -2429,7 +2463,7 @@
       </c>
       <c r="T6" s="17"/>
     </row>
-    <row r="7" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="16" t="s">
         <v>26</v>
       </c>
@@ -2491,7 +2525,7 @@
         <v>42277</v>
       </c>
     </row>
-    <row r="8" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="16" t="s">
         <v>101</v>
       </c>
@@ -2551,14 +2585,14 @@
       </c>
       <c r="T8" s="17"/>
     </row>
-    <row r="9" spans="1:20" s="28" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" s="28" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A9" s="19" t="s">
         <v>499</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>499</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="36" t="s">
         <v>508</v>
       </c>
       <c r="D9" s="19" t="s">
@@ -2611,12 +2645,12 @@
       </c>
       <c r="T9" s="20"/>
     </row>
-    <row r="10" spans="1:20" s="33" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+    <row r="10" spans="1:20" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="30" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:20" s="28" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" s="28" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A11" s="19" t="s">
         <v>36</v>
       </c>
@@ -2676,7 +2710,7 @@
       </c>
       <c r="T11" s="17"/>
     </row>
-    <row r="12" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A12" s="16" t="s">
         <v>3</v>
       </c>
@@ -2736,7 +2770,7 @@
       </c>
       <c r="T12" s="17"/>
     </row>
-    <row r="13" spans="1:20" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A13" s="16" t="s">
         <v>63</v>
       </c>
@@ -2796,7 +2830,7 @@
       </c>
       <c r="T13" s="17"/>
     </row>
-    <row r="14" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="16" t="s">
         <v>14</v>
       </c>
@@ -2856,7 +2890,7 @@
       </c>
       <c r="T14" s="17"/>
     </row>
-    <row r="15" spans="1:20" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A15" s="16" t="s">
         <v>41</v>
       </c>
@@ -2916,7 +2950,7 @@
       </c>
       <c r="T15" s="17"/>
     </row>
-    <row r="16" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A16" s="16" t="s">
         <v>5</v>
       </c>
@@ -2976,7 +3010,7 @@
       </c>
       <c r="T16" s="17"/>
     </row>
-    <row r="17" spans="1:20" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A17" s="16" t="s">
         <v>276</v>
       </c>
@@ -3036,7 +3070,7 @@
       </c>
       <c r="T17" s="17"/>
     </row>
-    <row r="18" spans="1:20" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A18" s="16" t="s">
         <v>277</v>
       </c>
@@ -3096,14 +3130,14 @@
       </c>
       <c r="T18" s="17"/>
     </row>
-    <row r="19" spans="1:20" s="28" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" s="28" customFormat="1" ht="47.6" x14ac:dyDescent="0.4">
       <c r="A19" s="19" t="s">
         <v>488</v>
       </c>
       <c r="B19" s="19" t="s">
         <v>488</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="34" t="s">
         <v>489</v>
       </c>
       <c r="D19" s="19" t="s">
@@ -3156,7 +3190,7 @@
       </c>
       <c r="T19" s="20"/>
     </row>
-    <row r="20" spans="1:20" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A20" s="16" t="s">
         <v>18</v>
       </c>
@@ -3216,7 +3250,7 @@
       </c>
       <c r="T20" s="17"/>
     </row>
-    <row r="21" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A21" s="16" t="s">
         <v>2</v>
       </c>
@@ -3276,7 +3310,7 @@
       </c>
       <c r="T21" s="17"/>
     </row>
-    <row r="22" spans="1:20" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A22" s="16" t="s">
         <v>8</v>
       </c>
@@ -3336,7 +3370,7 @@
       </c>
       <c r="T22" s="17"/>
     </row>
-    <row r="23" spans="1:20" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A23" s="16" t="s">
         <v>285</v>
       </c>
@@ -3396,7 +3430,7 @@
       </c>
       <c r="T23" s="17"/>
     </row>
-    <row r="24" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A24" s="16" t="s">
         <v>9</v>
       </c>
@@ -3456,7 +3490,7 @@
       </c>
       <c r="T24" s="17"/>
     </row>
-    <row r="25" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A25" s="16" t="s">
         <v>11</v>
       </c>
@@ -3514,7 +3548,7 @@
       </c>
       <c r="T25" s="17"/>
     </row>
-    <row r="26" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A26" s="16" t="s">
         <v>39</v>
       </c>
@@ -3574,7 +3608,7 @@
       </c>
       <c r="T26" s="17"/>
     </row>
-    <row r="27" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="16" t="s">
         <v>226</v>
       </c>
@@ -3634,14 +3668,14 @@
       </c>
       <c r="T27" s="17"/>
     </row>
-    <row r="28" spans="1:20" s="28" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" s="28" customFormat="1" ht="47.6" x14ac:dyDescent="0.4">
       <c r="A28" s="19" t="s">
         <v>480</v>
       </c>
       <c r="B28" s="19" t="s">
         <v>480</v>
       </c>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="34" t="s">
         <v>481</v>
       </c>
       <c r="D28" s="19" t="s">
@@ -3694,7 +3728,7 @@
       </c>
       <c r="T28" s="20"/>
     </row>
-    <row r="29" spans="1:20" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A29" s="16" t="s">
         <v>19</v>
       </c>
@@ -3754,12 +3788,12 @@
       </c>
       <c r="T29" s="17"/>
     </row>
-    <row r="30" spans="1:20" s="33" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="32" t="s">
+    <row r="30" spans="1:20" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="30" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A31" s="16" t="s">
         <v>67</v>
       </c>
@@ -3819,84 +3853,84 @@
       </c>
       <c r="T31" s="17"/>
     </row>
-    <row r="32" spans="1:20" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="16" t="s">
+    <row r="32" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="19" t="s">
+        <v>509</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>510</v>
+      </c>
+      <c r="C32" s="37" t="s">
+        <v>517</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>509</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>516</v>
+      </c>
+      <c r="G32" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H32" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I32" s="19" t="s">
+        <v>515</v>
+      </c>
+      <c r="J32" s="19" t="s">
+        <v>518</v>
+      </c>
+      <c r="K32" s="19" t="s">
+        <v>484</v>
+      </c>
+      <c r="L32" s="19" t="s">
+        <v>511</v>
+      </c>
+      <c r="M32" s="19" t="s">
+        <v>512</v>
+      </c>
+      <c r="N32" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="O32" s="19" t="s">
+        <v>513</v>
+      </c>
+      <c r="P32" s="25">
+        <v>44193</v>
+      </c>
+      <c r="Q32" s="19" t="s">
+        <v>514</v>
+      </c>
+      <c r="R32" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="S32" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="T32" s="20"/>
+    </row>
+    <row r="33" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B33" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C33" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D33" s="16" t="s">
         <v>68</v>
-      </c>
-      <c r="E32" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F32" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="G32" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="H32" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="I32" s="16" t="s">
-        <v>209</v>
-      </c>
-      <c r="J32" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K32" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="L32" s="16" t="s">
-        <v>248</v>
-      </c>
-      <c r="M32" s="16" t="s">
-        <v>262</v>
-      </c>
-      <c r="N32" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="O32" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="P32" s="24">
-        <v>42119</v>
-      </c>
-      <c r="Q32" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="R32" s="16" t="s">
-        <v>304</v>
-      </c>
-      <c r="S32" s="16" t="s">
-        <v>304</v>
-      </c>
-      <c r="T32" s="17"/>
-    </row>
-    <row r="33" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>55</v>
       </c>
       <c r="E33" s="16" t="s">
         <v>25</v>
       </c>
       <c r="F33" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G33" s="16" t="s">
         <v>20</v>
@@ -3905,31 +3939,31 @@
         <v>12</v>
       </c>
       <c r="I33" s="16" t="s">
-        <v>119</v>
+        <v>209</v>
       </c>
       <c r="J33" s="16" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K33" s="16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="L33" s="16" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="M33" s="16" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="N33" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O33" s="16" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="P33" s="24">
-        <v>41837</v>
+        <v>42119</v>
       </c>
       <c r="Q33" s="16" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="R33" s="16" t="s">
         <v>304</v>
@@ -3939,15 +3973,15 @@
       </c>
       <c r="T33" s="17"/>
     </row>
-    <row r="34" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A34" s="16" t="s">
         <v>55</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="D34" s="16" t="s">
         <v>55</v>
@@ -3983,7 +4017,7 @@
         <v>110</v>
       </c>
       <c r="O34" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P34" s="24">
         <v>41837</v>
@@ -3999,24 +4033,24 @@
       </c>
       <c r="T34" s="17"/>
     </row>
-    <row r="35" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A35" s="16" t="s">
-        <v>474</v>
+        <v>55</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>475</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>476</v>
+        <v>55</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>78</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>474</v>
+        <v>55</v>
       </c>
       <c r="E35" s="16" t="s">
         <v>25</v>
       </c>
       <c r="F35" s="16" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="G35" s="16" t="s">
         <v>20</v>
@@ -4025,31 +4059,31 @@
         <v>12</v>
       </c>
       <c r="I35" s="16" t="s">
-        <v>477</v>
+        <v>119</v>
       </c>
       <c r="J35" s="16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K35" s="16" t="s">
-        <v>478</v>
+        <v>126</v>
       </c>
       <c r="L35" s="16" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="M35" s="16" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="N35" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O35" s="16" t="s">
-        <v>479</v>
+        <v>153</v>
       </c>
       <c r="P35" s="24">
-        <v>43935</v>
+        <v>41837</v>
       </c>
       <c r="Q35" s="16" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="R35" s="16" t="s">
         <v>304</v>
@@ -4059,18 +4093,18 @@
       </c>
       <c r="T35" s="17"/>
     </row>
-    <row r="36" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A36" s="16" t="s">
-        <v>34</v>
+        <v>474</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>91</v>
+        <v>475</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>476</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>34</v>
+        <v>474</v>
       </c>
       <c r="E36" s="16" t="s">
         <v>25</v>
@@ -4085,31 +4119,31 @@
         <v>12</v>
       </c>
       <c r="I36" s="16" t="s">
-        <v>210</v>
+        <v>477</v>
       </c>
       <c r="J36" s="16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K36" s="16" t="s">
-        <v>128</v>
+        <v>478</v>
       </c>
       <c r="L36" s="16" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="M36" s="16" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="N36" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O36" s="16" t="s">
-        <v>155</v>
+        <v>479</v>
       </c>
       <c r="P36" s="24">
-        <v>41600</v>
+        <v>43935</v>
       </c>
       <c r="Q36" s="16" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="R36" s="16" t="s">
         <v>304</v>
@@ -4119,18 +4153,18 @@
       </c>
       <c r="T36" s="17"/>
     </row>
-    <row r="37" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A37" s="16" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="E37" s="16" t="s">
         <v>25</v>
@@ -4145,7 +4179,7 @@
         <v>12</v>
       </c>
       <c r="I37" s="16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J37" s="16" t="s">
         <v>5</v>
@@ -4163,13 +4197,13 @@
         <v>110</v>
       </c>
       <c r="O37" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P37" s="24">
-        <v>42220</v>
+        <v>41600</v>
       </c>
       <c r="Q37" s="16" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="R37" s="16" t="s">
         <v>304</v>
@@ -4179,24 +4213,24 @@
       </c>
       <c r="T37" s="17"/>
     </row>
-    <row r="38" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A38" s="16" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E38" s="16" t="s">
         <v>25</v>
       </c>
       <c r="F38" s="16" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="G38" s="16" t="s">
         <v>20</v>
@@ -4205,31 +4239,31 @@
         <v>12</v>
       </c>
       <c r="I38" s="16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J38" s="16" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K38" s="16" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="L38" s="16" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="M38" s="16" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="N38" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O38" s="16" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="P38" s="24">
-        <v>42158</v>
+        <v>42220</v>
       </c>
       <c r="Q38" s="16" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="R38" s="16" t="s">
         <v>304</v>
@@ -4239,15 +4273,15 @@
       </c>
       <c r="T38" s="17"/>
     </row>
-    <row r="39" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A39" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="D39" s="16" t="s">
         <v>43</v>
@@ -4283,7 +4317,7 @@
         <v>110</v>
       </c>
       <c r="O39" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="P39" s="24">
         <v>42158</v>
@@ -4299,24 +4333,24 @@
       </c>
       <c r="T39" s="17"/>
     </row>
-    <row r="40" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A40" s="16" t="s">
-        <v>234</v>
+        <v>43</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>235</v>
+        <v>43</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>236</v>
+        <v>79</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>234</v>
+        <v>43</v>
       </c>
       <c r="E40" s="16" t="s">
         <v>25</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>237</v>
+        <v>120</v>
       </c>
       <c r="G40" s="16" t="s">
         <v>20</v>
@@ -4325,31 +4359,31 @@
         <v>12</v>
       </c>
       <c r="I40" s="16" t="s">
-        <v>238</v>
+        <v>213</v>
       </c>
       <c r="J40" s="16" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K40" s="16" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="L40" s="16" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="M40" s="16" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="N40" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O40" s="16" t="s">
-        <v>239</v>
+        <v>159</v>
       </c>
       <c r="P40" s="24">
-        <v>42650</v>
+        <v>42158</v>
       </c>
       <c r="Q40" s="16" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="R40" s="16" t="s">
         <v>304</v>
@@ -4359,24 +4393,24 @@
       </c>
       <c r="T40" s="17"/>
     </row>
-    <row r="41" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A41" s="16" t="s">
-        <v>35</v>
+        <v>234</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>50</v>
+        <v>235</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>94</v>
+        <v>236</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>35</v>
+        <v>234</v>
       </c>
       <c r="E41" s="16" t="s">
         <v>25</v>
       </c>
       <c r="F41" s="16" t="s">
-        <v>110</v>
+        <v>237</v>
       </c>
       <c r="G41" s="16" t="s">
         <v>20</v>
@@ -4385,31 +4419,31 @@
         <v>12</v>
       </c>
       <c r="I41" s="16" t="s">
-        <v>212</v>
+        <v>238</v>
       </c>
       <c r="J41" s="16" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="K41" s="16" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="L41" s="16" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="M41" s="16" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="N41" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O41" s="16" t="s">
-        <v>157</v>
+        <v>239</v>
       </c>
       <c r="P41" s="24">
-        <v>41771</v>
+        <v>42650</v>
       </c>
       <c r="Q41" s="16" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="R41" s="16" t="s">
         <v>304</v>
@@ -4419,83 +4453,84 @@
       </c>
       <c r="T41" s="17"/>
     </row>
-    <row r="42" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A42" s="16" t="s">
-        <v>305</v>
+        <v>35</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>305</v>
-      </c>
-      <c r="C42" s="29" t="s">
-        <v>306</v>
+        <v>50</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>94</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>305</v>
+        <v>35</v>
       </c>
       <c r="E42" s="16" t="s">
-        <v>303</v>
+        <v>25</v>
       </c>
       <c r="F42" s="16" t="s">
-        <v>307</v>
+        <v>110</v>
       </c>
       <c r="G42" s="16" t="s">
         <v>20</v>
       </c>
       <c r="H42" s="16" t="s">
-        <v>175</v>
+        <v>12</v>
       </c>
       <c r="I42" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="J42" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="K42" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="L42" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="M42" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="N42" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="O42" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="P42" s="24">
+        <v>41771</v>
+      </c>
+      <c r="Q42" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="R42" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="S42" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="T42" s="17"/>
+    </row>
+    <row r="43" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+      <c r="A43" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="J42" s="16" t="s">
+      <c r="B43" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="K42" s="16" t="s">
+      <c r="C43" s="35" t="s">
+        <v>306</v>
+      </c>
+      <c r="D43" s="16" t="s">
         <v>305</v>
-      </c>
-      <c r="L42" s="16" t="s">
-        <v>308</v>
-      </c>
-      <c r="M42" s="16" t="s">
-        <v>472</v>
-      </c>
-      <c r="N42" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="O42" s="16" t="s">
-        <v>309</v>
-      </c>
-      <c r="P42" s="24">
-        <v>43788</v>
-      </c>
-      <c r="Q42" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="R42" s="16" t="s">
-        <v>304</v>
-      </c>
-      <c r="S42" s="16" t="s">
-        <v>310</v>
-      </c>
-      <c r="T42" s="17"/>
-      <c r="U42" s="30"/>
-    </row>
-    <row r="43" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="B43" s="16"/>
-      <c r="C43" s="29" t="s">
-        <v>312</v>
-      </c>
-      <c r="D43" s="16" t="s">
-        <v>313</v>
       </c>
       <c r="E43" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F43" s="16" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="G43" s="16" t="s">
         <v>20</v>
@@ -4516,45 +4551,45 @@
         <v>308</v>
       </c>
       <c r="M43" s="16" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="N43" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O43" s="16" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="P43" s="24">
         <v>43788</v>
       </c>
       <c r="Q43" s="16" t="s">
-        <v>316</v>
+        <v>27</v>
       </c>
       <c r="R43" s="16" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="S43" s="16" t="s">
         <v>310</v>
       </c>
       <c r="T43" s="17"/>
-      <c r="U43" s="30"/>
-    </row>
-    <row r="44" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U43" s="29"/>
+    </row>
+    <row r="44" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A44" s="16" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="B44" s="16"/>
-      <c r="C44" s="29" t="s">
-        <v>318</v>
+      <c r="C44" s="35" t="s">
+        <v>312</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="E44" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F44" s="16" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="G44" s="16" t="s">
         <v>20</v>
@@ -4562,9 +4597,15 @@
       <c r="H44" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="I44" s="16"/>
-      <c r="J44" s="16"/>
-      <c r="K44" s="16"/>
+      <c r="I44" s="16" t="s">
+        <v>305</v>
+      </c>
+      <c r="J44" s="16" t="s">
+        <v>305</v>
+      </c>
+      <c r="K44" s="16" t="s">
+        <v>305</v>
+      </c>
       <c r="L44" s="16" t="s">
         <v>308</v>
       </c>
@@ -4575,7 +4616,7 @@
         <v>110</v>
       </c>
       <c r="O44" s="16" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="P44" s="24">
         <v>43788</v>
@@ -4584,30 +4625,30 @@
         <v>316</v>
       </c>
       <c r="R44" s="16" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="S44" s="16" t="s">
         <v>310</v>
       </c>
       <c r="T44" s="17"/>
-      <c r="U44" s="30"/>
-    </row>
-    <row r="45" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U44" s="29"/>
+    </row>
+    <row r="45" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A45" s="16" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B45" s="16"/>
-      <c r="C45" s="29" t="s">
-        <v>323</v>
+      <c r="C45" s="35" t="s">
+        <v>318</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="E45" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F45" s="16" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="G45" s="16" t="s">
         <v>20</v>
@@ -4628,7 +4669,7 @@
         <v>110</v>
       </c>
       <c r="O45" s="16" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="P45" s="24">
         <v>43788</v>
@@ -4637,30 +4678,30 @@
         <v>316</v>
       </c>
       <c r="R45" s="16" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="S45" s="16" t="s">
         <v>310</v>
       </c>
       <c r="T45" s="17"/>
-      <c r="U45" s="30"/>
-    </row>
-    <row r="46" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U45" s="29"/>
+    </row>
+    <row r="46" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A46" s="16" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="B46" s="16"/>
-      <c r="C46" s="29" t="s">
-        <v>328</v>
+      <c r="C46" s="35" t="s">
+        <v>323</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="E46" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F46" s="16" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="G46" s="16" t="s">
         <v>20</v>
@@ -4681,7 +4722,7 @@
         <v>110</v>
       </c>
       <c r="O46" s="16" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="P46" s="24">
         <v>43788</v>
@@ -4696,24 +4737,24 @@
         <v>310</v>
       </c>
       <c r="T46" s="17"/>
-      <c r="U46" s="30"/>
-    </row>
-    <row r="47" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U46" s="29"/>
+    </row>
+    <row r="47" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A47" s="16" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="B47" s="16"/>
-      <c r="C47" s="29" t="s">
-        <v>333</v>
+      <c r="C47" s="35" t="s">
+        <v>328</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="E47" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F47" s="16" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="G47" s="16" t="s">
         <v>20</v>
@@ -4734,7 +4775,7 @@
         <v>110</v>
       </c>
       <c r="O47" s="16" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="P47" s="24">
         <v>43788</v>
@@ -4749,24 +4790,24 @@
         <v>310</v>
       </c>
       <c r="T47" s="17"/>
-      <c r="U47" s="30"/>
-    </row>
-    <row r="48" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U47" s="29"/>
+    </row>
+    <row r="48" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A48" s="16" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="B48" s="16"/>
-      <c r="C48" s="29" t="s">
-        <v>338</v>
+      <c r="C48" s="35" t="s">
+        <v>333</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="E48" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F48" s="16" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="G48" s="16" t="s">
         <v>20</v>
@@ -4787,7 +4828,7 @@
         <v>110</v>
       </c>
       <c r="O48" s="16" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="P48" s="24">
         <v>43788</v>
@@ -4802,24 +4843,24 @@
         <v>310</v>
       </c>
       <c r="T48" s="17"/>
-      <c r="U48" s="30"/>
-    </row>
-    <row r="49" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U48" s="29"/>
+    </row>
+    <row r="49" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A49" s="16" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="B49" s="16"/>
-      <c r="C49" s="29" t="s">
-        <v>343</v>
+      <c r="C49" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="E49" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F49" s="16" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G49" s="16" t="s">
         <v>20</v>
@@ -4840,7 +4881,7 @@
         <v>110</v>
       </c>
       <c r="O49" s="16" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="P49" s="24">
         <v>43788</v>
@@ -4855,24 +4896,24 @@
         <v>310</v>
       </c>
       <c r="T49" s="17"/>
-      <c r="U49" s="30"/>
-    </row>
-    <row r="50" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U49" s="29"/>
+    </row>
+    <row r="50" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A50" s="16" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="B50" s="16"/>
-      <c r="C50" s="29" t="s">
-        <v>348</v>
+      <c r="C50" s="35" t="s">
+        <v>343</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="E50" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F50" s="16" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="G50" s="16" t="s">
         <v>20</v>
@@ -4893,7 +4934,7 @@
         <v>110</v>
       </c>
       <c r="O50" s="16" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="P50" s="24">
         <v>43788</v>
@@ -4908,24 +4949,24 @@
         <v>310</v>
       </c>
       <c r="T50" s="17"/>
-      <c r="U50" s="30"/>
-    </row>
-    <row r="51" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U50" s="29"/>
+    </row>
+    <row r="51" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A51" s="16" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="B51" s="16"/>
-      <c r="C51" s="29" t="s">
-        <v>353</v>
+      <c r="C51" s="35" t="s">
+        <v>348</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="E51" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F51" s="16" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="G51" s="16" t="s">
         <v>20</v>
@@ -4946,7 +4987,7 @@
         <v>110</v>
       </c>
       <c r="O51" s="16" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="P51" s="24">
         <v>43788</v>
@@ -4961,24 +5002,24 @@
         <v>310</v>
       </c>
       <c r="T51" s="17"/>
-      <c r="U51" s="30"/>
-    </row>
-    <row r="52" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U51" s="29"/>
+    </row>
+    <row r="52" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A52" s="16" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="B52" s="16"/>
-      <c r="C52" s="29" t="s">
-        <v>358</v>
+      <c r="C52" s="35" t="s">
+        <v>353</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="E52" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F52" s="16" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="G52" s="16" t="s">
         <v>20</v>
@@ -4999,7 +5040,7 @@
         <v>110</v>
       </c>
       <c r="O52" s="16" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="P52" s="24">
         <v>43788</v>
@@ -5014,24 +5055,24 @@
         <v>310</v>
       </c>
       <c r="T52" s="17"/>
-      <c r="U52" s="30"/>
-    </row>
-    <row r="53" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U52" s="29"/>
+    </row>
+    <row r="53" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A53" s="16" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="B53" s="16"/>
-      <c r="C53" s="29" t="s">
-        <v>363</v>
+      <c r="C53" s="35" t="s">
+        <v>358</v>
       </c>
       <c r="D53" s="16" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="E53" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F53" s="16" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="G53" s="16" t="s">
         <v>20</v>
@@ -5052,7 +5093,7 @@
         <v>110</v>
       </c>
       <c r="O53" s="16" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="P53" s="24">
         <v>43788</v>
@@ -5067,24 +5108,24 @@
         <v>310</v>
       </c>
       <c r="T53" s="17"/>
-      <c r="U53" s="30"/>
-    </row>
-    <row r="54" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U53" s="29"/>
+    </row>
+    <row r="54" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A54" s="16" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="B54" s="16"/>
-      <c r="C54" s="29" t="s">
-        <v>368</v>
+      <c r="C54" s="35" t="s">
+        <v>363</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="E54" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F54" s="16" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="G54" s="16" t="s">
         <v>20</v>
@@ -5105,7 +5146,7 @@
         <v>110</v>
       </c>
       <c r="O54" s="16" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="P54" s="24">
         <v>43788</v>
@@ -5120,24 +5161,24 @@
         <v>310</v>
       </c>
       <c r="T54" s="17"/>
-      <c r="U54" s="30"/>
-    </row>
-    <row r="55" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U54" s="29"/>
+    </row>
+    <row r="55" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A55" s="16" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="B55" s="16"/>
-      <c r="C55" s="29" t="s">
-        <v>373</v>
+      <c r="C55" s="35" t="s">
+        <v>368</v>
       </c>
       <c r="D55" s="16" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="E55" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F55" s="16" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="G55" s="16" t="s">
         <v>20</v>
@@ -5158,7 +5199,7 @@
         <v>110</v>
       </c>
       <c r="O55" s="16" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="P55" s="24">
         <v>43788</v>
@@ -5173,174 +5214,168 @@
         <v>310</v>
       </c>
       <c r="T55" s="17"/>
-      <c r="U55" s="30"/>
-    </row>
-    <row r="56" spans="1:21" s="28" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A56" s="19" t="s">
+      <c r="U55" s="29"/>
+    </row>
+    <row r="56" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+      <c r="A56" s="16" t="s">
+        <v>372</v>
+      </c>
+      <c r="B56" s="16"/>
+      <c r="C56" s="35" t="s">
+        <v>373</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>374</v>
+      </c>
+      <c r="E56" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="F56" s="16" t="s">
+        <v>375</v>
+      </c>
+      <c r="G56" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H56" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="I56" s="16"/>
+      <c r="J56" s="16"/>
+      <c r="K56" s="16"/>
+      <c r="L56" s="16" t="s">
+        <v>308</v>
+      </c>
+      <c r="M56" s="16" t="s">
+        <v>471</v>
+      </c>
+      <c r="N56" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="O56" s="16" t="s">
+        <v>376</v>
+      </c>
+      <c r="P56" s="24">
+        <v>43788</v>
+      </c>
+      <c r="Q56" s="16" t="s">
+        <v>316</v>
+      </c>
+      <c r="R56" s="16" t="s">
+        <v>310</v>
+      </c>
+      <c r="S56" s="16" t="s">
+        <v>310</v>
+      </c>
+      <c r="T56" s="17"/>
+      <c r="U56" s="29"/>
+    </row>
+    <row r="57" spans="1:21" s="28" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+      <c r="A57" s="19" t="s">
         <v>492</v>
       </c>
-      <c r="B56" s="19" t="s">
+      <c r="B57" s="19" t="s">
         <v>493</v>
       </c>
-      <c r="C56" s="28" t="s">
+      <c r="C57" s="34" t="s">
         <v>494</v>
       </c>
-      <c r="D56" s="19" t="s">
+      <c r="D57" s="19" t="s">
         <v>492</v>
       </c>
-      <c r="E56" s="19" t="s">
+      <c r="E57" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F56" s="19" t="s">
+      <c r="F57" s="19" t="s">
         <v>498</v>
       </c>
-      <c r="G56" s="19" t="s">
+      <c r="G57" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H56" s="19" t="s">
+      <c r="H57" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="I56" s="19" t="s">
+      <c r="I57" s="19" t="s">
         <v>492</v>
       </c>
-      <c r="J56" s="19" t="s">
+      <c r="J57" s="19" t="s">
         <v>492</v>
       </c>
-      <c r="K56" s="19" t="s">
+      <c r="K57" s="19" t="s">
         <v>495</v>
       </c>
-      <c r="L56" s="19" t="s">
+      <c r="L57" s="19" t="s">
         <v>496</v>
       </c>
-      <c r="M56" s="19" t="s">
+      <c r="M57" s="19" t="s">
         <v>262</v>
       </c>
-      <c r="N56" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="O56" s="19" t="s">
+      <c r="N57" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="O57" s="19" t="s">
         <v>497</v>
       </c>
-      <c r="P56" s="25">
+      <c r="P57" s="25">
         <v>44111</v>
       </c>
-      <c r="Q56" s="19" t="s">
+      <c r="Q57" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="R56" s="19" t="s">
-        <v>304</v>
-      </c>
-      <c r="S56" s="19" t="s">
-        <v>304</v>
-      </c>
-      <c r="T56" s="20"/>
-    </row>
-    <row r="57" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="16"/>
-      <c r="B57" s="16"/>
-      <c r="C57" s="16"/>
-      <c r="D57" s="16"/>
-      <c r="E57" s="16"/>
-      <c r="F57" s="16"/>
-      <c r="G57" s="16"/>
-      <c r="H57" s="16"/>
-      <c r="I57" s="16"/>
-      <c r="J57" s="16"/>
-      <c r="K57" s="16"/>
-      <c r="L57" s="16"/>
-      <c r="M57" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="N57" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="O57" s="16"/>
-      <c r="P57" s="24">
-        <v>43788</v>
-      </c>
-      <c r="Q57" s="16"/>
-      <c r="R57" s="16"/>
-      <c r="S57" s="16"/>
-      <c r="T57" s="17"/>
-      <c r="U57" s="30"/>
-    </row>
-    <row r="58" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="B58" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="C58" s="29" t="s">
-        <v>378</v>
-      </c>
-      <c r="D58" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="E58" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="F58" s="16" t="s">
-        <v>379</v>
-      </c>
-      <c r="G58" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="H58" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="I58" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="J58" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="K58" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="L58" s="16" t="s">
-        <v>380</v>
-      </c>
+      <c r="R57" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="S57" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="T57" s="20"/>
+    </row>
+    <row r="58" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="16"/>
+      <c r="B58" s="16"/>
+      <c r="C58" s="16"/>
+      <c r="D58" s="16"/>
+      <c r="E58" s="16"/>
+      <c r="F58" s="16"/>
+      <c r="G58" s="16"/>
+      <c r="H58" s="16"/>
+      <c r="I58" s="16"/>
+      <c r="J58" s="16"/>
+      <c r="K58" s="16"/>
+      <c r="L58" s="16"/>
       <c r="M58" s="16" t="s">
-        <v>257</v>
+        <v>110</v>
       </c>
       <c r="N58" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="O58" s="16" t="s">
-        <v>381</v>
-      </c>
+      <c r="O58" s="16"/>
       <c r="P58" s="24">
         <v>43788</v>
       </c>
-      <c r="Q58" s="16" t="s">
-        <v>382</v>
-      </c>
-      <c r="R58" s="16" t="s">
-        <v>304</v>
-      </c>
-      <c r="S58" s="16" t="s">
-        <v>310</v>
-      </c>
+      <c r="Q58" s="16"/>
+      <c r="R58" s="16"/>
+      <c r="S58" s="16"/>
       <c r="T58" s="17"/>
-      <c r="U58" s="30"/>
-    </row>
-    <row r="59" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U58" s="29"/>
+    </row>
+    <row r="59" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A59" s="16" t="s">
-        <v>383</v>
-      </c>
-      <c r="B59" s="16"/>
-      <c r="C59" s="29" t="s">
-        <v>384</v>
+        <v>377</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="C59" s="35" t="s">
+        <v>378</v>
       </c>
       <c r="D59" s="16" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="E59" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F59" s="16" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="G59" s="16" t="s">
         <v>20</v>
@@ -5361,19 +5396,19 @@
         <v>380</v>
       </c>
       <c r="M59" s="16" t="s">
-        <v>470</v>
+        <v>257</v>
       </c>
       <c r="N59" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O59" s="16" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="P59" s="24">
         <v>43788</v>
       </c>
       <c r="Q59" s="16" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="R59" s="16" t="s">
         <v>304</v>
@@ -5382,24 +5417,24 @@
         <v>310</v>
       </c>
       <c r="T59" s="17"/>
-      <c r="U59" s="30"/>
-    </row>
-    <row r="60" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U59" s="29"/>
+    </row>
+    <row r="60" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A60" s="16" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="B60" s="16"/>
-      <c r="C60" s="29" t="s">
-        <v>390</v>
+      <c r="C60" s="35" t="s">
+        <v>384</v>
       </c>
       <c r="D60" s="16" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="E60" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F60" s="16" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="G60" s="16" t="s">
         <v>20</v>
@@ -5420,19 +5455,19 @@
         <v>380</v>
       </c>
       <c r="M60" s="16" t="s">
-        <v>257</v>
+        <v>470</v>
       </c>
       <c r="N60" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O60" s="16" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="P60" s="24">
         <v>43788</v>
       </c>
       <c r="Q60" s="16" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="R60" s="16" t="s">
         <v>304</v>
@@ -5441,24 +5476,24 @@
         <v>310</v>
       </c>
       <c r="T60" s="17"/>
-      <c r="U60" s="30"/>
-    </row>
-    <row r="61" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U60" s="29"/>
+    </row>
+    <row r="61" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A61" s="16" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="B61" s="16"/>
-      <c r="C61" s="29" t="s">
-        <v>395</v>
+      <c r="C61" s="35" t="s">
+        <v>390</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="E61" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F61" s="16" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="G61" s="16" t="s">
         <v>20</v>
@@ -5485,7 +5520,7 @@
         <v>110</v>
       </c>
       <c r="O61" s="16" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="P61" s="24">
         <v>43788</v>
@@ -5500,24 +5535,24 @@
         <v>310</v>
       </c>
       <c r="T61" s="17"/>
-      <c r="U61" s="30"/>
-    </row>
-    <row r="62" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U61" s="29"/>
+    </row>
+    <row r="62" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A62" s="16" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="B62" s="16"/>
-      <c r="C62" s="29" t="s">
-        <v>400</v>
+      <c r="C62" s="35" t="s">
+        <v>395</v>
       </c>
       <c r="D62" s="16" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="E62" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F62" s="16" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="G62" s="16" t="s">
         <v>20</v>
@@ -5538,19 +5573,19 @@
         <v>380</v>
       </c>
       <c r="M62" s="16" t="s">
-        <v>470</v>
+        <v>257</v>
       </c>
       <c r="N62" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O62" s="16" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="P62" s="24">
         <v>43788</v>
       </c>
       <c r="Q62" s="16" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="R62" s="16" t="s">
         <v>304</v>
@@ -5559,114 +5594,114 @@
         <v>310</v>
       </c>
       <c r="T62" s="17"/>
-      <c r="U62" s="30"/>
-    </row>
-    <row r="63" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="16"/>
+      <c r="U62" s="29"/>
+    </row>
+    <row r="63" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+      <c r="A63" s="16" t="s">
+        <v>399</v>
+      </c>
       <c r="B63" s="16"/>
-      <c r="C63" s="16"/>
-      <c r="D63" s="16"/>
-      <c r="E63" s="16"/>
-      <c r="F63" s="16"/>
-      <c r="G63" s="16"/>
-      <c r="H63" s="16"/>
-      <c r="I63" s="16"/>
-      <c r="J63" s="16"/>
-      <c r="K63" s="16"/>
-      <c r="L63" s="16"/>
+      <c r="C63" s="35" t="s">
+        <v>400</v>
+      </c>
+      <c r="D63" s="16" t="s">
+        <v>401</v>
+      </c>
+      <c r="E63" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="F63" s="16" t="s">
+        <v>402</v>
+      </c>
+      <c r="G63" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H63" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="I63" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="J63" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="K63" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="L63" s="16" t="s">
+        <v>380</v>
+      </c>
       <c r="M63" s="16" t="s">
-        <v>257</v>
+        <v>470</v>
       </c>
       <c r="N63" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="O63" s="16"/>
+      <c r="O63" s="16" t="s">
+        <v>403</v>
+      </c>
       <c r="P63" s="24">
         <v>43788</v>
       </c>
-      <c r="Q63" s="16"/>
-      <c r="R63" s="16"/>
-      <c r="S63" s="16"/>
+      <c r="Q63" s="16" t="s">
+        <v>388</v>
+      </c>
+      <c r="R63" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="S63" s="16" t="s">
+        <v>310</v>
+      </c>
       <c r="T63" s="17"/>
-      <c r="U63" s="30"/>
-    </row>
-    <row r="64" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="16" t="s">
-        <v>404</v>
-      </c>
-      <c r="B64" s="16" t="s">
-        <v>404</v>
-      </c>
-      <c r="C64" s="29" t="s">
-        <v>405</v>
-      </c>
-      <c r="D64" s="16" t="s">
-        <v>404</v>
-      </c>
-      <c r="E64" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="F64" s="16" t="s">
-        <v>406</v>
-      </c>
-      <c r="G64" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="H64" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="I64" s="16" t="s">
-        <v>404</v>
-      </c>
-      <c r="J64" s="16" t="s">
-        <v>404</v>
-      </c>
-      <c r="K64" s="16" t="s">
-        <v>404</v>
-      </c>
-      <c r="L64" s="16" t="s">
-        <v>407</v>
-      </c>
+      <c r="U63" s="29"/>
+    </row>
+    <row r="64" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A64" s="16"/>
+      <c r="B64" s="16"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="16"/>
+      <c r="H64" s="16"/>
+      <c r="I64" s="16"/>
+      <c r="J64" s="16"/>
+      <c r="K64" s="16"/>
+      <c r="L64" s="16"/>
       <c r="M64" s="16" t="s">
         <v>257</v>
       </c>
       <c r="N64" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="O64" s="16" t="s">
-        <v>408</v>
-      </c>
+      <c r="O64" s="16"/>
       <c r="P64" s="24">
         <v>43788</v>
       </c>
-      <c r="Q64" s="16" t="s">
-        <v>382</v>
-      </c>
-      <c r="R64" s="16" t="s">
-        <v>310</v>
-      </c>
-      <c r="S64" s="16" t="s">
-        <v>310</v>
-      </c>
+      <c r="Q64" s="16"/>
+      <c r="R64" s="16"/>
+      <c r="S64" s="16"/>
       <c r="T64" s="17"/>
-      <c r="U64" s="30"/>
-    </row>
-    <row r="65" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U64" s="29"/>
+    </row>
+    <row r="65" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A65" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="B65" s="16"/>
-      <c r="C65" s="29" t="s">
-        <v>410</v>
+        <v>404</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="C65" s="35" t="s">
+        <v>405</v>
       </c>
       <c r="D65" s="16" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="E65" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F65" s="16" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="G65" s="16" t="s">
         <v>20</v>
@@ -5693,7 +5728,7 @@
         <v>110</v>
       </c>
       <c r="O65" s="16" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="P65" s="24">
         <v>43788</v>
@@ -5702,30 +5737,30 @@
         <v>382</v>
       </c>
       <c r="R65" s="16" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="S65" s="16" t="s">
         <v>310</v>
       </c>
       <c r="T65" s="17"/>
-      <c r="U65" s="30"/>
-    </row>
-    <row r="66" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U65" s="29"/>
+    </row>
+    <row r="66" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A66" s="16" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="B66" s="16"/>
-      <c r="C66" s="29" t="s">
-        <v>415</v>
+      <c r="C66" s="35" t="s">
+        <v>410</v>
       </c>
       <c r="D66" s="16" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="E66" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F66" s="16" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="G66" s="16" t="s">
         <v>20</v>
@@ -5752,7 +5787,7 @@
         <v>110</v>
       </c>
       <c r="O66" s="16" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="P66" s="24">
         <v>43788</v>
@@ -5761,30 +5796,30 @@
         <v>382</v>
       </c>
       <c r="R66" s="16" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="S66" s="16" t="s">
         <v>310</v>
       </c>
       <c r="T66" s="17"/>
-      <c r="U66" s="30"/>
-    </row>
-    <row r="67" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U66" s="29"/>
+    </row>
+    <row r="67" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A67" s="16" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B67" s="16"/>
-      <c r="C67" s="29" t="s">
-        <v>420</v>
+      <c r="C67" s="35" t="s">
+        <v>415</v>
       </c>
       <c r="D67" s="16" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="E67" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F67" s="16" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="G67" s="16" t="s">
         <v>20</v>
@@ -5811,7 +5846,7 @@
         <v>110</v>
       </c>
       <c r="O67" s="16" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="P67" s="24">
         <v>43788</v>
@@ -5826,24 +5861,24 @@
         <v>310</v>
       </c>
       <c r="T67" s="17"/>
-      <c r="U67" s="30"/>
-    </row>
-    <row r="68" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U67" s="29"/>
+    </row>
+    <row r="68" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A68" s="16" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B68" s="16"/>
-      <c r="C68" s="29" t="s">
-        <v>425</v>
+      <c r="C68" s="35" t="s">
+        <v>420</v>
       </c>
       <c r="D68" s="16" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="E68" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F68" s="16" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="G68" s="16" t="s">
         <v>20</v>
@@ -5870,7 +5905,7 @@
         <v>110</v>
       </c>
       <c r="O68" s="16" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="P68" s="24">
         <v>43788</v>
@@ -5885,24 +5920,24 @@
         <v>310</v>
       </c>
       <c r="T68" s="17"/>
-      <c r="U68" s="30"/>
-    </row>
-    <row r="69" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U68" s="29"/>
+    </row>
+    <row r="69" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A69" s="16" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="B69" s="16"/>
-      <c r="C69" s="29" t="s">
-        <v>430</v>
+      <c r="C69" s="35" t="s">
+        <v>425</v>
       </c>
       <c r="D69" s="16" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="E69" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F69" s="16" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="G69" s="16" t="s">
         <v>20</v>
@@ -5929,7 +5964,7 @@
         <v>110</v>
       </c>
       <c r="O69" s="16" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="P69" s="24">
         <v>43788</v>
@@ -5944,24 +5979,24 @@
         <v>310</v>
       </c>
       <c r="T69" s="17"/>
-      <c r="U69" s="30"/>
-    </row>
-    <row r="70" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U69" s="29"/>
+    </row>
+    <row r="70" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A70" s="16" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="B70" s="16"/>
-      <c r="C70" s="29" t="s">
-        <v>435</v>
+      <c r="C70" s="35" t="s">
+        <v>430</v>
       </c>
       <c r="D70" s="16" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="E70" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F70" s="16" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="G70" s="16" t="s">
         <v>20</v>
@@ -5988,7 +6023,7 @@
         <v>110</v>
       </c>
       <c r="O70" s="16" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="P70" s="24">
         <v>43788</v>
@@ -6003,24 +6038,24 @@
         <v>310</v>
       </c>
       <c r="T70" s="17"/>
-      <c r="U70" s="30"/>
-    </row>
-    <row r="71" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U70" s="29"/>
+    </row>
+    <row r="71" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A71" s="16" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B71" s="16"/>
-      <c r="C71" s="29" t="s">
-        <v>440</v>
+      <c r="C71" s="35" t="s">
+        <v>435</v>
       </c>
       <c r="D71" s="16" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="E71" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F71" s="16" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="G71" s="16" t="s">
         <v>20</v>
@@ -6047,7 +6082,7 @@
         <v>110</v>
       </c>
       <c r="O71" s="16" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="P71" s="24">
         <v>43788</v>
@@ -6062,24 +6097,24 @@
         <v>310</v>
       </c>
       <c r="T71" s="17"/>
-      <c r="U71" s="30"/>
-    </row>
-    <row r="72" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U71" s="29"/>
+    </row>
+    <row r="72" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A72" s="16" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="B72" s="16"/>
-      <c r="C72" s="29" t="s">
-        <v>445</v>
+      <c r="C72" s="35" t="s">
+        <v>440</v>
       </c>
       <c r="D72" s="16" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="E72" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F72" s="16" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="G72" s="16" t="s">
         <v>20</v>
@@ -6106,7 +6141,7 @@
         <v>110</v>
       </c>
       <c r="O72" s="16" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="P72" s="24">
         <v>43788</v>
@@ -6121,24 +6156,24 @@
         <v>310</v>
       </c>
       <c r="T72" s="17"/>
-      <c r="U72" s="30"/>
-    </row>
-    <row r="73" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U72" s="29"/>
+    </row>
+    <row r="73" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A73" s="16" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="B73" s="16"/>
-      <c r="C73" s="29" t="s">
-        <v>450</v>
+      <c r="C73" s="35" t="s">
+        <v>445</v>
       </c>
       <c r="D73" s="16" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="E73" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F73" s="16" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="G73" s="16" t="s">
         <v>20</v>
@@ -6165,7 +6200,7 @@
         <v>110</v>
       </c>
       <c r="O73" s="16" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="P73" s="24">
         <v>43788</v>
@@ -6180,24 +6215,24 @@
         <v>310</v>
       </c>
       <c r="T73" s="17"/>
-      <c r="U73" s="30"/>
-    </row>
-    <row r="74" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U73" s="29"/>
+    </row>
+    <row r="74" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A74" s="16" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="B74" s="16"/>
-      <c r="C74" s="29" t="s">
-        <v>455</v>
+      <c r="C74" s="35" t="s">
+        <v>450</v>
       </c>
       <c r="D74" s="16" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="E74" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F74" s="16" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="G74" s="16" t="s">
         <v>20</v>
@@ -6224,7 +6259,7 @@
         <v>110</v>
       </c>
       <c r="O74" s="16" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="P74" s="24">
         <v>43788</v>
@@ -6239,24 +6274,24 @@
         <v>310</v>
       </c>
       <c r="T74" s="17"/>
-      <c r="U74" s="30"/>
-    </row>
-    <row r="75" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U74" s="29"/>
+    </row>
+    <row r="75" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A75" s="16" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="B75" s="16"/>
-      <c r="C75" s="29" t="s">
-        <v>460</v>
+      <c r="C75" s="35" t="s">
+        <v>455</v>
       </c>
       <c r="D75" s="16" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="E75" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F75" s="16" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="G75" s="16" t="s">
         <v>20</v>
@@ -6283,7 +6318,7 @@
         <v>110</v>
       </c>
       <c r="O75" s="16" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="P75" s="24">
         <v>43788</v>
@@ -6298,24 +6333,24 @@
         <v>310</v>
       </c>
       <c r="T75" s="17"/>
-      <c r="U75" s="30"/>
-    </row>
-    <row r="76" spans="1:21" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="U75" s="29"/>
+    </row>
+    <row r="76" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
       <c r="A76" s="16" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="B76" s="16"/>
-      <c r="C76" s="29" t="s">
-        <v>465</v>
+      <c r="C76" s="35" t="s">
+        <v>460</v>
       </c>
       <c r="D76" s="16" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="E76" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F76" s="16" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="G76" s="16" t="s">
         <v>20</v>
@@ -6342,7 +6377,7 @@
         <v>110</v>
       </c>
       <c r="O76" s="16" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="P76" s="24">
         <v>43788</v>
@@ -6357,81 +6392,84 @@
         <v>310</v>
       </c>
       <c r="T76" s="17"/>
-      <c r="U76" s="30"/>
-    </row>
-    <row r="77" spans="1:21" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="32" t="s">
+      <c r="U76" s="29"/>
+    </row>
+    <row r="77" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+      <c r="A77" s="16" t="s">
+        <v>464</v>
+      </c>
+      <c r="B77" s="16"/>
+      <c r="C77" s="35" t="s">
+        <v>465</v>
+      </c>
+      <c r="D77" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="E77" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="F77" s="16" t="s">
+        <v>467</v>
+      </c>
+      <c r="G77" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H77" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="I77" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="J77" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="K77" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="L77" s="16" t="s">
+        <v>407</v>
+      </c>
+      <c r="M77" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="N77" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="O77" s="16" t="s">
+        <v>468</v>
+      </c>
+      <c r="P77" s="24">
+        <v>43788</v>
+      </c>
+      <c r="Q77" s="16" t="s">
+        <v>382</v>
+      </c>
+      <c r="R77" s="16" t="s">
+        <v>310</v>
+      </c>
+      <c r="S77" s="16" t="s">
+        <v>310</v>
+      </c>
+      <c r="T77" s="17"/>
+      <c r="U77" s="29"/>
+    </row>
+    <row r="78" spans="1:21" s="31" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A78" s="30" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="78" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="16" t="s">
+    <row r="79" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B78" s="16" t="s">
+      <c r="B79" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="C78" s="16" t="s">
+      <c r="C79" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="D78" s="16" t="s">
+      <c r="D79" s="16" t="s">
         <v>60</v>
-      </c>
-      <c r="E78" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F78" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="G78" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="H78" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="I78" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="J78" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="K78" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="L78" s="16" t="s">
-        <v>249</v>
-      </c>
-      <c r="M78" s="16" t="s">
-        <v>256</v>
-      </c>
-      <c r="N78" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="O78" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="P78" s="24">
-        <v>42507</v>
-      </c>
-      <c r="Q78" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="R78" s="16"/>
-      <c r="S78" s="16"/>
-      <c r="T78" s="17"/>
-    </row>
-    <row r="79" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B79" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C79" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="D79" s="16" t="s">
-        <v>4</v>
       </c>
       <c r="E79" s="16" t="s">
         <v>25</v>
@@ -6446,48 +6484,48 @@
         <v>12</v>
       </c>
       <c r="I79" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J79" s="16" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="K79" s="16" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L79" s="16" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="M79" s="16" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="N79" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O79" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P79" s="24">
-        <v>41002</v>
+        <v>42507</v>
       </c>
       <c r="Q79" s="16" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="R79" s="16"/>
       <c r="S79" s="16"/>
       <c r="T79" s="17"/>
     </row>
-    <row r="80" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A80" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B80" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C80" s="16" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D80" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E80" s="16" t="s">
         <v>25</v>
@@ -6502,25 +6540,25 @@
         <v>12</v>
       </c>
       <c r="I80" s="16" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="J80" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K80" s="16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L80" s="16" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="M80" s="16" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="N80" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O80" s="16" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P80" s="24">
         <v>41002</v>
@@ -6532,18 +6570,18 @@
       <c r="S80" s="16"/>
       <c r="T80" s="17"/>
     </row>
-    <row r="81" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A81" s="16" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B81" s="16" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C81" s="16" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D81" s="16" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E81" s="16" t="s">
         <v>25</v>
@@ -6558,25 +6596,25 @@
         <v>12</v>
       </c>
       <c r="I81" s="16" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="J81" s="16" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="K81" s="16" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="L81" s="16" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="M81" s="16" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="N81" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O81" s="16" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="P81" s="24">
         <v>41002</v>
@@ -6588,40 +6626,72 @@
       <c r="S81" s="16"/>
       <c r="T81" s="17"/>
     </row>
-    <row r="82" spans="1:20" s="34" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="32" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="83" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="12" t="s">
+    <row r="82" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A82" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B82" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C82" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D82" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E82" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F82" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="G82" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H82" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I82" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="J82" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="K82" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="L82" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="M82" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="N82" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="O82" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="P82" s="24">
+        <v>41002</v>
+      </c>
+      <c r="Q82" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="R82" s="16"/>
+      <c r="S82" s="16"/>
+      <c r="T82" s="17"/>
+    </row>
+    <row r="83" spans="1:20" s="32" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A83" s="30" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A84" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="B83" s="3"/>
-      <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
-      <c r="E83" s="3"/>
-      <c r="F83" s="3"/>
-      <c r="G83" s="3"/>
-      <c r="I83" s="12"/>
-      <c r="J83" s="3"/>
-      <c r="K83" s="3"/>
-      <c r="L83" s="3"/>
-      <c r="M83" s="3"/>
-      <c r="N83" s="3"/>
-      <c r="O83" s="3"/>
-      <c r="P83" s="26"/>
-      <c r="Q83" s="3"/>
-      <c r="R83" s="3"/>
-      <c r="S83" s="3"/>
-      <c r="T83" s="3"/>
-    </row>
-    <row r="84" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="12" t="s">
-        <v>185</v>
-      </c>
       <c r="B84" s="3"/>
-      <c r="C84" s="3"/>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
@@ -6639,17 +6709,16 @@
       <c r="S84" s="3"/>
       <c r="T84" s="3"/>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A85" s="13" t="s">
-        <v>186</v>
+    <row r="85" spans="1:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A85" s="12" t="s">
+        <v>185</v>
       </c>
       <c r="B85" s="3"/>
-      <c r="C85" s="3"/>
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
-      <c r="I85" s="13"/>
+      <c r="I85" s="12"/>
       <c r="J85" s="3"/>
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
@@ -6662,12 +6731,11 @@
       <c r="S85" s="3"/>
       <c r="T85" s="3"/>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A86" s="13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B86" s="3"/>
-      <c r="C86" s="3"/>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
@@ -6685,24 +6753,47 @@
       <c r="S86" s="3"/>
       <c r="T86" s="3"/>
     </row>
-    <row r="87" spans="1:20" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A87" s="21" t="s">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A87" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="B87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
+      <c r="G87" s="3"/>
+      <c r="I87" s="13"/>
+      <c r="J87" s="3"/>
+      <c r="K87" s="3"/>
+      <c r="L87" s="3"/>
+      <c r="M87" s="3"/>
+      <c r="N87" s="3"/>
+      <c r="O87" s="3"/>
+      <c r="P87" s="26"/>
+      <c r="Q87" s="3"/>
+      <c r="R87" s="3"/>
+      <c r="S87" s="3"/>
+      <c r="T87" s="3"/>
+    </row>
+    <row r="88" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A88" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="P87" s="27"/>
-    </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A88" s="22" t="s">
+      <c r="C88" s="12"/>
+      <c r="P88" s="27"/>
+    </row>
+    <row r="89" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A89" s="22" t="s">
         <v>225</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A34:O37">
-    <sortCondition ref="A34:A37"/>
+  <sortState ref="A35:O38">
+    <sortCondition ref="A35:A38"/>
   </sortState>
   <mergeCells count="6">
-    <mergeCell ref="A77:XFD77"/>
-    <mergeCell ref="A82:XFD82"/>
+    <mergeCell ref="A78:XFD78"/>
+    <mergeCell ref="A83:XFD83"/>
     <mergeCell ref="A2:XFD2"/>
     <mergeCell ref="A4:XFD4"/>
     <mergeCell ref="A10:XFD10"/>
@@ -6725,14 +6816,14 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="141.5703125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="11.84375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="12.3828125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="141.53515625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
@@ -6743,7 +6834,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="6">
         <v>42080</v>
       </c>
@@ -6754,7 +6845,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="6">
         <v>42119</v>
       </c>
@@ -6765,7 +6856,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="6">
         <v>42131</v>
       </c>
@@ -6776,7 +6867,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="6">
         <v>42158</v>
       </c>
@@ -6787,7 +6878,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="6">
         <v>42248</v>
       </c>
@@ -6798,7 +6889,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="6">
         <v>42249</v>
       </c>
@@ -6809,7 +6900,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" s="6">
         <v>42507</v>
       </c>
@@ -6820,7 +6911,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" s="6">
         <v>42582</v>
       </c>
@@ -6831,7 +6922,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" s="6">
         <v>42724</v>
       </c>
@@ -6842,74 +6933,74 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11" s="33">
         <v>42835</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="32" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
-      <c r="B12" s="34"/>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A12" s="33"/>
+      <c r="B12" s="32"/>
       <c r="C12" s="7" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
-      <c r="B13" s="34"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A13" s="33"/>
+      <c r="B13" s="32"/>
       <c r="C13" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="34"/>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A14" s="33"/>
+      <c r="B14" s="32"/>
       <c r="C14" s="7" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
-      <c r="B15" s="34"/>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A15" s="33"/>
+      <c r="B15" s="32"/>
       <c r="C15" s="7" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
-      <c r="B16" s="34"/>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A16" s="33"/>
+      <c r="B16" s="32"/>
       <c r="C16" s="7" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
-      <c r="B17" s="34"/>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A17" s="33"/>
+      <c r="B17" s="32"/>
       <c r="C17" s="7" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
-      <c r="B18" s="34"/>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A18" s="33"/>
+      <c r="B18" s="32"/>
       <c r="C18" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
-      <c r="B19" s="34"/>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A19" s="33"/>
+      <c r="B19" s="32"/>
       <c r="C19" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" s="8">
         <v>42839</v>
       </c>
@@ -6920,7 +7011,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" s="8">
         <v>42839</v>
       </c>
@@ -6931,7 +7022,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" s="10">
         <v>42858</v>
       </c>
@@ -6942,7 +7033,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23" s="10">
         <v>42858</v>
       </c>
@@ -6953,7 +7044,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24" s="6">
         <v>42928</v>
       </c>
@@ -6964,7 +7055,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25" s="6">
         <v>42969</v>
       </c>
@@ -6975,7 +7066,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26" s="14">
         <v>42969</v>
       </c>
@@ -6986,7 +7077,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27" s="6">
         <v>43718</v>
       </c>
@@ -6997,7 +7088,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A28" s="6">
         <v>43804</v>
       </c>

</xml_diff>

<commit_message>
Issue #319: Namespace Updates - ID Requested:multi
Add the namespace 'multi' to the namespace registry and LDDTool config.properties file.

    Namespace ID Requested: multi
    Discipline or Mission LDD? Discipline
    Steward Organization Name: PDS PPI Node
    LDD Steward Name: Joseph Mafi
    LDD Steward Email: jmafi@igpp.ucla.edu
    LDD Description: The Multidimensional dictionary contains classes that describe relationships between multidimensional data objects contained within a single data product.
    Rationale for creation of new LDD: These classes are needed in order to describe the relationships between multidimensional array objects. They replicate the DEPEND_n attributes provided in CDF metadata. These classes were previously defined in v1 of the Particle dictionary, however, they apply to more than just particle data.

Resolves #319
</commit_message>
<xml_diff>
--- a/model-ontology/src/ontology/Data/pds-namespace-registry.xlsx
+++ b/model-ontology/src/ontology/Data/pds-namespace-registry.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20371"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\AAAPDS4\AADataModel\0000_Design\Namespaces_1002\NameSpaceRegistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D43093-C62B-4F56-BE56-154ED8752095}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C95BA38C-BA55-4812-B7EE-A6F99CEF0447}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1157" yWindow="1063" windowWidth="26657" windowHeight="12857" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1068" windowWidth="26652" windowHeight="12852" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Namespaces" sheetId="1" r:id="rId1"/>
     <sheet name="Change Log" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Namespaces!$A$11:$Q$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Namespaces!$A$11:$Q$30</definedName>
   </definedNames>
   <calcPr calcId="140001"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1343" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4705" uniqueCount="523">
   <si>
     <t>Registration Date</t>
   </si>
@@ -1589,6 +1589,18 @@
   </si>
   <si>
     <t>sbnpsi</t>
+  </si>
+  <si>
+    <t>multi</t>
+  </si>
+  <si>
+    <t>http://pds.nasa.gov/pds4/multi/v1</t>
+  </si>
+  <si>
+    <t>PDS4_MULTI</t>
+  </si>
+  <si>
+    <t>The Multidimensional dictionary contains classes that describe relationships between multidimensional data objects contained within a single data product.</t>
   </si>
 </sst>
 </file>
@@ -1755,7 +1767,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1844,6 +1856,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1856,16 +1881,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2179,39 +2197,39 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U89"/>
+  <dimension ref="A1:U90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="15.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.3828125" style="22" customWidth="1"/>
-    <col min="2" max="2" width="16.69140625" style="22" customWidth="1"/>
-    <col min="3" max="3" width="46.15234375" style="12" customWidth="1"/>
-    <col min="4" max="4" width="13.3828125" style="22" customWidth="1"/>
-    <col min="5" max="5" width="14.3828125" style="22" customWidth="1"/>
-    <col min="6" max="6" width="22.84375" style="22" customWidth="1"/>
-    <col min="7" max="7" width="12.3828125" style="22" customWidth="1"/>
-    <col min="8" max="8" width="21.3828125" style="22" customWidth="1"/>
-    <col min="9" max="9" width="25.3046875" style="22" customWidth="1"/>
-    <col min="10" max="10" width="13.15234375" style="22" customWidth="1"/>
-    <col min="11" max="11" width="18.765625" style="22" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" style="22" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="46.109375" style="12" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" style="22" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="22" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" style="22" customWidth="1"/>
+    <col min="9" max="9" width="25.33203125" style="22" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" style="22" customWidth="1"/>
+    <col min="11" max="11" width="18.77734375" style="22" customWidth="1"/>
     <col min="12" max="12" width="23" style="22" customWidth="1"/>
-    <col min="13" max="13" width="38.69140625" style="22" customWidth="1"/>
-    <col min="14" max="14" width="10.15234375" style="22" customWidth="1"/>
-    <col min="15" max="15" width="53.84375" style="22" customWidth="1"/>
-    <col min="16" max="16" width="16.15234375" style="27" customWidth="1"/>
-    <col min="17" max="17" width="14.15234375" style="22" customWidth="1"/>
-    <col min="18" max="18" width="11.3828125" style="22" customWidth="1"/>
-    <col min="19" max="19" width="11.15234375" style="22" customWidth="1"/>
-    <col min="20" max="20" width="13.69140625" style="22" customWidth="1"/>
-    <col min="21" max="16384" width="8.84375" style="22"/>
+    <col min="13" max="13" width="38.6640625" style="22" customWidth="1"/>
+    <col min="14" max="14" width="10.109375" style="22" customWidth="1"/>
+    <col min="15" max="15" width="53.88671875" style="22" customWidth="1"/>
+    <col min="16" max="16" width="16.109375" style="27" customWidth="1"/>
+    <col min="17" max="17" width="14.109375" style="22" customWidth="1"/>
+    <col min="18" max="18" width="11.33203125" style="22" customWidth="1"/>
+    <col min="19" max="19" width="11.109375" style="22" customWidth="1"/>
+    <col min="20" max="20" width="13.6640625" style="22" customWidth="1"/>
+    <col min="21" max="16384" width="8.88671875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="47.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="47.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>179</v>
       </c>
@@ -2273,12 +2291,12 @@
         <v>302</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:20" s="36" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="35" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>2</v>
       </c>
@@ -2338,12 +2356,12 @@
       </c>
       <c r="T3" s="17"/>
     </row>
-    <row r="4" spans="1:20" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="30" t="s">
+    <row r="4" spans="1:20" s="36" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="35" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:20" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>102</v>
       </c>
@@ -2403,7 +2421,7 @@
       </c>
       <c r="T5" s="17"/>
     </row>
-    <row r="6" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:20" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>189</v>
       </c>
@@ -2463,7 +2481,7 @@
       </c>
       <c r="T6" s="17"/>
     </row>
-    <row r="7" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>26</v>
       </c>
@@ -2525,7 +2543,7 @@
         <v>42277</v>
       </c>
     </row>
-    <row r="8" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>101</v>
       </c>
@@ -2585,14 +2603,14 @@
       </c>
       <c r="T8" s="17"/>
     </row>
-    <row r="9" spans="1:20" s="28" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:20" s="28" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
         <v>499</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>499</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="33" t="s">
         <v>508</v>
       </c>
       <c r="D9" s="19" t="s">
@@ -2645,12 +2663,12 @@
       </c>
       <c r="T9" s="20"/>
     </row>
-    <row r="10" spans="1:20" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="30" t="s">
+    <row r="10" spans="1:20" s="36" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="35" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:20" s="28" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:20" s="28" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
         <v>36</v>
       </c>
@@ -2710,7 +2728,7 @@
       </c>
       <c r="T11" s="17"/>
     </row>
-    <row r="12" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
         <v>3</v>
       </c>
@@ -2770,7 +2788,7 @@
       </c>
       <c r="T12" s="17"/>
     </row>
-    <row r="13" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:20" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
         <v>63</v>
       </c>
@@ -2830,7 +2848,7 @@
       </c>
       <c r="T13" s="17"/>
     </row>
-    <row r="14" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>14</v>
       </c>
@@ -2890,7 +2908,7 @@
       </c>
       <c r="T14" s="17"/>
     </row>
-    <row r="15" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:20" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
         <v>41</v>
       </c>
@@ -2950,7 +2968,7 @@
       </c>
       <c r="T15" s="17"/>
     </row>
-    <row r="16" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
         <v>5</v>
       </c>
@@ -3010,7 +3028,7 @@
       </c>
       <c r="T16" s="17"/>
     </row>
-    <row r="17" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:20" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
         <v>276</v>
       </c>
@@ -3070,7 +3088,7 @@
       </c>
       <c r="T17" s="17"/>
     </row>
-    <row r="18" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:20" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
         <v>277</v>
       </c>
@@ -3130,14 +3148,14 @@
       </c>
       <c r="T18" s="17"/>
     </row>
-    <row r="19" spans="1:20" s="28" customFormat="1" ht="47.6" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:20" s="28" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
         <v>488</v>
       </c>
       <c r="B19" s="19" t="s">
         <v>488</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="31" t="s">
         <v>489</v>
       </c>
       <c r="D19" s="19" t="s">
@@ -3190,7 +3208,7 @@
       </c>
       <c r="T19" s="20"/>
     </row>
-    <row r="20" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:20" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
         <v>18</v>
       </c>
@@ -3250,7 +3268,7 @@
       </c>
       <c r="T20" s="17"/>
     </row>
-    <row r="21" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
         <v>2</v>
       </c>
@@ -3310,7 +3328,7 @@
       </c>
       <c r="T21" s="17"/>
     </row>
-    <row r="22" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:20" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
         <v>8</v>
       </c>
@@ -3370,7 +3388,7 @@
       </c>
       <c r="T22" s="17"/>
     </row>
-    <row r="23" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:20" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
         <v>285</v>
       </c>
@@ -3430,7 +3448,7 @@
       </c>
       <c r="T23" s="17"/>
     </row>
-    <row r="24" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
         <v>9</v>
       </c>
@@ -3490,7 +3508,7 @@
       </c>
       <c r="T24" s="17"/>
     </row>
-    <row r="25" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16" t="s">
         <v>11</v>
       </c>
@@ -3548,7 +3566,7 @@
       </c>
       <c r="T25" s="17"/>
     </row>
-    <row r="26" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="16" t="s">
         <v>39</v>
       </c>
@@ -3608,7 +3626,7 @@
       </c>
       <c r="T26" s="17"/>
     </row>
-    <row r="27" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16" t="s">
         <v>226</v>
       </c>
@@ -3668,14 +3686,14 @@
       </c>
       <c r="T27" s="17"/>
     </row>
-    <row r="28" spans="1:20" s="28" customFormat="1" ht="47.6" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:20" s="28" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A28" s="19" t="s">
         <v>480</v>
       </c>
       <c r="B28" s="19" t="s">
         <v>480</v>
       </c>
-      <c r="C28" s="34" t="s">
+      <c r="C28" s="31" t="s">
         <v>481</v>
       </c>
       <c r="D28" s="19" t="s">
@@ -3728,7 +3746,7 @@
       </c>
       <c r="T28" s="20"/>
     </row>
-    <row r="29" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:20" s="30" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A29" s="16" t="s">
         <v>19</v>
       </c>
@@ -3788,209 +3806,209 @@
       </c>
       <c r="T29" s="17"/>
     </row>
-    <row r="30" spans="1:20" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="30" t="s">
+    <row r="30" spans="1:20" s="28" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="19" t="s">
+        <v>519</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>519</v>
+      </c>
+      <c r="C30" s="39" t="s">
+        <v>520</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>519</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>521</v>
+      </c>
+      <c r="G30" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I30" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="J30" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="K30" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="L30" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="M30" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="N30" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="O30" s="19" t="s">
+        <v>522</v>
+      </c>
+      <c r="P30" s="25">
+        <v>44257</v>
+      </c>
+      <c r="Q30" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="R30" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="S30" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="T30" s="20"/>
+    </row>
+    <row r="31" spans="1:20" s="36" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="35" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="16" t="s">
+    <row r="32" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B32" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C32" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D32" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E31" s="16" t="s">
+      <c r="E32" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F31" s="16" t="s">
+      <c r="F32" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="G31" s="16" t="s">
+      <c r="G32" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="H31" s="16" t="s">
+      <c r="H32" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I31" s="16" t="s">
+      <c r="I32" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="J31" s="16" t="s">
+      <c r="J32" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="K31" s="16" t="s">
+      <c r="K32" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="L31" s="16" t="s">
+      <c r="L32" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="M31" s="16" t="s">
+      <c r="M32" s="16" t="s">
         <v>272</v>
       </c>
-      <c r="N31" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="O31" s="16" t="s">
+      <c r="N32" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="O32" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="P31" s="24">
+      <c r="P32" s="24">
         <v>42089</v>
       </c>
-      <c r="Q31" s="16" t="s">
+      <c r="Q32" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="R31" s="16" t="s">
-        <v>304</v>
-      </c>
-      <c r="S31" s="16" t="s">
-        <v>304</v>
-      </c>
-      <c r="T31" s="17"/>
-    </row>
-    <row r="32" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="19" t="s">
+      <c r="R32" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="S32" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="T32" s="17"/>
+    </row>
+    <row r="33" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="19" t="s">
         <v>509</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="B33" s="19" t="s">
         <v>510</v>
       </c>
-      <c r="C32" s="37" t="s">
+      <c r="C33" s="34" t="s">
         <v>517</v>
       </c>
-      <c r="D32" s="19" t="s">
+      <c r="D33" s="19" t="s">
         <v>509</v>
       </c>
-      <c r="E32" s="19" t="s">
+      <c r="E33" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F32" s="19" t="s">
+      <c r="F33" s="19" t="s">
         <v>516</v>
       </c>
-      <c r="G32" s="19" t="s">
+      <c r="G33" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H32" s="19" t="s">
+      <c r="H33" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="I32" s="19" t="s">
+      <c r="I33" s="19" t="s">
         <v>515</v>
       </c>
-      <c r="J32" s="19" t="s">
+      <c r="J33" s="19" t="s">
         <v>518</v>
       </c>
-      <c r="K32" s="19" t="s">
+      <c r="K33" s="19" t="s">
         <v>484</v>
       </c>
-      <c r="L32" s="19" t="s">
+      <c r="L33" s="19" t="s">
         <v>511</v>
       </c>
-      <c r="M32" s="19" t="s">
+      <c r="M33" s="19" t="s">
         <v>512</v>
       </c>
-      <c r="N32" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="O32" s="19" t="s">
+      <c r="N33" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="O33" s="19" t="s">
         <v>513</v>
       </c>
-      <c r="P32" s="25">
+      <c r="P33" s="25">
         <v>44193</v>
       </c>
-      <c r="Q32" s="19" t="s">
+      <c r="Q33" s="19" t="s">
         <v>514</v>
       </c>
-      <c r="R32" s="19" t="s">
-        <v>304</v>
-      </c>
-      <c r="S32" s="19" t="s">
-        <v>304</v>
-      </c>
-      <c r="T32" s="20"/>
-    </row>
-    <row r="33" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="16" t="s">
+      <c r="R33" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="S33" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="T33" s="20"/>
+    </row>
+    <row r="34" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B34" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="C34" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="D34" s="16" t="s">
         <v>68</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F33" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="G33" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="H33" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="I33" s="16" t="s">
-        <v>209</v>
-      </c>
-      <c r="J33" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K33" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="L33" s="16" t="s">
-        <v>248</v>
-      </c>
-      <c r="M33" s="16" t="s">
-        <v>262</v>
-      </c>
-      <c r="N33" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="O33" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="P33" s="24">
-        <v>42119</v>
-      </c>
-      <c r="Q33" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="R33" s="16" t="s">
-        <v>304</v>
-      </c>
-      <c r="S33" s="16" t="s">
-        <v>304</v>
-      </c>
-      <c r="T33" s="17"/>
-    </row>
-    <row r="34" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>55</v>
       </c>
       <c r="E34" s="16" t="s">
         <v>25</v>
       </c>
       <c r="F34" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G34" s="16" t="s">
         <v>20</v>
@@ -3999,31 +4017,31 @@
         <v>12</v>
       </c>
       <c r="I34" s="16" t="s">
-        <v>119</v>
+        <v>209</v>
       </c>
       <c r="J34" s="16" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K34" s="16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="L34" s="16" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="M34" s="16" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="N34" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O34" s="16" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="P34" s="24">
-        <v>41837</v>
+        <v>42119</v>
       </c>
       <c r="Q34" s="16" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="R34" s="16" t="s">
         <v>304</v>
@@ -4033,15 +4051,15 @@
       </c>
       <c r="T34" s="17"/>
     </row>
-    <row r="35" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="16" t="s">
         <v>55</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="D35" s="16" t="s">
         <v>55</v>
@@ -4077,7 +4095,7 @@
         <v>110</v>
       </c>
       <c r="O35" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P35" s="24">
         <v>41837</v>
@@ -4093,24 +4111,24 @@
       </c>
       <c r="T35" s="17"/>
     </row>
-    <row r="36" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A36" s="16" t="s">
-        <v>474</v>
+        <v>55</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>475</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>476</v>
+        <v>55</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>78</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>474</v>
+        <v>55</v>
       </c>
       <c r="E36" s="16" t="s">
         <v>25</v>
       </c>
       <c r="F36" s="16" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="G36" s="16" t="s">
         <v>20</v>
@@ -4119,31 +4137,31 @@
         <v>12</v>
       </c>
       <c r="I36" s="16" t="s">
-        <v>477</v>
+        <v>119</v>
       </c>
       <c r="J36" s="16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K36" s="16" t="s">
-        <v>478</v>
+        <v>126</v>
       </c>
       <c r="L36" s="16" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="M36" s="16" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="N36" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O36" s="16" t="s">
-        <v>479</v>
+        <v>153</v>
       </c>
       <c r="P36" s="24">
-        <v>43935</v>
+        <v>41837</v>
       </c>
       <c r="Q36" s="16" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="R36" s="16" t="s">
         <v>304</v>
@@ -4153,18 +4171,18 @@
       </c>
       <c r="T36" s="17"/>
     </row>
-    <row r="37" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="16" t="s">
-        <v>34</v>
+        <v>474</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" s="16" t="s">
-        <v>91</v>
+        <v>475</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>476</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>34</v>
+        <v>474</v>
       </c>
       <c r="E37" s="16" t="s">
         <v>25</v>
@@ -4179,31 +4197,31 @@
         <v>12</v>
       </c>
       <c r="I37" s="16" t="s">
-        <v>210</v>
+        <v>477</v>
       </c>
       <c r="J37" s="16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K37" s="16" t="s">
-        <v>128</v>
+        <v>478</v>
       </c>
       <c r="L37" s="16" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="M37" s="16" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="N37" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O37" s="16" t="s">
-        <v>155</v>
+        <v>479</v>
       </c>
       <c r="P37" s="24">
-        <v>41600</v>
+        <v>43935</v>
       </c>
       <c r="Q37" s="16" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="R37" s="16" t="s">
         <v>304</v>
@@ -4213,18 +4231,18 @@
       </c>
       <c r="T37" s="17"/>
     </row>
-    <row r="38" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="16" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="E38" s="16" t="s">
         <v>25</v>
@@ -4239,7 +4257,7 @@
         <v>12</v>
       </c>
       <c r="I38" s="16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J38" s="16" t="s">
         <v>5</v>
@@ -4257,13 +4275,13 @@
         <v>110</v>
       </c>
       <c r="O38" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P38" s="24">
-        <v>42220</v>
+        <v>41600</v>
       </c>
       <c r="Q38" s="16" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="R38" s="16" t="s">
         <v>304</v>
@@ -4273,24 +4291,24 @@
       </c>
       <c r="T38" s="17"/>
     </row>
-    <row r="39" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="16" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E39" s="16" t="s">
         <v>25</v>
       </c>
       <c r="F39" s="16" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="G39" s="16" t="s">
         <v>20</v>
@@ -4299,31 +4317,31 @@
         <v>12</v>
       </c>
       <c r="I39" s="16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J39" s="16" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K39" s="16" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="L39" s="16" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="M39" s="16" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="N39" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O39" s="16" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="P39" s="24">
-        <v>42158</v>
+        <v>42220</v>
       </c>
       <c r="Q39" s="16" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="R39" s="16" t="s">
         <v>304</v>
@@ -4333,15 +4351,15 @@
       </c>
       <c r="T39" s="17"/>
     </row>
-    <row r="40" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="D40" s="16" t="s">
         <v>43</v>
@@ -4377,7 +4395,7 @@
         <v>110</v>
       </c>
       <c r="O40" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="P40" s="24">
         <v>42158</v>
@@ -4393,24 +4411,24 @@
       </c>
       <c r="T40" s="17"/>
     </row>
-    <row r="41" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16" t="s">
-        <v>234</v>
+        <v>43</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>235</v>
+        <v>43</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>236</v>
+        <v>79</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>234</v>
+        <v>43</v>
       </c>
       <c r="E41" s="16" t="s">
         <v>25</v>
       </c>
       <c r="F41" s="16" t="s">
-        <v>237</v>
+        <v>120</v>
       </c>
       <c r="G41" s="16" t="s">
         <v>20</v>
@@ -4419,31 +4437,31 @@
         <v>12</v>
       </c>
       <c r="I41" s="16" t="s">
-        <v>238</v>
+        <v>213</v>
       </c>
       <c r="J41" s="16" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K41" s="16" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="L41" s="16" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="M41" s="16" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="N41" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O41" s="16" t="s">
-        <v>239</v>
+        <v>159</v>
       </c>
       <c r="P41" s="24">
-        <v>42650</v>
+        <v>42158</v>
       </c>
       <c r="Q41" s="16" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="R41" s="16" t="s">
         <v>304</v>
@@ -4453,24 +4471,24 @@
       </c>
       <c r="T41" s="17"/>
     </row>
-    <row r="42" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="16" t="s">
-        <v>35</v>
+        <v>234</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>50</v>
+        <v>235</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>94</v>
+        <v>236</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>35</v>
+        <v>234</v>
       </c>
       <c r="E42" s="16" t="s">
         <v>25</v>
       </c>
       <c r="F42" s="16" t="s">
-        <v>110</v>
+        <v>237</v>
       </c>
       <c r="G42" s="16" t="s">
         <v>20</v>
@@ -4479,31 +4497,31 @@
         <v>12</v>
       </c>
       <c r="I42" s="16" t="s">
-        <v>212</v>
+        <v>238</v>
       </c>
       <c r="J42" s="16" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="K42" s="16" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="L42" s="16" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="M42" s="16" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="N42" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O42" s="16" t="s">
-        <v>157</v>
+        <v>239</v>
       </c>
       <c r="P42" s="24">
-        <v>41771</v>
+        <v>42650</v>
       </c>
       <c r="Q42" s="16" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="R42" s="16" t="s">
         <v>304</v>
@@ -4513,83 +4531,84 @@
       </c>
       <c r="T42" s="17"/>
     </row>
-    <row r="43" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="16" t="s">
-        <v>305</v>
+        <v>35</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>305</v>
-      </c>
-      <c r="C43" s="35" t="s">
-        <v>306</v>
+        <v>50</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>94</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>305</v>
+        <v>35</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>303</v>
+        <v>25</v>
       </c>
       <c r="F43" s="16" t="s">
-        <v>307</v>
+        <v>110</v>
       </c>
       <c r="G43" s="16" t="s">
         <v>20</v>
       </c>
       <c r="H43" s="16" t="s">
-        <v>175</v>
+        <v>12</v>
       </c>
       <c r="I43" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="J43" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="K43" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="L43" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="M43" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="N43" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="O43" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="P43" s="24">
+        <v>41771</v>
+      </c>
+      <c r="Q43" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="R43" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="S43" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="T43" s="17"/>
+    </row>
+    <row r="44" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="J43" s="16" t="s">
+      <c r="B44" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="K43" s="16" t="s">
+      <c r="C44" s="32" t="s">
+        <v>306</v>
+      </c>
+      <c r="D44" s="16" t="s">
         <v>305</v>
-      </c>
-      <c r="L43" s="16" t="s">
-        <v>308</v>
-      </c>
-      <c r="M43" s="16" t="s">
-        <v>472</v>
-      </c>
-      <c r="N43" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="O43" s="16" t="s">
-        <v>309</v>
-      </c>
-      <c r="P43" s="24">
-        <v>43788</v>
-      </c>
-      <c r="Q43" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="R43" s="16" t="s">
-        <v>304</v>
-      </c>
-      <c r="S43" s="16" t="s">
-        <v>310</v>
-      </c>
-      <c r="T43" s="17"/>
-      <c r="U43" s="29"/>
-    </row>
-    <row r="44" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
-      <c r="A44" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="B44" s="16"/>
-      <c r="C44" s="35" t="s">
-        <v>312</v>
-      </c>
-      <c r="D44" s="16" t="s">
-        <v>313</v>
       </c>
       <c r="E44" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F44" s="16" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="G44" s="16" t="s">
         <v>20</v>
@@ -4610,22 +4629,22 @@
         <v>308</v>
       </c>
       <c r="M44" s="16" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="N44" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O44" s="16" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="P44" s="24">
         <v>43788</v>
       </c>
       <c r="Q44" s="16" t="s">
-        <v>316</v>
+        <v>27</v>
       </c>
       <c r="R44" s="16" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="S44" s="16" t="s">
         <v>310</v>
@@ -4633,22 +4652,22 @@
       <c r="T44" s="17"/>
       <c r="U44" s="29"/>
     </row>
-    <row r="45" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A45" s="16" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="B45" s="16"/>
-      <c r="C45" s="35" t="s">
-        <v>318</v>
+      <c r="C45" s="32" t="s">
+        <v>312</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="E45" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F45" s="16" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="G45" s="16" t="s">
         <v>20</v>
@@ -4656,9 +4675,15 @@
       <c r="H45" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="I45" s="16"/>
-      <c r="J45" s="16"/>
-      <c r="K45" s="16"/>
+      <c r="I45" s="16" t="s">
+        <v>305</v>
+      </c>
+      <c r="J45" s="16" t="s">
+        <v>305</v>
+      </c>
+      <c r="K45" s="16" t="s">
+        <v>305</v>
+      </c>
       <c r="L45" s="16" t="s">
         <v>308</v>
       </c>
@@ -4669,7 +4694,7 @@
         <v>110</v>
       </c>
       <c r="O45" s="16" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="P45" s="24">
         <v>43788</v>
@@ -4678,7 +4703,7 @@
         <v>316</v>
       </c>
       <c r="R45" s="16" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="S45" s="16" t="s">
         <v>310</v>
@@ -4686,22 +4711,22 @@
       <c r="T45" s="17"/>
       <c r="U45" s="29"/>
     </row>
-    <row r="46" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A46" s="16" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B46" s="16"/>
-      <c r="C46" s="35" t="s">
-        <v>323</v>
+      <c r="C46" s="32" t="s">
+        <v>318</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="E46" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F46" s="16" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="G46" s="16" t="s">
         <v>20</v>
@@ -4722,7 +4747,7 @@
         <v>110</v>
       </c>
       <c r="O46" s="16" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="P46" s="24">
         <v>43788</v>
@@ -4731,7 +4756,7 @@
         <v>316</v>
       </c>
       <c r="R46" s="16" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="S46" s="16" t="s">
         <v>310</v>
@@ -4739,22 +4764,22 @@
       <c r="T46" s="17"/>
       <c r="U46" s="29"/>
     </row>
-    <row r="47" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A47" s="16" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="B47" s="16"/>
-      <c r="C47" s="35" t="s">
-        <v>328</v>
+      <c r="C47" s="32" t="s">
+        <v>323</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="E47" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F47" s="16" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="G47" s="16" t="s">
         <v>20</v>
@@ -4775,7 +4800,7 @@
         <v>110</v>
       </c>
       <c r="O47" s="16" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="P47" s="24">
         <v>43788</v>
@@ -4792,22 +4817,22 @@
       <c r="T47" s="17"/>
       <c r="U47" s="29"/>
     </row>
-    <row r="48" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A48" s="16" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="B48" s="16"/>
-      <c r="C48" s="35" t="s">
-        <v>333</v>
+      <c r="C48" s="32" t="s">
+        <v>328</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="E48" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F48" s="16" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="G48" s="16" t="s">
         <v>20</v>
@@ -4828,7 +4853,7 @@
         <v>110</v>
       </c>
       <c r="O48" s="16" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="P48" s="24">
         <v>43788</v>
@@ -4845,22 +4870,22 @@
       <c r="T48" s="17"/>
       <c r="U48" s="29"/>
     </row>
-    <row r="49" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A49" s="16" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="B49" s="16"/>
-      <c r="C49" s="35" t="s">
-        <v>338</v>
+      <c r="C49" s="32" t="s">
+        <v>333</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="E49" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F49" s="16" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="G49" s="16" t="s">
         <v>20</v>
@@ -4881,7 +4906,7 @@
         <v>110</v>
       </c>
       <c r="O49" s="16" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="P49" s="24">
         <v>43788</v>
@@ -4898,22 +4923,22 @@
       <c r="T49" s="17"/>
       <c r="U49" s="29"/>
     </row>
-    <row r="50" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A50" s="16" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="B50" s="16"/>
-      <c r="C50" s="35" t="s">
-        <v>343</v>
+      <c r="C50" s="32" t="s">
+        <v>338</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="E50" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F50" s="16" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G50" s="16" t="s">
         <v>20</v>
@@ -4934,7 +4959,7 @@
         <v>110</v>
       </c>
       <c r="O50" s="16" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="P50" s="24">
         <v>43788</v>
@@ -4951,22 +4976,22 @@
       <c r="T50" s="17"/>
       <c r="U50" s="29"/>
     </row>
-    <row r="51" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A51" s="16" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="B51" s="16"/>
-      <c r="C51" s="35" t="s">
-        <v>348</v>
+      <c r="C51" s="32" t="s">
+        <v>343</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="E51" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F51" s="16" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="G51" s="16" t="s">
         <v>20</v>
@@ -4987,7 +5012,7 @@
         <v>110</v>
       </c>
       <c r="O51" s="16" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="P51" s="24">
         <v>43788</v>
@@ -5004,22 +5029,22 @@
       <c r="T51" s="17"/>
       <c r="U51" s="29"/>
     </row>
-    <row r="52" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A52" s="16" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="B52" s="16"/>
-      <c r="C52" s="35" t="s">
-        <v>353</v>
+      <c r="C52" s="32" t="s">
+        <v>348</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="E52" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F52" s="16" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="G52" s="16" t="s">
         <v>20</v>
@@ -5040,7 +5065,7 @@
         <v>110</v>
       </c>
       <c r="O52" s="16" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="P52" s="24">
         <v>43788</v>
@@ -5057,22 +5082,22 @@
       <c r="T52" s="17"/>
       <c r="U52" s="29"/>
     </row>
-    <row r="53" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A53" s="16" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="B53" s="16"/>
-      <c r="C53" s="35" t="s">
-        <v>358</v>
+      <c r="C53" s="32" t="s">
+        <v>353</v>
       </c>
       <c r="D53" s="16" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="E53" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F53" s="16" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="G53" s="16" t="s">
         <v>20</v>
@@ -5093,7 +5118,7 @@
         <v>110</v>
       </c>
       <c r="O53" s="16" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="P53" s="24">
         <v>43788</v>
@@ -5110,22 +5135,22 @@
       <c r="T53" s="17"/>
       <c r="U53" s="29"/>
     </row>
-    <row r="54" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A54" s="16" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="B54" s="16"/>
-      <c r="C54" s="35" t="s">
-        <v>363</v>
+      <c r="C54" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="E54" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F54" s="16" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="G54" s="16" t="s">
         <v>20</v>
@@ -5146,7 +5171,7 @@
         <v>110</v>
       </c>
       <c r="O54" s="16" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="P54" s="24">
         <v>43788</v>
@@ -5163,22 +5188,22 @@
       <c r="T54" s="17"/>
       <c r="U54" s="29"/>
     </row>
-    <row r="55" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A55" s="16" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="B55" s="16"/>
-      <c r="C55" s="35" t="s">
-        <v>368</v>
+      <c r="C55" s="32" t="s">
+        <v>363</v>
       </c>
       <c r="D55" s="16" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="E55" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F55" s="16" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="G55" s="16" t="s">
         <v>20</v>
@@ -5199,7 +5224,7 @@
         <v>110</v>
       </c>
       <c r="O55" s="16" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="P55" s="24">
         <v>43788</v>
@@ -5216,22 +5241,22 @@
       <c r="T55" s="17"/>
       <c r="U55" s="29"/>
     </row>
-    <row r="56" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A56" s="16" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="B56" s="16"/>
-      <c r="C56" s="35" t="s">
-        <v>373</v>
+      <c r="C56" s="32" t="s">
+        <v>368</v>
       </c>
       <c r="D56" s="16" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="E56" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F56" s="16" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="G56" s="16" t="s">
         <v>20</v>
@@ -5252,7 +5277,7 @@
         <v>110</v>
       </c>
       <c r="O56" s="16" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="P56" s="24">
         <v>43788</v>
@@ -5269,172 +5294,166 @@
       <c r="T56" s="17"/>
       <c r="U56" s="29"/>
     </row>
-    <row r="57" spans="1:21" s="28" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
-      <c r="A57" s="19" t="s">
+    <row r="57" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A57" s="16" t="s">
+        <v>372</v>
+      </c>
+      <c r="B57" s="16"/>
+      <c r="C57" s="32" t="s">
+        <v>373</v>
+      </c>
+      <c r="D57" s="16" t="s">
+        <v>374</v>
+      </c>
+      <c r="E57" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="F57" s="16" t="s">
+        <v>375</v>
+      </c>
+      <c r="G57" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H57" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="I57" s="16"/>
+      <c r="J57" s="16"/>
+      <c r="K57" s="16"/>
+      <c r="L57" s="16" t="s">
+        <v>308</v>
+      </c>
+      <c r="M57" s="16" t="s">
+        <v>471</v>
+      </c>
+      <c r="N57" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="O57" s="16" t="s">
+        <v>376</v>
+      </c>
+      <c r="P57" s="24">
+        <v>43788</v>
+      </c>
+      <c r="Q57" s="16" t="s">
+        <v>316</v>
+      </c>
+      <c r="R57" s="16" t="s">
+        <v>310</v>
+      </c>
+      <c r="S57" s="16" t="s">
+        <v>310</v>
+      </c>
+      <c r="T57" s="17"/>
+      <c r="U57" s="29"/>
+    </row>
+    <row r="58" spans="1:21" s="28" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A58" s="19" t="s">
         <v>492</v>
       </c>
-      <c r="B57" s="19" t="s">
+      <c r="B58" s="19" t="s">
         <v>493</v>
       </c>
-      <c r="C57" s="34" t="s">
+      <c r="C58" s="31" t="s">
         <v>494</v>
       </c>
-      <c r="D57" s="19" t="s">
+      <c r="D58" s="19" t="s">
         <v>492</v>
       </c>
-      <c r="E57" s="19" t="s">
+      <c r="E58" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F57" s="19" t="s">
+      <c r="F58" s="19" t="s">
         <v>498</v>
       </c>
-      <c r="G57" s="19" t="s">
+      <c r="G58" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H57" s="19" t="s">
+      <c r="H58" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="I57" s="19" t="s">
+      <c r="I58" s="19" t="s">
         <v>492</v>
       </c>
-      <c r="J57" s="19" t="s">
+      <c r="J58" s="19" t="s">
         <v>492</v>
       </c>
-      <c r="K57" s="19" t="s">
+      <c r="K58" s="19" t="s">
         <v>495</v>
       </c>
-      <c r="L57" s="19" t="s">
+      <c r="L58" s="19" t="s">
         <v>496</v>
       </c>
-      <c r="M57" s="19" t="s">
+      <c r="M58" s="19" t="s">
         <v>262</v>
       </c>
-      <c r="N57" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="O57" s="19" t="s">
+      <c r="N58" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="O58" s="19" t="s">
         <v>497</v>
       </c>
-      <c r="P57" s="25">
+      <c r="P58" s="25">
         <v>44111</v>
       </c>
-      <c r="Q57" s="19" t="s">
+      <c r="Q58" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="R57" s="19" t="s">
-        <v>304</v>
-      </c>
-      <c r="S57" s="19" t="s">
-        <v>304</v>
-      </c>
-      <c r="T57" s="20"/>
-    </row>
-    <row r="58" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="16"/>
-      <c r="B58" s="16"/>
-      <c r="C58" s="16"/>
-      <c r="D58" s="16"/>
-      <c r="E58" s="16"/>
-      <c r="F58" s="16"/>
-      <c r="G58" s="16"/>
-      <c r="H58" s="16"/>
-      <c r="I58" s="16"/>
-      <c r="J58" s="16"/>
-      <c r="K58" s="16"/>
-      <c r="L58" s="16"/>
-      <c r="M58" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="N58" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="O58" s="16"/>
-      <c r="P58" s="24">
-        <v>43788</v>
-      </c>
-      <c r="Q58" s="16"/>
-      <c r="R58" s="16"/>
-      <c r="S58" s="16"/>
-      <c r="T58" s="17"/>
-      <c r="U58" s="29"/>
-    </row>
-    <row r="59" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
-      <c r="A59" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="B59" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="C59" s="35" t="s">
-        <v>378</v>
-      </c>
-      <c r="D59" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="E59" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="F59" s="16" t="s">
-        <v>379</v>
-      </c>
-      <c r="G59" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="H59" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="I59" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="J59" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="K59" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="L59" s="16" t="s">
-        <v>380</v>
-      </c>
+      <c r="R58" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="S58" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="T58" s="20"/>
+    </row>
+    <row r="59" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="16"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="16"/>
+      <c r="E59" s="16"/>
+      <c r="F59" s="16"/>
+      <c r="G59" s="16"/>
+      <c r="H59" s="16"/>
+      <c r="I59" s="16"/>
+      <c r="J59" s="16"/>
+      <c r="K59" s="16"/>
+      <c r="L59" s="16"/>
       <c r="M59" s="16" t="s">
-        <v>257</v>
+        <v>110</v>
       </c>
       <c r="N59" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="O59" s="16" t="s">
-        <v>381</v>
-      </c>
+      <c r="O59" s="16"/>
       <c r="P59" s="24">
         <v>43788</v>
       </c>
-      <c r="Q59" s="16" t="s">
-        <v>382</v>
-      </c>
-      <c r="R59" s="16" t="s">
-        <v>304</v>
-      </c>
-      <c r="S59" s="16" t="s">
-        <v>310</v>
-      </c>
+      <c r="Q59" s="16"/>
+      <c r="R59" s="16"/>
+      <c r="S59" s="16"/>
       <c r="T59" s="17"/>
       <c r="U59" s="29"/>
     </row>
-    <row r="60" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A60" s="16" t="s">
-        <v>383</v>
-      </c>
-      <c r="B60" s="16"/>
-      <c r="C60" s="35" t="s">
-        <v>384</v>
+        <v>377</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="C60" s="32" t="s">
+        <v>378</v>
       </c>
       <c r="D60" s="16" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="E60" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F60" s="16" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="G60" s="16" t="s">
         <v>20</v>
@@ -5455,19 +5474,19 @@
         <v>380</v>
       </c>
       <c r="M60" s="16" t="s">
-        <v>470</v>
+        <v>257</v>
       </c>
       <c r="N60" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O60" s="16" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="P60" s="24">
         <v>43788</v>
       </c>
       <c r="Q60" s="16" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="R60" s="16" t="s">
         <v>304</v>
@@ -5478,22 +5497,22 @@
       <c r="T60" s="17"/>
       <c r="U60" s="29"/>
     </row>
-    <row r="61" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A61" s="16" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="B61" s="16"/>
-      <c r="C61" s="35" t="s">
-        <v>390</v>
+      <c r="C61" s="32" t="s">
+        <v>384</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="E61" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F61" s="16" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="G61" s="16" t="s">
         <v>20</v>
@@ -5514,19 +5533,19 @@
         <v>380</v>
       </c>
       <c r="M61" s="16" t="s">
-        <v>257</v>
+        <v>470</v>
       </c>
       <c r="N61" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O61" s="16" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="P61" s="24">
         <v>43788</v>
       </c>
       <c r="Q61" s="16" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="R61" s="16" t="s">
         <v>304</v>
@@ -5537,22 +5556,22 @@
       <c r="T61" s="17"/>
       <c r="U61" s="29"/>
     </row>
-    <row r="62" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A62" s="16" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="B62" s="16"/>
-      <c r="C62" s="35" t="s">
-        <v>395</v>
+      <c r="C62" s="32" t="s">
+        <v>390</v>
       </c>
       <c r="D62" s="16" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="E62" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F62" s="16" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="G62" s="16" t="s">
         <v>20</v>
@@ -5579,7 +5598,7 @@
         <v>110</v>
       </c>
       <c r="O62" s="16" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="P62" s="24">
         <v>43788</v>
@@ -5596,22 +5615,22 @@
       <c r="T62" s="17"/>
       <c r="U62" s="29"/>
     </row>
-    <row r="63" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A63" s="16" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="B63" s="16"/>
-      <c r="C63" s="35" t="s">
-        <v>400</v>
+      <c r="C63" s="32" t="s">
+        <v>395</v>
       </c>
       <c r="D63" s="16" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="E63" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F63" s="16" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="G63" s="16" t="s">
         <v>20</v>
@@ -5632,19 +5651,19 @@
         <v>380</v>
       </c>
       <c r="M63" s="16" t="s">
-        <v>470</v>
+        <v>257</v>
       </c>
       <c r="N63" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O63" s="16" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="P63" s="24">
         <v>43788</v>
       </c>
       <c r="Q63" s="16" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="R63" s="16" t="s">
         <v>304</v>
@@ -5655,112 +5674,112 @@
       <c r="T63" s="17"/>
       <c r="U63" s="29"/>
     </row>
-    <row r="64" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="16"/>
+    <row r="64" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A64" s="16" t="s">
+        <v>399</v>
+      </c>
       <c r="B64" s="16"/>
-      <c r="C64" s="16"/>
-      <c r="D64" s="16"/>
-      <c r="E64" s="16"/>
-      <c r="F64" s="16"/>
-      <c r="G64" s="16"/>
-      <c r="H64" s="16"/>
-      <c r="I64" s="16"/>
-      <c r="J64" s="16"/>
-      <c r="K64" s="16"/>
-      <c r="L64" s="16"/>
+      <c r="C64" s="32" t="s">
+        <v>400</v>
+      </c>
+      <c r="D64" s="16" t="s">
+        <v>401</v>
+      </c>
+      <c r="E64" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="F64" s="16" t="s">
+        <v>402</v>
+      </c>
+      <c r="G64" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H64" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="I64" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="J64" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="K64" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="L64" s="16" t="s">
+        <v>380</v>
+      </c>
       <c r="M64" s="16" t="s">
-        <v>257</v>
+        <v>470</v>
       </c>
       <c r="N64" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="O64" s="16"/>
+      <c r="O64" s="16" t="s">
+        <v>403</v>
+      </c>
       <c r="P64" s="24">
         <v>43788</v>
       </c>
-      <c r="Q64" s="16"/>
-      <c r="R64" s="16"/>
-      <c r="S64" s="16"/>
+      <c r="Q64" s="16" t="s">
+        <v>388</v>
+      </c>
+      <c r="R64" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="S64" s="16" t="s">
+        <v>310</v>
+      </c>
       <c r="T64" s="17"/>
       <c r="U64" s="29"/>
     </row>
-    <row r="65" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
-      <c r="A65" s="16" t="s">
-        <v>404</v>
-      </c>
-      <c r="B65" s="16" t="s">
-        <v>404</v>
-      </c>
-      <c r="C65" s="35" t="s">
-        <v>405</v>
-      </c>
-      <c r="D65" s="16" t="s">
-        <v>404</v>
-      </c>
-      <c r="E65" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="F65" s="16" t="s">
-        <v>406</v>
-      </c>
-      <c r="G65" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="H65" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="I65" s="16" t="s">
-        <v>404</v>
-      </c>
-      <c r="J65" s="16" t="s">
-        <v>404</v>
-      </c>
-      <c r="K65" s="16" t="s">
-        <v>404</v>
-      </c>
-      <c r="L65" s="16" t="s">
-        <v>407</v>
-      </c>
+    <row r="65" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="16"/>
+      <c r="B65" s="16"/>
+      <c r="C65" s="16"/>
+      <c r="D65" s="16"/>
+      <c r="E65" s="16"/>
+      <c r="F65" s="16"/>
+      <c r="G65" s="16"/>
+      <c r="H65" s="16"/>
+      <c r="I65" s="16"/>
+      <c r="J65" s="16"/>
+      <c r="K65" s="16"/>
+      <c r="L65" s="16"/>
       <c r="M65" s="16" t="s">
         <v>257</v>
       </c>
       <c r="N65" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="O65" s="16" t="s">
-        <v>408</v>
-      </c>
+      <c r="O65" s="16"/>
       <c r="P65" s="24">
         <v>43788</v>
       </c>
-      <c r="Q65" s="16" t="s">
-        <v>382</v>
-      </c>
-      <c r="R65" s="16" t="s">
-        <v>310</v>
-      </c>
-      <c r="S65" s="16" t="s">
-        <v>310</v>
-      </c>
+      <c r="Q65" s="16"/>
+      <c r="R65" s="16"/>
+      <c r="S65" s="16"/>
       <c r="T65" s="17"/>
       <c r="U65" s="29"/>
     </row>
-    <row r="66" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="B66" s="16"/>
-      <c r="C66" s="35" t="s">
-        <v>410</v>
+        <v>404</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="C66" s="32" t="s">
+        <v>405</v>
       </c>
       <c r="D66" s="16" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="E66" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F66" s="16" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="G66" s="16" t="s">
         <v>20</v>
@@ -5787,7 +5806,7 @@
         <v>110</v>
       </c>
       <c r="O66" s="16" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="P66" s="24">
         <v>43788</v>
@@ -5796,7 +5815,7 @@
         <v>382</v>
       </c>
       <c r="R66" s="16" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="S66" s="16" t="s">
         <v>310</v>
@@ -5804,22 +5823,22 @@
       <c r="T66" s="17"/>
       <c r="U66" s="29"/>
     </row>
-    <row r="67" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A67" s="16" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="B67" s="16"/>
-      <c r="C67" s="35" t="s">
-        <v>415</v>
+      <c r="C67" s="32" t="s">
+        <v>410</v>
       </c>
       <c r="D67" s="16" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="E67" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F67" s="16" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="G67" s="16" t="s">
         <v>20</v>
@@ -5846,7 +5865,7 @@
         <v>110</v>
       </c>
       <c r="O67" s="16" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="P67" s="24">
         <v>43788</v>
@@ -5855,7 +5874,7 @@
         <v>382</v>
       </c>
       <c r="R67" s="16" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="S67" s="16" t="s">
         <v>310</v>
@@ -5863,22 +5882,22 @@
       <c r="T67" s="17"/>
       <c r="U67" s="29"/>
     </row>
-    <row r="68" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A68" s="16" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B68" s="16"/>
-      <c r="C68" s="35" t="s">
-        <v>420</v>
+      <c r="C68" s="32" t="s">
+        <v>415</v>
       </c>
       <c r="D68" s="16" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="E68" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F68" s="16" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="G68" s="16" t="s">
         <v>20</v>
@@ -5905,7 +5924,7 @@
         <v>110</v>
       </c>
       <c r="O68" s="16" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="P68" s="24">
         <v>43788</v>
@@ -5922,22 +5941,22 @@
       <c r="T68" s="17"/>
       <c r="U68" s="29"/>
     </row>
-    <row r="69" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A69" s="16" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B69" s="16"/>
-      <c r="C69" s="35" t="s">
-        <v>425</v>
+      <c r="C69" s="32" t="s">
+        <v>420</v>
       </c>
       <c r="D69" s="16" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="E69" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F69" s="16" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="G69" s="16" t="s">
         <v>20</v>
@@ -5964,7 +5983,7 @@
         <v>110</v>
       </c>
       <c r="O69" s="16" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="P69" s="24">
         <v>43788</v>
@@ -5981,22 +6000,22 @@
       <c r="T69" s="17"/>
       <c r="U69" s="29"/>
     </row>
-    <row r="70" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A70" s="16" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="B70" s="16"/>
-      <c r="C70" s="35" t="s">
-        <v>430</v>
+      <c r="C70" s="32" t="s">
+        <v>425</v>
       </c>
       <c r="D70" s="16" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="E70" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F70" s="16" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="G70" s="16" t="s">
         <v>20</v>
@@ -6023,7 +6042,7 @@
         <v>110</v>
       </c>
       <c r="O70" s="16" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="P70" s="24">
         <v>43788</v>
@@ -6040,22 +6059,22 @@
       <c r="T70" s="17"/>
       <c r="U70" s="29"/>
     </row>
-    <row r="71" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A71" s="16" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="B71" s="16"/>
-      <c r="C71" s="35" t="s">
-        <v>435</v>
+      <c r="C71" s="32" t="s">
+        <v>430</v>
       </c>
       <c r="D71" s="16" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="E71" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F71" s="16" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="G71" s="16" t="s">
         <v>20</v>
@@ -6082,7 +6101,7 @@
         <v>110</v>
       </c>
       <c r="O71" s="16" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="P71" s="24">
         <v>43788</v>
@@ -6099,22 +6118,22 @@
       <c r="T71" s="17"/>
       <c r="U71" s="29"/>
     </row>
-    <row r="72" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A72" s="16" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B72" s="16"/>
-      <c r="C72" s="35" t="s">
-        <v>440</v>
+      <c r="C72" s="32" t="s">
+        <v>435</v>
       </c>
       <c r="D72" s="16" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="E72" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F72" s="16" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="G72" s="16" t="s">
         <v>20</v>
@@ -6141,7 +6160,7 @@
         <v>110</v>
       </c>
       <c r="O72" s="16" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="P72" s="24">
         <v>43788</v>
@@ -6158,22 +6177,22 @@
       <c r="T72" s="17"/>
       <c r="U72" s="29"/>
     </row>
-    <row r="73" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="16" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="B73" s="16"/>
-      <c r="C73" s="35" t="s">
-        <v>445</v>
+      <c r="C73" s="32" t="s">
+        <v>440</v>
       </c>
       <c r="D73" s="16" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="E73" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F73" s="16" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="G73" s="16" t="s">
         <v>20</v>
@@ -6200,7 +6219,7 @@
         <v>110</v>
       </c>
       <c r="O73" s="16" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="P73" s="24">
         <v>43788</v>
@@ -6217,22 +6236,22 @@
       <c r="T73" s="17"/>
       <c r="U73" s="29"/>
     </row>
-    <row r="74" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A74" s="16" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="B74" s="16"/>
-      <c r="C74" s="35" t="s">
-        <v>450</v>
+      <c r="C74" s="32" t="s">
+        <v>445</v>
       </c>
       <c r="D74" s="16" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="E74" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F74" s="16" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="G74" s="16" t="s">
         <v>20</v>
@@ -6259,7 +6278,7 @@
         <v>110</v>
       </c>
       <c r="O74" s="16" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="P74" s="24">
         <v>43788</v>
@@ -6276,22 +6295,22 @@
       <c r="T74" s="17"/>
       <c r="U74" s="29"/>
     </row>
-    <row r="75" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A75" s="16" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="B75" s="16"/>
-      <c r="C75" s="35" t="s">
-        <v>455</v>
+      <c r="C75" s="32" t="s">
+        <v>450</v>
       </c>
       <c r="D75" s="16" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="E75" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F75" s="16" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="G75" s="16" t="s">
         <v>20</v>
@@ -6318,7 +6337,7 @@
         <v>110</v>
       </c>
       <c r="O75" s="16" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="P75" s="24">
         <v>43788</v>
@@ -6335,22 +6354,22 @@
       <c r="T75" s="17"/>
       <c r="U75" s="29"/>
     </row>
-    <row r="76" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A76" s="16" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="B76" s="16"/>
-      <c r="C76" s="35" t="s">
-        <v>460</v>
+      <c r="C76" s="32" t="s">
+        <v>455</v>
       </c>
       <c r="D76" s="16" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="E76" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F76" s="16" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="G76" s="16" t="s">
         <v>20</v>
@@ -6377,7 +6396,7 @@
         <v>110</v>
       </c>
       <c r="O76" s="16" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="P76" s="24">
         <v>43788</v>
@@ -6394,22 +6413,22 @@
       <c r="T76" s="17"/>
       <c r="U76" s="29"/>
     </row>
-    <row r="77" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A77" s="16" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="B77" s="16"/>
-      <c r="C77" s="35" t="s">
-        <v>465</v>
+      <c r="C77" s="32" t="s">
+        <v>460</v>
       </c>
       <c r="D77" s="16" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="E77" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F77" s="16" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="G77" s="16" t="s">
         <v>20</v>
@@ -6436,7 +6455,7 @@
         <v>110</v>
       </c>
       <c r="O77" s="16" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="P77" s="24">
         <v>43788</v>
@@ -6453,79 +6472,82 @@
       <c r="T77" s="17"/>
       <c r="U77" s="29"/>
     </row>
-    <row r="78" spans="1:21" s="31" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A78" s="30" t="s">
+    <row r="78" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A78" s="16" t="s">
+        <v>464</v>
+      </c>
+      <c r="B78" s="16"/>
+      <c r="C78" s="32" t="s">
+        <v>465</v>
+      </c>
+      <c r="D78" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="E78" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="F78" s="16" t="s">
+        <v>467</v>
+      </c>
+      <c r="G78" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H78" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="I78" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="J78" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="K78" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="L78" s="16" t="s">
+        <v>407</v>
+      </c>
+      <c r="M78" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="N78" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="O78" s="16" t="s">
+        <v>468</v>
+      </c>
+      <c r="P78" s="24">
+        <v>43788</v>
+      </c>
+      <c r="Q78" s="16" t="s">
+        <v>382</v>
+      </c>
+      <c r="R78" s="16" t="s">
+        <v>310</v>
+      </c>
+      <c r="S78" s="16" t="s">
+        <v>310</v>
+      </c>
+      <c r="T78" s="17"/>
+      <c r="U78" s="29"/>
+    </row>
+    <row r="79" spans="1:21" s="36" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="35" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="79" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="16" t="s">
+    <row r="80" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B79" s="16" t="s">
+      <c r="B80" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="C79" s="16" t="s">
+      <c r="C80" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="D79" s="16" t="s">
+      <c r="D80" s="16" t="s">
         <v>60</v>
-      </c>
-      <c r="E79" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F79" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="G79" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="H79" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="I79" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="J79" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="K79" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="L79" s="16" t="s">
-        <v>249</v>
-      </c>
-      <c r="M79" s="16" t="s">
-        <v>256</v>
-      </c>
-      <c r="N79" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="O79" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="P79" s="24">
-        <v>42507</v>
-      </c>
-      <c r="Q79" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="R79" s="16"/>
-      <c r="S79" s="16"/>
-      <c r="T79" s="17"/>
-    </row>
-    <row r="80" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B80" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C80" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="D80" s="16" t="s">
-        <v>4</v>
       </c>
       <c r="E80" s="16" t="s">
         <v>25</v>
@@ -6540,48 +6562,48 @@
         <v>12</v>
       </c>
       <c r="I80" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J80" s="16" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="K80" s="16" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L80" s="16" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="M80" s="16" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="N80" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O80" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P80" s="24">
-        <v>41002</v>
+        <v>42507</v>
       </c>
       <c r="Q80" s="16" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="R80" s="16"/>
       <c r="S80" s="16"/>
       <c r="T80" s="17"/>
     </row>
-    <row r="81" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B81" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C81" s="16" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D81" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E81" s="16" t="s">
         <v>25</v>
@@ -6596,25 +6618,25 @@
         <v>12</v>
       </c>
       <c r="I81" s="16" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="J81" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K81" s="16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L81" s="16" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="M81" s="16" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="N81" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O81" s="16" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P81" s="24">
         <v>41002</v>
@@ -6626,18 +6648,18 @@
       <c r="S81" s="16"/>
       <c r="T81" s="17"/>
     </row>
-    <row r="82" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="16" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B82" s="16" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C82" s="16" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D82" s="16" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E82" s="16" t="s">
         <v>25</v>
@@ -6652,25 +6674,25 @@
         <v>12</v>
       </c>
       <c r="I82" s="16" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="J82" s="16" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="K82" s="16" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="L82" s="16" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="M82" s="16" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="N82" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O82" s="16" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="P82" s="24">
         <v>41002</v>
@@ -6682,36 +6704,70 @@
       <c r="S82" s="16"/>
       <c r="T82" s="17"/>
     </row>
-    <row r="83" spans="1:20" s="32" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A83" s="30" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="84" spans="1:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="12" t="s">
+    <row r="83" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B83" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C83" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D83" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E83" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F83" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="G83" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H83" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I83" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="J83" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="K83" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="L83" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="M83" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="N83" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="O83" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="P83" s="24">
+        <v>41002</v>
+      </c>
+      <c r="Q83" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="R83" s="16"/>
+      <c r="S83" s="16"/>
+      <c r="T83" s="17"/>
+    </row>
+    <row r="84" spans="1:20" s="37" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="35" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="12" t="s">
         <v>184</v>
-      </c>
-      <c r="B84" s="3"/>
-      <c r="D84" s="3"/>
-      <c r="E84" s="3"/>
-      <c r="F84" s="3"/>
-      <c r="G84" s="3"/>
-      <c r="I84" s="12"/>
-      <c r="J84" s="3"/>
-      <c r="K84" s="3"/>
-      <c r="L84" s="3"/>
-      <c r="M84" s="3"/>
-      <c r="N84" s="3"/>
-      <c r="O84" s="3"/>
-      <c r="P84" s="26"/>
-      <c r="Q84" s="3"/>
-      <c r="R84" s="3"/>
-      <c r="S84" s="3"/>
-      <c r="T84" s="3"/>
-    </row>
-    <row r="85" spans="1:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="12" t="s">
-        <v>185</v>
       </c>
       <c r="B85" s="3"/>
       <c r="D85" s="3"/>
@@ -6731,16 +6787,16 @@
       <c r="S85" s="3"/>
       <c r="T85" s="3"/>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A86" s="13" t="s">
-        <v>186</v>
+    <row r="86" spans="1:20" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="12" t="s">
+        <v>185</v>
       </c>
       <c r="B86" s="3"/>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
-      <c r="I86" s="13"/>
+      <c r="I86" s="12"/>
       <c r="J86" s="3"/>
       <c r="K86" s="3"/>
       <c r="L86" s="3"/>
@@ -6753,9 +6809,9 @@
       <c r="S86" s="3"/>
       <c r="T86" s="3"/>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A87" s="13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B87" s="3"/>
       <c r="D87" s="3"/>
@@ -6775,29 +6831,51 @@
       <c r="S87" s="3"/>
       <c r="T87" s="3"/>
     </row>
-    <row r="88" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="21" t="s">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A88" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="B88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+      <c r="G88" s="3"/>
+      <c r="I88" s="13"/>
+      <c r="J88" s="3"/>
+      <c r="K88" s="3"/>
+      <c r="L88" s="3"/>
+      <c r="M88" s="3"/>
+      <c r="N88" s="3"/>
+      <c r="O88" s="3"/>
+      <c r="P88" s="26"/>
+      <c r="Q88" s="3"/>
+      <c r="R88" s="3"/>
+      <c r="S88" s="3"/>
+      <c r="T88" s="3"/>
+    </row>
+    <row r="89" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="C88" s="12"/>
-      <c r="P88" s="27"/>
-    </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A89" s="22" t="s">
+      <c r="C89" s="12"/>
+      <c r="P89" s="27"/>
+    </row>
+    <row r="90" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A90" s="22" t="s">
         <v>225</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A35:O38">
-    <sortCondition ref="A35:A38"/>
+  <sortState ref="A36:O39">
+    <sortCondition ref="A36:A39"/>
   </sortState>
   <mergeCells count="6">
-    <mergeCell ref="A78:XFD78"/>
-    <mergeCell ref="A83:XFD83"/>
+    <mergeCell ref="A79:XFD79"/>
+    <mergeCell ref="A84:XFD84"/>
     <mergeCell ref="A2:XFD2"/>
     <mergeCell ref="A4:XFD4"/>
     <mergeCell ref="A10:XFD10"/>
-    <mergeCell ref="A30:XFD30"/>
+    <mergeCell ref="A31:XFD31"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6816,14 +6894,14 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.84375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="12.3828125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="141.53515625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="141.5546875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
@@ -6834,7 +6912,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>42080</v>
       </c>
@@ -6845,7 +6923,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>42119</v>
       </c>
@@ -6856,7 +6934,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>42131</v>
       </c>
@@ -6867,7 +6945,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>42158</v>
       </c>
@@ -6878,7 +6956,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>42248</v>
       </c>
@@ -6889,7 +6967,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>42249</v>
       </c>
@@ -6900,7 +6978,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>42507</v>
       </c>
@@ -6911,7 +6989,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>42582</v>
       </c>
@@ -6922,7 +7000,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>42724</v>
       </c>
@@ -6933,74 +7011,74 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A11" s="33">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="38">
         <v>42835</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="37" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A12" s="33"/>
-      <c r="B12" s="32"/>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="38"/>
+      <c r="B12" s="37"/>
       <c r="C12" s="7" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A13" s="33"/>
-      <c r="B13" s="32"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="38"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A14" s="33"/>
-      <c r="B14" s="32"/>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="38"/>
+      <c r="B14" s="37"/>
       <c r="C14" s="7" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A15" s="33"/>
-      <c r="B15" s="32"/>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="38"/>
+      <c r="B15" s="37"/>
       <c r="C15" s="7" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A16" s="33"/>
-      <c r="B16" s="32"/>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="38"/>
+      <c r="B16" s="37"/>
       <c r="C16" s="7" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A17" s="33"/>
-      <c r="B17" s="32"/>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="38"/>
+      <c r="B17" s="37"/>
       <c r="C17" s="7" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A18" s="33"/>
-      <c r="B18" s="32"/>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="38"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A19" s="33"/>
-      <c r="B19" s="32"/>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="38"/>
+      <c r="B19" s="37"/>
       <c r="C19" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>42839</v>
       </c>
@@ -7011,7 +7089,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
         <v>42839</v>
       </c>
@@ -7022,7 +7100,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="10">
         <v>42858</v>
       </c>
@@ -7033,7 +7111,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="10">
         <v>42858</v>
       </c>
@@ -7044,7 +7122,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>42928</v>
       </c>
@@ -7055,7 +7133,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>42969</v>
       </c>
@@ -7066,7 +7144,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="14">
         <v>42969</v>
       </c>
@@ -7077,7 +7155,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>43718</v>
       </c>
@@ -7088,7 +7166,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>43804</v>
       </c>

</xml_diff>

<commit_message>
Issue #319: Namespace Updates - ID Requested:multi (#320)
Add the namespace 'multi' to the namespace registry and LDDTool config.properties file.

    Namespace ID Requested: multi
    Discipline or Mission LDD? Discipline
    Steward Organization Name: PDS PPI Node
    LDD Steward Name: Joseph Mafi
    LDD Steward Email: jmafi@igpp.ucla.edu
    LDD Description: The Multidimensional dictionary contains classes that describe relationships between multidimensional data objects contained within a single data product.
    Rationale for creation of new LDD: These classes are needed in order to describe the relationships between multidimensional array objects. They replicate the DEPEND_n attributes provided in CDF metadata. These classes were previously defined in v1 of the Particle dictionary, however, they apply to more than just particle data.

Resolves #319
</commit_message>
<xml_diff>
--- a/model-ontology/src/ontology/Data/pds-namespace-registry.xlsx
+++ b/model-ontology/src/ontology/Data/pds-namespace-registry.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20371"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA5PDSProjN\AAAPDS4\AADataModel\0000_Design\Namespaces_1002\NameSpaceRegistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D43093-C62B-4F56-BE56-154ED8752095}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C95BA38C-BA55-4812-B7EE-A6F99CEF0447}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1157" yWindow="1063" windowWidth="26657" windowHeight="12857" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1068" windowWidth="26652" windowHeight="12852" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Namespaces" sheetId="1" r:id="rId1"/>
     <sheet name="Change Log" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Namespaces!$A$11:$Q$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Namespaces!$A$11:$Q$30</definedName>
   </definedNames>
   <calcPr calcId="140001"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1343" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4705" uniqueCount="523">
   <si>
     <t>Registration Date</t>
   </si>
@@ -1589,6 +1589,18 @@
   </si>
   <si>
     <t>sbnpsi</t>
+  </si>
+  <si>
+    <t>multi</t>
+  </si>
+  <si>
+    <t>http://pds.nasa.gov/pds4/multi/v1</t>
+  </si>
+  <si>
+    <t>PDS4_MULTI</t>
+  </si>
+  <si>
+    <t>The Multidimensional dictionary contains classes that describe relationships between multidimensional data objects contained within a single data product.</t>
   </si>
 </sst>
 </file>
@@ -1755,7 +1767,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1844,6 +1856,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1856,16 +1881,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2179,39 +2197,39 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U89"/>
+  <dimension ref="A1:U90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="15.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.3828125" style="22" customWidth="1"/>
-    <col min="2" max="2" width="16.69140625" style="22" customWidth="1"/>
-    <col min="3" max="3" width="46.15234375" style="12" customWidth="1"/>
-    <col min="4" max="4" width="13.3828125" style="22" customWidth="1"/>
-    <col min="5" max="5" width="14.3828125" style="22" customWidth="1"/>
-    <col min="6" max="6" width="22.84375" style="22" customWidth="1"/>
-    <col min="7" max="7" width="12.3828125" style="22" customWidth="1"/>
-    <col min="8" max="8" width="21.3828125" style="22" customWidth="1"/>
-    <col min="9" max="9" width="25.3046875" style="22" customWidth="1"/>
-    <col min="10" max="10" width="13.15234375" style="22" customWidth="1"/>
-    <col min="11" max="11" width="18.765625" style="22" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" style="22" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="46.109375" style="12" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" style="22" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="22" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" style="22" customWidth="1"/>
+    <col min="9" max="9" width="25.33203125" style="22" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" style="22" customWidth="1"/>
+    <col min="11" max="11" width="18.77734375" style="22" customWidth="1"/>
     <col min="12" max="12" width="23" style="22" customWidth="1"/>
-    <col min="13" max="13" width="38.69140625" style="22" customWidth="1"/>
-    <col min="14" max="14" width="10.15234375" style="22" customWidth="1"/>
-    <col min="15" max="15" width="53.84375" style="22" customWidth="1"/>
-    <col min="16" max="16" width="16.15234375" style="27" customWidth="1"/>
-    <col min="17" max="17" width="14.15234375" style="22" customWidth="1"/>
-    <col min="18" max="18" width="11.3828125" style="22" customWidth="1"/>
-    <col min="19" max="19" width="11.15234375" style="22" customWidth="1"/>
-    <col min="20" max="20" width="13.69140625" style="22" customWidth="1"/>
-    <col min="21" max="16384" width="8.84375" style="22"/>
+    <col min="13" max="13" width="38.6640625" style="22" customWidth="1"/>
+    <col min="14" max="14" width="10.109375" style="22" customWidth="1"/>
+    <col min="15" max="15" width="53.88671875" style="22" customWidth="1"/>
+    <col min="16" max="16" width="16.109375" style="27" customWidth="1"/>
+    <col min="17" max="17" width="14.109375" style="22" customWidth="1"/>
+    <col min="18" max="18" width="11.33203125" style="22" customWidth="1"/>
+    <col min="19" max="19" width="11.109375" style="22" customWidth="1"/>
+    <col min="20" max="20" width="13.6640625" style="22" customWidth="1"/>
+    <col min="21" max="16384" width="8.88671875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="47.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="47.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>179</v>
       </c>
@@ -2273,12 +2291,12 @@
         <v>302</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:20" s="36" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="35" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>2</v>
       </c>
@@ -2338,12 +2356,12 @@
       </c>
       <c r="T3" s="17"/>
     </row>
-    <row r="4" spans="1:20" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="30" t="s">
+    <row r="4" spans="1:20" s="36" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="35" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:20" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>102</v>
       </c>
@@ -2403,7 +2421,7 @@
       </c>
       <c r="T5" s="17"/>
     </row>
-    <row r="6" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:20" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>189</v>
       </c>
@@ -2463,7 +2481,7 @@
       </c>
       <c r="T6" s="17"/>
     </row>
-    <row r="7" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>26</v>
       </c>
@@ -2525,7 +2543,7 @@
         <v>42277</v>
       </c>
     </row>
-    <row r="8" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>101</v>
       </c>
@@ -2585,14 +2603,14 @@
       </c>
       <c r="T8" s="17"/>
     </row>
-    <row r="9" spans="1:20" s="28" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:20" s="28" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
         <v>499</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>499</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="33" t="s">
         <v>508</v>
       </c>
       <c r="D9" s="19" t="s">
@@ -2645,12 +2663,12 @@
       </c>
       <c r="T9" s="20"/>
     </row>
-    <row r="10" spans="1:20" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="30" t="s">
+    <row r="10" spans="1:20" s="36" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="35" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:20" s="28" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:20" s="28" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
         <v>36</v>
       </c>
@@ -2710,7 +2728,7 @@
       </c>
       <c r="T11" s="17"/>
     </row>
-    <row r="12" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
         <v>3</v>
       </c>
@@ -2770,7 +2788,7 @@
       </c>
       <c r="T12" s="17"/>
     </row>
-    <row r="13" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:20" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
         <v>63</v>
       </c>
@@ -2830,7 +2848,7 @@
       </c>
       <c r="T13" s="17"/>
     </row>
-    <row r="14" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>14</v>
       </c>
@@ -2890,7 +2908,7 @@
       </c>
       <c r="T14" s="17"/>
     </row>
-    <row r="15" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:20" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
         <v>41</v>
       </c>
@@ -2950,7 +2968,7 @@
       </c>
       <c r="T15" s="17"/>
     </row>
-    <row r="16" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
         <v>5</v>
       </c>
@@ -3010,7 +3028,7 @@
       </c>
       <c r="T16" s="17"/>
     </row>
-    <row r="17" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:20" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
         <v>276</v>
       </c>
@@ -3070,7 +3088,7 @@
       </c>
       <c r="T17" s="17"/>
     </row>
-    <row r="18" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:20" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
         <v>277</v>
       </c>
@@ -3130,14 +3148,14 @@
       </c>
       <c r="T18" s="17"/>
     </row>
-    <row r="19" spans="1:20" s="28" customFormat="1" ht="47.6" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:20" s="28" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
         <v>488</v>
       </c>
       <c r="B19" s="19" t="s">
         <v>488</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="31" t="s">
         <v>489</v>
       </c>
       <c r="D19" s="19" t="s">
@@ -3190,7 +3208,7 @@
       </c>
       <c r="T19" s="20"/>
     </row>
-    <row r="20" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:20" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
         <v>18</v>
       </c>
@@ -3250,7 +3268,7 @@
       </c>
       <c r="T20" s="17"/>
     </row>
-    <row r="21" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
         <v>2</v>
       </c>
@@ -3310,7 +3328,7 @@
       </c>
       <c r="T21" s="17"/>
     </row>
-    <row r="22" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:20" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
         <v>8</v>
       </c>
@@ -3370,7 +3388,7 @@
       </c>
       <c r="T22" s="17"/>
     </row>
-    <row r="23" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:20" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
         <v>285</v>
       </c>
@@ -3430,7 +3448,7 @@
       </c>
       <c r="T23" s="17"/>
     </row>
-    <row r="24" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
         <v>9</v>
       </c>
@@ -3490,7 +3508,7 @@
       </c>
       <c r="T24" s="17"/>
     </row>
-    <row r="25" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16" t="s">
         <v>11</v>
       </c>
@@ -3548,7 +3566,7 @@
       </c>
       <c r="T25" s="17"/>
     </row>
-    <row r="26" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="16" t="s">
         <v>39</v>
       </c>
@@ -3608,7 +3626,7 @@
       </c>
       <c r="T26" s="17"/>
     </row>
-    <row r="27" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16" t="s">
         <v>226</v>
       </c>
@@ -3668,14 +3686,14 @@
       </c>
       <c r="T27" s="17"/>
     </row>
-    <row r="28" spans="1:20" s="28" customFormat="1" ht="47.6" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:20" s="28" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A28" s="19" t="s">
         <v>480</v>
       </c>
       <c r="B28" s="19" t="s">
         <v>480</v>
       </c>
-      <c r="C28" s="34" t="s">
+      <c r="C28" s="31" t="s">
         <v>481</v>
       </c>
       <c r="D28" s="19" t="s">
@@ -3728,7 +3746,7 @@
       </c>
       <c r="T28" s="20"/>
     </row>
-    <row r="29" spans="1:20" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:20" s="30" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A29" s="16" t="s">
         <v>19</v>
       </c>
@@ -3788,209 +3806,209 @@
       </c>
       <c r="T29" s="17"/>
     </row>
-    <row r="30" spans="1:20" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="30" t="s">
+    <row r="30" spans="1:20" s="28" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="19" t="s">
+        <v>519</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>519</v>
+      </c>
+      <c r="C30" s="39" t="s">
+        <v>520</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>519</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>521</v>
+      </c>
+      <c r="G30" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I30" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="J30" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="K30" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="L30" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="M30" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="N30" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="O30" s="19" t="s">
+        <v>522</v>
+      </c>
+      <c r="P30" s="25">
+        <v>44257</v>
+      </c>
+      <c r="Q30" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="R30" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="S30" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="T30" s="20"/>
+    </row>
+    <row r="31" spans="1:20" s="36" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="35" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="16" t="s">
+    <row r="32" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B32" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C32" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D32" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E31" s="16" t="s">
+      <c r="E32" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F31" s="16" t="s">
+      <c r="F32" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="G31" s="16" t="s">
+      <c r="G32" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="H31" s="16" t="s">
+      <c r="H32" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I31" s="16" t="s">
+      <c r="I32" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="J31" s="16" t="s">
+      <c r="J32" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="K31" s="16" t="s">
+      <c r="K32" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="L31" s="16" t="s">
+      <c r="L32" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="M31" s="16" t="s">
+      <c r="M32" s="16" t="s">
         <v>272</v>
       </c>
-      <c r="N31" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="O31" s="16" t="s">
+      <c r="N32" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="O32" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="P31" s="24">
+      <c r="P32" s="24">
         <v>42089</v>
       </c>
-      <c r="Q31" s="16" t="s">
+      <c r="Q32" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="R31" s="16" t="s">
-        <v>304</v>
-      </c>
-      <c r="S31" s="16" t="s">
-        <v>304</v>
-      </c>
-      <c r="T31" s="17"/>
-    </row>
-    <row r="32" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="19" t="s">
+      <c r="R32" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="S32" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="T32" s="17"/>
+    </row>
+    <row r="33" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="19" t="s">
         <v>509</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="B33" s="19" t="s">
         <v>510</v>
       </c>
-      <c r="C32" s="37" t="s">
+      <c r="C33" s="34" t="s">
         <v>517</v>
       </c>
-      <c r="D32" s="19" t="s">
+      <c r="D33" s="19" t="s">
         <v>509</v>
       </c>
-      <c r="E32" s="19" t="s">
+      <c r="E33" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F32" s="19" t="s">
+      <c r="F33" s="19" t="s">
         <v>516</v>
       </c>
-      <c r="G32" s="19" t="s">
+      <c r="G33" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H32" s="19" t="s">
+      <c r="H33" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="I32" s="19" t="s">
+      <c r="I33" s="19" t="s">
         <v>515</v>
       </c>
-      <c r="J32" s="19" t="s">
+      <c r="J33" s="19" t="s">
         <v>518</v>
       </c>
-      <c r="K32" s="19" t="s">
+      <c r="K33" s="19" t="s">
         <v>484</v>
       </c>
-      <c r="L32" s="19" t="s">
+      <c r="L33" s="19" t="s">
         <v>511</v>
       </c>
-      <c r="M32" s="19" t="s">
+      <c r="M33" s="19" t="s">
         <v>512</v>
       </c>
-      <c r="N32" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="O32" s="19" t="s">
+      <c r="N33" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="O33" s="19" t="s">
         <v>513</v>
       </c>
-      <c r="P32" s="25">
+      <c r="P33" s="25">
         <v>44193</v>
       </c>
-      <c r="Q32" s="19" t="s">
+      <c r="Q33" s="19" t="s">
         <v>514</v>
       </c>
-      <c r="R32" s="19" t="s">
-        <v>304</v>
-      </c>
-      <c r="S32" s="19" t="s">
-        <v>304</v>
-      </c>
-      <c r="T32" s="20"/>
-    </row>
-    <row r="33" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="16" t="s">
+      <c r="R33" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="S33" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="T33" s="20"/>
+    </row>
+    <row r="34" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B34" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="C34" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="D34" s="16" t="s">
         <v>68</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F33" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="G33" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="H33" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="I33" s="16" t="s">
-        <v>209</v>
-      </c>
-      <c r="J33" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K33" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="L33" s="16" t="s">
-        <v>248</v>
-      </c>
-      <c r="M33" s="16" t="s">
-        <v>262</v>
-      </c>
-      <c r="N33" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="O33" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="P33" s="24">
-        <v>42119</v>
-      </c>
-      <c r="Q33" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="R33" s="16" t="s">
-        <v>304</v>
-      </c>
-      <c r="S33" s="16" t="s">
-        <v>304</v>
-      </c>
-      <c r="T33" s="17"/>
-    </row>
-    <row r="34" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>55</v>
       </c>
       <c r="E34" s="16" t="s">
         <v>25</v>
       </c>
       <c r="F34" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G34" s="16" t="s">
         <v>20</v>
@@ -3999,31 +4017,31 @@
         <v>12</v>
       </c>
       <c r="I34" s="16" t="s">
-        <v>119</v>
+        <v>209</v>
       </c>
       <c r="J34" s="16" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K34" s="16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="L34" s="16" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="M34" s="16" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="N34" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O34" s="16" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="P34" s="24">
-        <v>41837</v>
+        <v>42119</v>
       </c>
       <c r="Q34" s="16" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="R34" s="16" t="s">
         <v>304</v>
@@ -4033,15 +4051,15 @@
       </c>
       <c r="T34" s="17"/>
     </row>
-    <row r="35" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="16" t="s">
         <v>55</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="D35" s="16" t="s">
         <v>55</v>
@@ -4077,7 +4095,7 @@
         <v>110</v>
       </c>
       <c r="O35" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P35" s="24">
         <v>41837</v>
@@ -4093,24 +4111,24 @@
       </c>
       <c r="T35" s="17"/>
     </row>
-    <row r="36" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A36" s="16" t="s">
-        <v>474</v>
+        <v>55</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>475</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>476</v>
+        <v>55</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>78</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>474</v>
+        <v>55</v>
       </c>
       <c r="E36" s="16" t="s">
         <v>25</v>
       </c>
       <c r="F36" s="16" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="G36" s="16" t="s">
         <v>20</v>
@@ -4119,31 +4137,31 @@
         <v>12</v>
       </c>
       <c r="I36" s="16" t="s">
-        <v>477</v>
+        <v>119</v>
       </c>
       <c r="J36" s="16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K36" s="16" t="s">
-        <v>478</v>
+        <v>126</v>
       </c>
       <c r="L36" s="16" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="M36" s="16" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="N36" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O36" s="16" t="s">
-        <v>479</v>
+        <v>153</v>
       </c>
       <c r="P36" s="24">
-        <v>43935</v>
+        <v>41837</v>
       </c>
       <c r="Q36" s="16" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="R36" s="16" t="s">
         <v>304</v>
@@ -4153,18 +4171,18 @@
       </c>
       <c r="T36" s="17"/>
     </row>
-    <row r="37" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="16" t="s">
-        <v>34</v>
+        <v>474</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" s="16" t="s">
-        <v>91</v>
+        <v>475</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>476</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>34</v>
+        <v>474</v>
       </c>
       <c r="E37" s="16" t="s">
         <v>25</v>
@@ -4179,31 +4197,31 @@
         <v>12</v>
       </c>
       <c r="I37" s="16" t="s">
-        <v>210</v>
+        <v>477</v>
       </c>
       <c r="J37" s="16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K37" s="16" t="s">
-        <v>128</v>
+        <v>478</v>
       </c>
       <c r="L37" s="16" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="M37" s="16" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="N37" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O37" s="16" t="s">
-        <v>155</v>
+        <v>479</v>
       </c>
       <c r="P37" s="24">
-        <v>41600</v>
+        <v>43935</v>
       </c>
       <c r="Q37" s="16" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="R37" s="16" t="s">
         <v>304</v>
@@ -4213,18 +4231,18 @@
       </c>
       <c r="T37" s="17"/>
     </row>
-    <row r="38" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="16" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="E38" s="16" t="s">
         <v>25</v>
@@ -4239,7 +4257,7 @@
         <v>12</v>
       </c>
       <c r="I38" s="16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J38" s="16" t="s">
         <v>5</v>
@@ -4257,13 +4275,13 @@
         <v>110</v>
       </c>
       <c r="O38" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P38" s="24">
-        <v>42220</v>
+        <v>41600</v>
       </c>
       <c r="Q38" s="16" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="R38" s="16" t="s">
         <v>304</v>
@@ -4273,24 +4291,24 @@
       </c>
       <c r="T38" s="17"/>
     </row>
-    <row r="39" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="16" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E39" s="16" t="s">
         <v>25</v>
       </c>
       <c r="F39" s="16" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="G39" s="16" t="s">
         <v>20</v>
@@ -4299,31 +4317,31 @@
         <v>12</v>
       </c>
       <c r="I39" s="16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J39" s="16" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K39" s="16" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="L39" s="16" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="M39" s="16" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="N39" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O39" s="16" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="P39" s="24">
-        <v>42158</v>
+        <v>42220</v>
       </c>
       <c r="Q39" s="16" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="R39" s="16" t="s">
         <v>304</v>
@@ -4333,15 +4351,15 @@
       </c>
       <c r="T39" s="17"/>
     </row>
-    <row r="40" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="D40" s="16" t="s">
         <v>43</v>
@@ -4377,7 +4395,7 @@
         <v>110</v>
       </c>
       <c r="O40" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="P40" s="24">
         <v>42158</v>
@@ -4393,24 +4411,24 @@
       </c>
       <c r="T40" s="17"/>
     </row>
-    <row r="41" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16" t="s">
-        <v>234</v>
+        <v>43</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>235</v>
+        <v>43</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>236</v>
+        <v>79</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>234</v>
+        <v>43</v>
       </c>
       <c r="E41" s="16" t="s">
         <v>25</v>
       </c>
       <c r="F41" s="16" t="s">
-        <v>237</v>
+        <v>120</v>
       </c>
       <c r="G41" s="16" t="s">
         <v>20</v>
@@ -4419,31 +4437,31 @@
         <v>12</v>
       </c>
       <c r="I41" s="16" t="s">
-        <v>238</v>
+        <v>213</v>
       </c>
       <c r="J41" s="16" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K41" s="16" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="L41" s="16" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="M41" s="16" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="N41" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O41" s="16" t="s">
-        <v>239</v>
+        <v>159</v>
       </c>
       <c r="P41" s="24">
-        <v>42650</v>
+        <v>42158</v>
       </c>
       <c r="Q41" s="16" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="R41" s="16" t="s">
         <v>304</v>
@@ -4453,24 +4471,24 @@
       </c>
       <c r="T41" s="17"/>
     </row>
-    <row r="42" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="16" t="s">
-        <v>35</v>
+        <v>234</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>50</v>
+        <v>235</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>94</v>
+        <v>236</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>35</v>
+        <v>234</v>
       </c>
       <c r="E42" s="16" t="s">
         <v>25</v>
       </c>
       <c r="F42" s="16" t="s">
-        <v>110</v>
+        <v>237</v>
       </c>
       <c r="G42" s="16" t="s">
         <v>20</v>
@@ -4479,31 +4497,31 @@
         <v>12</v>
       </c>
       <c r="I42" s="16" t="s">
-        <v>212</v>
+        <v>238</v>
       </c>
       <c r="J42" s="16" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="K42" s="16" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="L42" s="16" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="M42" s="16" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="N42" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O42" s="16" t="s">
-        <v>157</v>
+        <v>239</v>
       </c>
       <c r="P42" s="24">
-        <v>41771</v>
+        <v>42650</v>
       </c>
       <c r="Q42" s="16" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="R42" s="16" t="s">
         <v>304</v>
@@ -4513,83 +4531,84 @@
       </c>
       <c r="T42" s="17"/>
     </row>
-    <row r="43" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="16" t="s">
-        <v>305</v>
+        <v>35</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>305</v>
-      </c>
-      <c r="C43" s="35" t="s">
-        <v>306</v>
+        <v>50</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>94</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>305</v>
+        <v>35</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>303</v>
+        <v>25</v>
       </c>
       <c r="F43" s="16" t="s">
-        <v>307</v>
+        <v>110</v>
       </c>
       <c r="G43" s="16" t="s">
         <v>20</v>
       </c>
       <c r="H43" s="16" t="s">
-        <v>175</v>
+        <v>12</v>
       </c>
       <c r="I43" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="J43" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="K43" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="L43" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="M43" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="N43" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="O43" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="P43" s="24">
+        <v>41771</v>
+      </c>
+      <c r="Q43" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="R43" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="S43" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="T43" s="17"/>
+    </row>
+    <row r="44" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="J43" s="16" t="s">
+      <c r="B44" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="K43" s="16" t="s">
+      <c r="C44" s="32" t="s">
+        <v>306</v>
+      </c>
+      <c r="D44" s="16" t="s">
         <v>305</v>
-      </c>
-      <c r="L43" s="16" t="s">
-        <v>308</v>
-      </c>
-      <c r="M43" s="16" t="s">
-        <v>472</v>
-      </c>
-      <c r="N43" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="O43" s="16" t="s">
-        <v>309</v>
-      </c>
-      <c r="P43" s="24">
-        <v>43788</v>
-      </c>
-      <c r="Q43" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="R43" s="16" t="s">
-        <v>304</v>
-      </c>
-      <c r="S43" s="16" t="s">
-        <v>310</v>
-      </c>
-      <c r="T43" s="17"/>
-      <c r="U43" s="29"/>
-    </row>
-    <row r="44" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
-      <c r="A44" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="B44" s="16"/>
-      <c r="C44" s="35" t="s">
-        <v>312</v>
-      </c>
-      <c r="D44" s="16" t="s">
-        <v>313</v>
       </c>
       <c r="E44" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F44" s="16" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="G44" s="16" t="s">
         <v>20</v>
@@ -4610,22 +4629,22 @@
         <v>308</v>
       </c>
       <c r="M44" s="16" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="N44" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O44" s="16" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="P44" s="24">
         <v>43788</v>
       </c>
       <c r="Q44" s="16" t="s">
-        <v>316</v>
+        <v>27</v>
       </c>
       <c r="R44" s="16" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="S44" s="16" t="s">
         <v>310</v>
@@ -4633,22 +4652,22 @@
       <c r="T44" s="17"/>
       <c r="U44" s="29"/>
     </row>
-    <row r="45" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A45" s="16" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="B45" s="16"/>
-      <c r="C45" s="35" t="s">
-        <v>318</v>
+      <c r="C45" s="32" t="s">
+        <v>312</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="E45" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F45" s="16" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="G45" s="16" t="s">
         <v>20</v>
@@ -4656,9 +4675,15 @@
       <c r="H45" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="I45" s="16"/>
-      <c r="J45" s="16"/>
-      <c r="K45" s="16"/>
+      <c r="I45" s="16" t="s">
+        <v>305</v>
+      </c>
+      <c r="J45" s="16" t="s">
+        <v>305</v>
+      </c>
+      <c r="K45" s="16" t="s">
+        <v>305</v>
+      </c>
       <c r="L45" s="16" t="s">
         <v>308</v>
       </c>
@@ -4669,7 +4694,7 @@
         <v>110</v>
       </c>
       <c r="O45" s="16" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="P45" s="24">
         <v>43788</v>
@@ -4678,7 +4703,7 @@
         <v>316</v>
       </c>
       <c r="R45" s="16" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="S45" s="16" t="s">
         <v>310</v>
@@ -4686,22 +4711,22 @@
       <c r="T45" s="17"/>
       <c r="U45" s="29"/>
     </row>
-    <row r="46" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A46" s="16" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B46" s="16"/>
-      <c r="C46" s="35" t="s">
-        <v>323</v>
+      <c r="C46" s="32" t="s">
+        <v>318</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="E46" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F46" s="16" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="G46" s="16" t="s">
         <v>20</v>
@@ -4722,7 +4747,7 @@
         <v>110</v>
       </c>
       <c r="O46" s="16" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="P46" s="24">
         <v>43788</v>
@@ -4731,7 +4756,7 @@
         <v>316</v>
       </c>
       <c r="R46" s="16" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="S46" s="16" t="s">
         <v>310</v>
@@ -4739,22 +4764,22 @@
       <c r="T46" s="17"/>
       <c r="U46" s="29"/>
     </row>
-    <row r="47" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A47" s="16" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="B47" s="16"/>
-      <c r="C47" s="35" t="s">
-        <v>328</v>
+      <c r="C47" s="32" t="s">
+        <v>323</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="E47" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F47" s="16" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="G47" s="16" t="s">
         <v>20</v>
@@ -4775,7 +4800,7 @@
         <v>110</v>
       </c>
       <c r="O47" s="16" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="P47" s="24">
         <v>43788</v>
@@ -4792,22 +4817,22 @@
       <c r="T47" s="17"/>
       <c r="U47" s="29"/>
     </row>
-    <row r="48" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A48" s="16" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="B48" s="16"/>
-      <c r="C48" s="35" t="s">
-        <v>333</v>
+      <c r="C48" s="32" t="s">
+        <v>328</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="E48" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F48" s="16" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="G48" s="16" t="s">
         <v>20</v>
@@ -4828,7 +4853,7 @@
         <v>110</v>
       </c>
       <c r="O48" s="16" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="P48" s="24">
         <v>43788</v>
@@ -4845,22 +4870,22 @@
       <c r="T48" s="17"/>
       <c r="U48" s="29"/>
     </row>
-    <row r="49" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A49" s="16" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="B49" s="16"/>
-      <c r="C49" s="35" t="s">
-        <v>338</v>
+      <c r="C49" s="32" t="s">
+        <v>333</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="E49" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F49" s="16" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="G49" s="16" t="s">
         <v>20</v>
@@ -4881,7 +4906,7 @@
         <v>110</v>
       </c>
       <c r="O49" s="16" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="P49" s="24">
         <v>43788</v>
@@ -4898,22 +4923,22 @@
       <c r="T49" s="17"/>
       <c r="U49" s="29"/>
     </row>
-    <row r="50" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A50" s="16" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="B50" s="16"/>
-      <c r="C50" s="35" t="s">
-        <v>343</v>
+      <c r="C50" s="32" t="s">
+        <v>338</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="E50" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F50" s="16" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G50" s="16" t="s">
         <v>20</v>
@@ -4934,7 +4959,7 @@
         <v>110</v>
       </c>
       <c r="O50" s="16" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="P50" s="24">
         <v>43788</v>
@@ -4951,22 +4976,22 @@
       <c r="T50" s="17"/>
       <c r="U50" s="29"/>
     </row>
-    <row r="51" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A51" s="16" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="B51" s="16"/>
-      <c r="C51" s="35" t="s">
-        <v>348</v>
+      <c r="C51" s="32" t="s">
+        <v>343</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="E51" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F51" s="16" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="G51" s="16" t="s">
         <v>20</v>
@@ -4987,7 +5012,7 @@
         <v>110</v>
       </c>
       <c r="O51" s="16" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="P51" s="24">
         <v>43788</v>
@@ -5004,22 +5029,22 @@
       <c r="T51" s="17"/>
       <c r="U51" s="29"/>
     </row>
-    <row r="52" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A52" s="16" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="B52" s="16"/>
-      <c r="C52" s="35" t="s">
-        <v>353</v>
+      <c r="C52" s="32" t="s">
+        <v>348</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="E52" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F52" s="16" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="G52" s="16" t="s">
         <v>20</v>
@@ -5040,7 +5065,7 @@
         <v>110</v>
       </c>
       <c r="O52" s="16" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="P52" s="24">
         <v>43788</v>
@@ -5057,22 +5082,22 @@
       <c r="T52" s="17"/>
       <c r="U52" s="29"/>
     </row>
-    <row r="53" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A53" s="16" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="B53" s="16"/>
-      <c r="C53" s="35" t="s">
-        <v>358</v>
+      <c r="C53" s="32" t="s">
+        <v>353</v>
       </c>
       <c r="D53" s="16" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="E53" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F53" s="16" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="G53" s="16" t="s">
         <v>20</v>
@@ -5093,7 +5118,7 @@
         <v>110</v>
       </c>
       <c r="O53" s="16" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="P53" s="24">
         <v>43788</v>
@@ -5110,22 +5135,22 @@
       <c r="T53" s="17"/>
       <c r="U53" s="29"/>
     </row>
-    <row r="54" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A54" s="16" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="B54" s="16"/>
-      <c r="C54" s="35" t="s">
-        <v>363</v>
+      <c r="C54" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="E54" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F54" s="16" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="G54" s="16" t="s">
         <v>20</v>
@@ -5146,7 +5171,7 @@
         <v>110</v>
       </c>
       <c r="O54" s="16" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="P54" s="24">
         <v>43788</v>
@@ -5163,22 +5188,22 @@
       <c r="T54" s="17"/>
       <c r="U54" s="29"/>
     </row>
-    <row r="55" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A55" s="16" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="B55" s="16"/>
-      <c r="C55" s="35" t="s">
-        <v>368</v>
+      <c r="C55" s="32" t="s">
+        <v>363</v>
       </c>
       <c r="D55" s="16" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="E55" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F55" s="16" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="G55" s="16" t="s">
         <v>20</v>
@@ -5199,7 +5224,7 @@
         <v>110</v>
       </c>
       <c r="O55" s="16" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="P55" s="24">
         <v>43788</v>
@@ -5216,22 +5241,22 @@
       <c r="T55" s="17"/>
       <c r="U55" s="29"/>
     </row>
-    <row r="56" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A56" s="16" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="B56" s="16"/>
-      <c r="C56" s="35" t="s">
-        <v>373</v>
+      <c r="C56" s="32" t="s">
+        <v>368</v>
       </c>
       <c r="D56" s="16" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="E56" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F56" s="16" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="G56" s="16" t="s">
         <v>20</v>
@@ -5252,7 +5277,7 @@
         <v>110</v>
       </c>
       <c r="O56" s="16" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="P56" s="24">
         <v>43788</v>
@@ -5269,172 +5294,166 @@
       <c r="T56" s="17"/>
       <c r="U56" s="29"/>
     </row>
-    <row r="57" spans="1:21" s="28" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
-      <c r="A57" s="19" t="s">
+    <row r="57" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A57" s="16" t="s">
+        <v>372</v>
+      </c>
+      <c r="B57" s="16"/>
+      <c r="C57" s="32" t="s">
+        <v>373</v>
+      </c>
+      <c r="D57" s="16" t="s">
+        <v>374</v>
+      </c>
+      <c r="E57" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="F57" s="16" t="s">
+        <v>375</v>
+      </c>
+      <c r="G57" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H57" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="I57" s="16"/>
+      <c r="J57" s="16"/>
+      <c r="K57" s="16"/>
+      <c r="L57" s="16" t="s">
+        <v>308</v>
+      </c>
+      <c r="M57" s="16" t="s">
+        <v>471</v>
+      </c>
+      <c r="N57" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="O57" s="16" t="s">
+        <v>376</v>
+      </c>
+      <c r="P57" s="24">
+        <v>43788</v>
+      </c>
+      <c r="Q57" s="16" t="s">
+        <v>316</v>
+      </c>
+      <c r="R57" s="16" t="s">
+        <v>310</v>
+      </c>
+      <c r="S57" s="16" t="s">
+        <v>310</v>
+      </c>
+      <c r="T57" s="17"/>
+      <c r="U57" s="29"/>
+    </row>
+    <row r="58" spans="1:21" s="28" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A58" s="19" t="s">
         <v>492</v>
       </c>
-      <c r="B57" s="19" t="s">
+      <c r="B58" s="19" t="s">
         <v>493</v>
       </c>
-      <c r="C57" s="34" t="s">
+      <c r="C58" s="31" t="s">
         <v>494</v>
       </c>
-      <c r="D57" s="19" t="s">
+      <c r="D58" s="19" t="s">
         <v>492</v>
       </c>
-      <c r="E57" s="19" t="s">
+      <c r="E58" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F57" s="19" t="s">
+      <c r="F58" s="19" t="s">
         <v>498</v>
       </c>
-      <c r="G57" s="19" t="s">
+      <c r="G58" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H57" s="19" t="s">
+      <c r="H58" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="I57" s="19" t="s">
+      <c r="I58" s="19" t="s">
         <v>492</v>
       </c>
-      <c r="J57" s="19" t="s">
+      <c r="J58" s="19" t="s">
         <v>492</v>
       </c>
-      <c r="K57" s="19" t="s">
+      <c r="K58" s="19" t="s">
         <v>495</v>
       </c>
-      <c r="L57" s="19" t="s">
+      <c r="L58" s="19" t="s">
         <v>496</v>
       </c>
-      <c r="M57" s="19" t="s">
+      <c r="M58" s="19" t="s">
         <v>262</v>
       </c>
-      <c r="N57" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="O57" s="19" t="s">
+      <c r="N58" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="O58" s="19" t="s">
         <v>497</v>
       </c>
-      <c r="P57" s="25">
+      <c r="P58" s="25">
         <v>44111</v>
       </c>
-      <c r="Q57" s="19" t="s">
+      <c r="Q58" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="R57" s="19" t="s">
-        <v>304</v>
-      </c>
-      <c r="S57" s="19" t="s">
-        <v>304</v>
-      </c>
-      <c r="T57" s="20"/>
-    </row>
-    <row r="58" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="16"/>
-      <c r="B58" s="16"/>
-      <c r="C58" s="16"/>
-      <c r="D58" s="16"/>
-      <c r="E58" s="16"/>
-      <c r="F58" s="16"/>
-      <c r="G58" s="16"/>
-      <c r="H58" s="16"/>
-      <c r="I58" s="16"/>
-      <c r="J58" s="16"/>
-      <c r="K58" s="16"/>
-      <c r="L58" s="16"/>
-      <c r="M58" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="N58" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="O58" s="16"/>
-      <c r="P58" s="24">
-        <v>43788</v>
-      </c>
-      <c r="Q58" s="16"/>
-      <c r="R58" s="16"/>
-      <c r="S58" s="16"/>
-      <c r="T58" s="17"/>
-      <c r="U58" s="29"/>
-    </row>
-    <row r="59" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
-      <c r="A59" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="B59" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="C59" s="35" t="s">
-        <v>378</v>
-      </c>
-      <c r="D59" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="E59" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="F59" s="16" t="s">
-        <v>379</v>
-      </c>
-      <c r="G59" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="H59" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="I59" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="J59" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="K59" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="L59" s="16" t="s">
-        <v>380</v>
-      </c>
+      <c r="R58" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="S58" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="T58" s="20"/>
+    </row>
+    <row r="59" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="16"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="16"/>
+      <c r="E59" s="16"/>
+      <c r="F59" s="16"/>
+      <c r="G59" s="16"/>
+      <c r="H59" s="16"/>
+      <c r="I59" s="16"/>
+      <c r="J59" s="16"/>
+      <c r="K59" s="16"/>
+      <c r="L59" s="16"/>
       <c r="M59" s="16" t="s">
-        <v>257</v>
+        <v>110</v>
       </c>
       <c r="N59" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="O59" s="16" t="s">
-        <v>381</v>
-      </c>
+      <c r="O59" s="16"/>
       <c r="P59" s="24">
         <v>43788</v>
       </c>
-      <c r="Q59" s="16" t="s">
-        <v>382</v>
-      </c>
-      <c r="R59" s="16" t="s">
-        <v>304</v>
-      </c>
-      <c r="S59" s="16" t="s">
-        <v>310</v>
-      </c>
+      <c r="Q59" s="16"/>
+      <c r="R59" s="16"/>
+      <c r="S59" s="16"/>
       <c r="T59" s="17"/>
       <c r="U59" s="29"/>
     </row>
-    <row r="60" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A60" s="16" t="s">
-        <v>383</v>
-      </c>
-      <c r="B60" s="16"/>
-      <c r="C60" s="35" t="s">
-        <v>384</v>
+        <v>377</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="C60" s="32" t="s">
+        <v>378</v>
       </c>
       <c r="D60" s="16" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="E60" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F60" s="16" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="G60" s="16" t="s">
         <v>20</v>
@@ -5455,19 +5474,19 @@
         <v>380</v>
       </c>
       <c r="M60" s="16" t="s">
-        <v>470</v>
+        <v>257</v>
       </c>
       <c r="N60" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O60" s="16" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="P60" s="24">
         <v>43788</v>
       </c>
       <c r="Q60" s="16" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="R60" s="16" t="s">
         <v>304</v>
@@ -5478,22 +5497,22 @@
       <c r="T60" s="17"/>
       <c r="U60" s="29"/>
     </row>
-    <row r="61" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A61" s="16" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="B61" s="16"/>
-      <c r="C61" s="35" t="s">
-        <v>390</v>
+      <c r="C61" s="32" t="s">
+        <v>384</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="E61" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F61" s="16" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="G61" s="16" t="s">
         <v>20</v>
@@ -5514,19 +5533,19 @@
         <v>380</v>
       </c>
       <c r="M61" s="16" t="s">
-        <v>257</v>
+        <v>470</v>
       </c>
       <c r="N61" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O61" s="16" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="P61" s="24">
         <v>43788</v>
       </c>
       <c r="Q61" s="16" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="R61" s="16" t="s">
         <v>304</v>
@@ -5537,22 +5556,22 @@
       <c r="T61" s="17"/>
       <c r="U61" s="29"/>
     </row>
-    <row r="62" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A62" s="16" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="B62" s="16"/>
-      <c r="C62" s="35" t="s">
-        <v>395</v>
+      <c r="C62" s="32" t="s">
+        <v>390</v>
       </c>
       <c r="D62" s="16" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="E62" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F62" s="16" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="G62" s="16" t="s">
         <v>20</v>
@@ -5579,7 +5598,7 @@
         <v>110</v>
       </c>
       <c r="O62" s="16" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="P62" s="24">
         <v>43788</v>
@@ -5596,22 +5615,22 @@
       <c r="T62" s="17"/>
       <c r="U62" s="29"/>
     </row>
-    <row r="63" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A63" s="16" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="B63" s="16"/>
-      <c r="C63" s="35" t="s">
-        <v>400</v>
+      <c r="C63" s="32" t="s">
+        <v>395</v>
       </c>
       <c r="D63" s="16" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="E63" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F63" s="16" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="G63" s="16" t="s">
         <v>20</v>
@@ -5632,19 +5651,19 @@
         <v>380</v>
       </c>
       <c r="M63" s="16" t="s">
-        <v>470</v>
+        <v>257</v>
       </c>
       <c r="N63" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O63" s="16" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="P63" s="24">
         <v>43788</v>
       </c>
       <c r="Q63" s="16" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="R63" s="16" t="s">
         <v>304</v>
@@ -5655,112 +5674,112 @@
       <c r="T63" s="17"/>
       <c r="U63" s="29"/>
     </row>
-    <row r="64" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="16"/>
+    <row r="64" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A64" s="16" t="s">
+        <v>399</v>
+      </c>
       <c r="B64" s="16"/>
-      <c r="C64" s="16"/>
-      <c r="D64" s="16"/>
-      <c r="E64" s="16"/>
-      <c r="F64" s="16"/>
-      <c r="G64" s="16"/>
-      <c r="H64" s="16"/>
-      <c r="I64" s="16"/>
-      <c r="J64" s="16"/>
-      <c r="K64" s="16"/>
-      <c r="L64" s="16"/>
+      <c r="C64" s="32" t="s">
+        <v>400</v>
+      </c>
+      <c r="D64" s="16" t="s">
+        <v>401</v>
+      </c>
+      <c r="E64" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="F64" s="16" t="s">
+        <v>402</v>
+      </c>
+      <c r="G64" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H64" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="I64" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="J64" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="K64" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="L64" s="16" t="s">
+        <v>380</v>
+      </c>
       <c r="M64" s="16" t="s">
-        <v>257</v>
+        <v>470</v>
       </c>
       <c r="N64" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="O64" s="16"/>
+      <c r="O64" s="16" t="s">
+        <v>403</v>
+      </c>
       <c r="P64" s="24">
         <v>43788</v>
       </c>
-      <c r="Q64" s="16"/>
-      <c r="R64" s="16"/>
-      <c r="S64" s="16"/>
+      <c r="Q64" s="16" t="s">
+        <v>388</v>
+      </c>
+      <c r="R64" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="S64" s="16" t="s">
+        <v>310</v>
+      </c>
       <c r="T64" s="17"/>
       <c r="U64" s="29"/>
     </row>
-    <row r="65" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
-      <c r="A65" s="16" t="s">
-        <v>404</v>
-      </c>
-      <c r="B65" s="16" t="s">
-        <v>404</v>
-      </c>
-      <c r="C65" s="35" t="s">
-        <v>405</v>
-      </c>
-      <c r="D65" s="16" t="s">
-        <v>404</v>
-      </c>
-      <c r="E65" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="F65" s="16" t="s">
-        <v>406</v>
-      </c>
-      <c r="G65" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="H65" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="I65" s="16" t="s">
-        <v>404</v>
-      </c>
-      <c r="J65" s="16" t="s">
-        <v>404</v>
-      </c>
-      <c r="K65" s="16" t="s">
-        <v>404</v>
-      </c>
-      <c r="L65" s="16" t="s">
-        <v>407</v>
-      </c>
+    <row r="65" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="16"/>
+      <c r="B65" s="16"/>
+      <c r="C65" s="16"/>
+      <c r="D65" s="16"/>
+      <c r="E65" s="16"/>
+      <c r="F65" s="16"/>
+      <c r="G65" s="16"/>
+      <c r="H65" s="16"/>
+      <c r="I65" s="16"/>
+      <c r="J65" s="16"/>
+      <c r="K65" s="16"/>
+      <c r="L65" s="16"/>
       <c r="M65" s="16" t="s">
         <v>257</v>
       </c>
       <c r="N65" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="O65" s="16" t="s">
-        <v>408</v>
-      </c>
+      <c r="O65" s="16"/>
       <c r="P65" s="24">
         <v>43788</v>
       </c>
-      <c r="Q65" s="16" t="s">
-        <v>382</v>
-      </c>
-      <c r="R65" s="16" t="s">
-        <v>310</v>
-      </c>
-      <c r="S65" s="16" t="s">
-        <v>310</v>
-      </c>
+      <c r="Q65" s="16"/>
+      <c r="R65" s="16"/>
+      <c r="S65" s="16"/>
       <c r="T65" s="17"/>
       <c r="U65" s="29"/>
     </row>
-    <row r="66" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="B66" s="16"/>
-      <c r="C66" s="35" t="s">
-        <v>410</v>
+        <v>404</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="C66" s="32" t="s">
+        <v>405</v>
       </c>
       <c r="D66" s="16" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="E66" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F66" s="16" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="G66" s="16" t="s">
         <v>20</v>
@@ -5787,7 +5806,7 @@
         <v>110</v>
       </c>
       <c r="O66" s="16" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="P66" s="24">
         <v>43788</v>
@@ -5796,7 +5815,7 @@
         <v>382</v>
       </c>
       <c r="R66" s="16" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="S66" s="16" t="s">
         <v>310</v>
@@ -5804,22 +5823,22 @@
       <c r="T66" s="17"/>
       <c r="U66" s="29"/>
     </row>
-    <row r="67" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A67" s="16" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="B67" s="16"/>
-      <c r="C67" s="35" t="s">
-        <v>415</v>
+      <c r="C67" s="32" t="s">
+        <v>410</v>
       </c>
       <c r="D67" s="16" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="E67" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F67" s="16" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="G67" s="16" t="s">
         <v>20</v>
@@ -5846,7 +5865,7 @@
         <v>110</v>
       </c>
       <c r="O67" s="16" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="P67" s="24">
         <v>43788</v>
@@ -5855,7 +5874,7 @@
         <v>382</v>
       </c>
       <c r="R67" s="16" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="S67" s="16" t="s">
         <v>310</v>
@@ -5863,22 +5882,22 @@
       <c r="T67" s="17"/>
       <c r="U67" s="29"/>
     </row>
-    <row r="68" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A68" s="16" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B68" s="16"/>
-      <c r="C68" s="35" t="s">
-        <v>420</v>
+      <c r="C68" s="32" t="s">
+        <v>415</v>
       </c>
       <c r="D68" s="16" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="E68" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F68" s="16" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="G68" s="16" t="s">
         <v>20</v>
@@ -5905,7 +5924,7 @@
         <v>110</v>
       </c>
       <c r="O68" s="16" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="P68" s="24">
         <v>43788</v>
@@ -5922,22 +5941,22 @@
       <c r="T68" s="17"/>
       <c r="U68" s="29"/>
     </row>
-    <row r="69" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A69" s="16" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B69" s="16"/>
-      <c r="C69" s="35" t="s">
-        <v>425</v>
+      <c r="C69" s="32" t="s">
+        <v>420</v>
       </c>
       <c r="D69" s="16" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="E69" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F69" s="16" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="G69" s="16" t="s">
         <v>20</v>
@@ -5964,7 +5983,7 @@
         <v>110</v>
       </c>
       <c r="O69" s="16" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="P69" s="24">
         <v>43788</v>
@@ -5981,22 +6000,22 @@
       <c r="T69" s="17"/>
       <c r="U69" s="29"/>
     </row>
-    <row r="70" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A70" s="16" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="B70" s="16"/>
-      <c r="C70" s="35" t="s">
-        <v>430</v>
+      <c r="C70" s="32" t="s">
+        <v>425</v>
       </c>
       <c r="D70" s="16" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="E70" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F70" s="16" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="G70" s="16" t="s">
         <v>20</v>
@@ -6023,7 +6042,7 @@
         <v>110</v>
       </c>
       <c r="O70" s="16" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="P70" s="24">
         <v>43788</v>
@@ -6040,22 +6059,22 @@
       <c r="T70" s="17"/>
       <c r="U70" s="29"/>
     </row>
-    <row r="71" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A71" s="16" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="B71" s="16"/>
-      <c r="C71" s="35" t="s">
-        <v>435</v>
+      <c r="C71" s="32" t="s">
+        <v>430</v>
       </c>
       <c r="D71" s="16" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="E71" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F71" s="16" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="G71" s="16" t="s">
         <v>20</v>
@@ -6082,7 +6101,7 @@
         <v>110</v>
       </c>
       <c r="O71" s="16" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="P71" s="24">
         <v>43788</v>
@@ -6099,22 +6118,22 @@
       <c r="T71" s="17"/>
       <c r="U71" s="29"/>
     </row>
-    <row r="72" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A72" s="16" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B72" s="16"/>
-      <c r="C72" s="35" t="s">
-        <v>440</v>
+      <c r="C72" s="32" t="s">
+        <v>435</v>
       </c>
       <c r="D72" s="16" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="E72" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F72" s="16" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="G72" s="16" t="s">
         <v>20</v>
@@ -6141,7 +6160,7 @@
         <v>110</v>
       </c>
       <c r="O72" s="16" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="P72" s="24">
         <v>43788</v>
@@ -6158,22 +6177,22 @@
       <c r="T72" s="17"/>
       <c r="U72" s="29"/>
     </row>
-    <row r="73" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="16" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="B73" s="16"/>
-      <c r="C73" s="35" t="s">
-        <v>445</v>
+      <c r="C73" s="32" t="s">
+        <v>440</v>
       </c>
       <c r="D73" s="16" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="E73" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F73" s="16" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="G73" s="16" t="s">
         <v>20</v>
@@ -6200,7 +6219,7 @@
         <v>110</v>
       </c>
       <c r="O73" s="16" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="P73" s="24">
         <v>43788</v>
@@ -6217,22 +6236,22 @@
       <c r="T73" s="17"/>
       <c r="U73" s="29"/>
     </row>
-    <row r="74" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A74" s="16" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="B74" s="16"/>
-      <c r="C74" s="35" t="s">
-        <v>450</v>
+      <c r="C74" s="32" t="s">
+        <v>445</v>
       </c>
       <c r="D74" s="16" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="E74" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F74" s="16" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="G74" s="16" t="s">
         <v>20</v>
@@ -6259,7 +6278,7 @@
         <v>110</v>
       </c>
       <c r="O74" s="16" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="P74" s="24">
         <v>43788</v>
@@ -6276,22 +6295,22 @@
       <c r="T74" s="17"/>
       <c r="U74" s="29"/>
     </row>
-    <row r="75" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A75" s="16" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="B75" s="16"/>
-      <c r="C75" s="35" t="s">
-        <v>455</v>
+      <c r="C75" s="32" t="s">
+        <v>450</v>
       </c>
       <c r="D75" s="16" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="E75" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F75" s="16" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="G75" s="16" t="s">
         <v>20</v>
@@ -6318,7 +6337,7 @@
         <v>110</v>
       </c>
       <c r="O75" s="16" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="P75" s="24">
         <v>43788</v>
@@ -6335,22 +6354,22 @@
       <c r="T75" s="17"/>
       <c r="U75" s="29"/>
     </row>
-    <row r="76" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A76" s="16" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="B76" s="16"/>
-      <c r="C76" s="35" t="s">
-        <v>460</v>
+      <c r="C76" s="32" t="s">
+        <v>455</v>
       </c>
       <c r="D76" s="16" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="E76" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F76" s="16" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="G76" s="16" t="s">
         <v>20</v>
@@ -6377,7 +6396,7 @@
         <v>110</v>
       </c>
       <c r="O76" s="16" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="P76" s="24">
         <v>43788</v>
@@ -6394,22 +6413,22 @@
       <c r="T76" s="17"/>
       <c r="U76" s="29"/>
     </row>
-    <row r="77" spans="1:21" s="13" customFormat="1" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A77" s="16" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="B77" s="16"/>
-      <c r="C77" s="35" t="s">
-        <v>465</v>
+      <c r="C77" s="32" t="s">
+        <v>460</v>
       </c>
       <c r="D77" s="16" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="E77" s="16" t="s">
         <v>303</v>
       </c>
       <c r="F77" s="16" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="G77" s="16" t="s">
         <v>20</v>
@@ -6436,7 +6455,7 @@
         <v>110</v>
       </c>
       <c r="O77" s="16" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="P77" s="24">
         <v>43788</v>
@@ -6453,79 +6472,82 @@
       <c r="T77" s="17"/>
       <c r="U77" s="29"/>
     </row>
-    <row r="78" spans="1:21" s="31" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A78" s="30" t="s">
+    <row r="78" spans="1:21" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A78" s="16" t="s">
+        <v>464</v>
+      </c>
+      <c r="B78" s="16"/>
+      <c r="C78" s="32" t="s">
+        <v>465</v>
+      </c>
+      <c r="D78" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="E78" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="F78" s="16" t="s">
+        <v>467</v>
+      </c>
+      <c r="G78" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H78" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="I78" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="J78" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="K78" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="L78" s="16" t="s">
+        <v>407</v>
+      </c>
+      <c r="M78" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="N78" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="O78" s="16" t="s">
+        <v>468</v>
+      </c>
+      <c r="P78" s="24">
+        <v>43788</v>
+      </c>
+      <c r="Q78" s="16" t="s">
+        <v>382</v>
+      </c>
+      <c r="R78" s="16" t="s">
+        <v>310</v>
+      </c>
+      <c r="S78" s="16" t="s">
+        <v>310</v>
+      </c>
+      <c r="T78" s="17"/>
+      <c r="U78" s="29"/>
+    </row>
+    <row r="79" spans="1:21" s="36" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="35" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="79" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="16" t="s">
+    <row r="80" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B79" s="16" t="s">
+      <c r="B80" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="C79" s="16" t="s">
+      <c r="C80" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="D79" s="16" t="s">
+      <c r="D80" s="16" t="s">
         <v>60</v>
-      </c>
-      <c r="E79" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F79" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="G79" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="H79" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="I79" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="J79" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="K79" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="L79" s="16" t="s">
-        <v>249</v>
-      </c>
-      <c r="M79" s="16" t="s">
-        <v>256</v>
-      </c>
-      <c r="N79" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="O79" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="P79" s="24">
-        <v>42507</v>
-      </c>
-      <c r="Q79" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="R79" s="16"/>
-      <c r="S79" s="16"/>
-      <c r="T79" s="17"/>
-    </row>
-    <row r="80" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B80" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C80" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="D80" s="16" t="s">
-        <v>4</v>
       </c>
       <c r="E80" s="16" t="s">
         <v>25</v>
@@ -6540,48 +6562,48 @@
         <v>12</v>
       </c>
       <c r="I80" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J80" s="16" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="K80" s="16" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L80" s="16" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="M80" s="16" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="N80" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O80" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P80" s="24">
-        <v>41002</v>
+        <v>42507</v>
       </c>
       <c r="Q80" s="16" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="R80" s="16"/>
       <c r="S80" s="16"/>
       <c r="T80" s="17"/>
     </row>
-    <row r="81" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B81" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C81" s="16" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D81" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E81" s="16" t="s">
         <v>25</v>
@@ -6596,25 +6618,25 @@
         <v>12</v>
       </c>
       <c r="I81" s="16" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="J81" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K81" s="16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L81" s="16" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="M81" s="16" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="N81" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O81" s="16" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P81" s="24">
         <v>41002</v>
@@ -6626,18 +6648,18 @@
       <c r="S81" s="16"/>
       <c r="T81" s="17"/>
     </row>
-    <row r="82" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="16" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B82" s="16" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C82" s="16" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D82" s="16" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E82" s="16" t="s">
         <v>25</v>
@@ -6652,25 +6674,25 @@
         <v>12</v>
       </c>
       <c r="I82" s="16" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="J82" s="16" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="K82" s="16" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="L82" s="16" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="M82" s="16" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="N82" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O82" s="16" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="P82" s="24">
         <v>41002</v>
@@ -6682,36 +6704,70 @@
       <c r="S82" s="16"/>
       <c r="T82" s="17"/>
     </row>
-    <row r="83" spans="1:20" s="32" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A83" s="30" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="84" spans="1:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="12" t="s">
+    <row r="83" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B83" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C83" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D83" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E83" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F83" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="G83" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H83" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I83" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="J83" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="K83" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="L83" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="M83" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="N83" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="O83" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="P83" s="24">
+        <v>41002</v>
+      </c>
+      <c r="Q83" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="R83" s="16"/>
+      <c r="S83" s="16"/>
+      <c r="T83" s="17"/>
+    </row>
+    <row r="84" spans="1:20" s="37" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="35" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="12" t="s">
         <v>184</v>
-      </c>
-      <c r="B84" s="3"/>
-      <c r="D84" s="3"/>
-      <c r="E84" s="3"/>
-      <c r="F84" s="3"/>
-      <c r="G84" s="3"/>
-      <c r="I84" s="12"/>
-      <c r="J84" s="3"/>
-      <c r="K84" s="3"/>
-      <c r="L84" s="3"/>
-      <c r="M84" s="3"/>
-      <c r="N84" s="3"/>
-      <c r="O84" s="3"/>
-      <c r="P84" s="26"/>
-      <c r="Q84" s="3"/>
-      <c r="R84" s="3"/>
-      <c r="S84" s="3"/>
-      <c r="T84" s="3"/>
-    </row>
-    <row r="85" spans="1:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="12" t="s">
-        <v>185</v>
       </c>
       <c r="B85" s="3"/>
       <c r="D85" s="3"/>
@@ -6731,16 +6787,16 @@
       <c r="S85" s="3"/>
       <c r="T85" s="3"/>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A86" s="13" t="s">
-        <v>186</v>
+    <row r="86" spans="1:20" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="12" t="s">
+        <v>185</v>
       </c>
       <c r="B86" s="3"/>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
-      <c r="I86" s="13"/>
+      <c r="I86" s="12"/>
       <c r="J86" s="3"/>
       <c r="K86" s="3"/>
       <c r="L86" s="3"/>
@@ -6753,9 +6809,9 @@
       <c r="S86" s="3"/>
       <c r="T86" s="3"/>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A87" s="13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B87" s="3"/>
       <c r="D87" s="3"/>
@@ -6775,29 +6831,51 @@
       <c r="S87" s="3"/>
       <c r="T87" s="3"/>
     </row>
-    <row r="88" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="21" t="s">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A88" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="B88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+      <c r="G88" s="3"/>
+      <c r="I88" s="13"/>
+      <c r="J88" s="3"/>
+      <c r="K88" s="3"/>
+      <c r="L88" s="3"/>
+      <c r="M88" s="3"/>
+      <c r="N88" s="3"/>
+      <c r="O88" s="3"/>
+      <c r="P88" s="26"/>
+      <c r="Q88" s="3"/>
+      <c r="R88" s="3"/>
+      <c r="S88" s="3"/>
+      <c r="T88" s="3"/>
+    </row>
+    <row r="89" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="C88" s="12"/>
-      <c r="P88" s="27"/>
-    </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A89" s="22" t="s">
+      <c r="C89" s="12"/>
+      <c r="P89" s="27"/>
+    </row>
+    <row r="90" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A90" s="22" t="s">
         <v>225</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A35:O38">
-    <sortCondition ref="A35:A38"/>
+  <sortState ref="A36:O39">
+    <sortCondition ref="A36:A39"/>
   </sortState>
   <mergeCells count="6">
-    <mergeCell ref="A78:XFD78"/>
-    <mergeCell ref="A83:XFD83"/>
+    <mergeCell ref="A79:XFD79"/>
+    <mergeCell ref="A84:XFD84"/>
     <mergeCell ref="A2:XFD2"/>
     <mergeCell ref="A4:XFD4"/>
     <mergeCell ref="A10:XFD10"/>
-    <mergeCell ref="A30:XFD30"/>
+    <mergeCell ref="A31:XFD31"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6816,14 +6894,14 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.84375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="12.3828125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="141.53515625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="141.5546875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
@@ -6834,7 +6912,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>42080</v>
       </c>
@@ -6845,7 +6923,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>42119</v>
       </c>
@@ -6856,7 +6934,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>42131</v>
       </c>
@@ -6867,7 +6945,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>42158</v>
       </c>
@@ -6878,7 +6956,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>42248</v>
       </c>
@@ -6889,7 +6967,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>42249</v>
       </c>
@@ -6900,7 +6978,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>42507</v>
       </c>
@@ -6911,7 +6989,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>42582</v>
       </c>
@@ -6922,7 +7000,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>42724</v>
       </c>
@@ -6933,74 +7011,74 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A11" s="33">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="38">
         <v>42835</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="37" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A12" s="33"/>
-      <c r="B12" s="32"/>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="38"/>
+      <c r="B12" s="37"/>
       <c r="C12" s="7" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A13" s="33"/>
-      <c r="B13" s="32"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="38"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A14" s="33"/>
-      <c r="B14" s="32"/>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="38"/>
+      <c r="B14" s="37"/>
       <c r="C14" s="7" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A15" s="33"/>
-      <c r="B15" s="32"/>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="38"/>
+      <c r="B15" s="37"/>
       <c r="C15" s="7" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A16" s="33"/>
-      <c r="B16" s="32"/>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="38"/>
+      <c r="B16" s="37"/>
       <c r="C16" s="7" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A17" s="33"/>
-      <c r="B17" s="32"/>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="38"/>
+      <c r="B17" s="37"/>
       <c r="C17" s="7" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A18" s="33"/>
-      <c r="B18" s="32"/>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="38"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A19" s="33"/>
-      <c r="B19" s="32"/>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="38"/>
+      <c r="B19" s="37"/>
       <c r="C19" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>42839</v>
       </c>
@@ -7011,7 +7089,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
         <v>42839</v>
       </c>
@@ -7022,7 +7100,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="10">
         <v>42858</v>
       </c>
@@ -7033,7 +7111,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="10">
         <v>42858</v>
       </c>
@@ -7044,7 +7122,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>42928</v>
       </c>
@@ -7055,7 +7133,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>42969</v>
       </c>
@@ -7066,7 +7144,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="14">
         <v>42969</v>
       </c>
@@ -7077,7 +7155,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>43718</v>
       </c>
@@ -7088,7 +7166,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>43804</v>
       </c>

</xml_diff>